<commit_message>
actualizar noticias hasta el 17 de agosto y cambiar de gpt 4o a 5
</commit_message>
<xml_diff>
--- a/tipo de cambio y tasas de interés.xlsx
+++ b/tipo de cambio y tasas de interés.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C54C98-E3FF-4D38-989D-B81509C113EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7621B9D-97C9-4BA2-A032-15E661B266D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo de Cambio" sheetId="1" r:id="rId1"/>
@@ -607,6 +607,9 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -681,9 +684,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -698,25 +698,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}" name="Tabla1" displayName="Tabla1" ref="A1:E40" totalsRowShown="0" dataDxfId="4" dataCellStyle="Moneda">
-  <autoFilter ref="A1:E40" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}" name="Tabla1" displayName="Tabla1" ref="A1:E54" totalsRowShown="0" dataDxfId="5" dataCellStyle="Moneda">
+  <autoFilter ref="A1:E54" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8E09B427-5E44-4BBB-89FC-35463079BE46}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{3D7466AA-D045-44D9-96B5-BDFB7062F58C}" name="Fecha" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{157C7180-B5CE-4C51-9BD0-3AEECF3B91F1}" name="Tipo de Cambio FIX" dataDxfId="2" dataCellStyle="Moneda"/>
-    <tableColumn id="4" xr3:uid="{74B4BBBC-E72A-423F-B8FA-CE596B4E990E}" name="Nivel máximo" dataDxfId="1" dataCellStyle="Moneda"/>
-    <tableColumn id="5" xr3:uid="{74EB6E0A-1398-4291-8596-80BA6140571D}" name="Nivel mínimo" dataDxfId="0" dataCellStyle="Moneda"/>
+    <tableColumn id="2" xr3:uid="{3D7466AA-D045-44D9-96B5-BDFB7062F58C}" name="Fecha" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{157C7180-B5CE-4C51-9BD0-3AEECF3B91F1}" name="Tipo de Cambio FIX" dataDxfId="3" dataCellStyle="Moneda"/>
+    <tableColumn id="4" xr3:uid="{74B4BBBC-E72A-423F-B8FA-CE596B4E990E}" name="Nivel máximo" dataDxfId="2" dataCellStyle="Moneda"/>
+    <tableColumn id="5" xr3:uid="{74EB6E0A-1398-4291-8596-80BA6140571D}" name="Nivel mínimo" dataDxfId="1" dataCellStyle="Moneda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}" name="Tabla2" displayName="Tabla2" ref="A1:F39" totalsRowShown="0">
-  <autoFilter ref="A1:F39" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}" name="Tabla2" displayName="Tabla2" ref="A1:F53" totalsRowShown="0">
+  <autoFilter ref="A1:F53" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B700B119-8C38-4F55-BC79-C4D6BC8E0C88}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{47E09E7D-A904-4405-9048-49D33EE0E8EB}" name="Fecha" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{47E09E7D-A904-4405-9048-49D33EE0E8EB}" name="Fecha" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{0E168449-32EF-450B-812C-11DC4F0F3A30}" name="Tasa de Interés Objetivo"/>
     <tableColumn id="4" xr3:uid="{EE5A2D13-088C-4226-A754-1A001EC14095}" name="TIIE 28 días"/>
     <tableColumn id="5" xr3:uid="{91C093C9-2029-4DE0-AF73-BB6DB79C251D}" name="TIIE 91 días"/>
@@ -1023,11 +1023,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892B4731-B44C-4F20-9A44-95C4BD8A73FF}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1716,6 +1714,244 @@
         <v>18.687999999999999</v>
       </c>
     </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>2025</v>
+      </c>
+      <c r="B41" s="1">
+        <v>45867</v>
+      </c>
+      <c r="C41" s="2">
+        <v>18.764199999999999</v>
+      </c>
+      <c r="D41" s="2">
+        <v>18.829000000000001</v>
+      </c>
+      <c r="E41" s="2">
+        <v>18.728999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>2025</v>
+      </c>
+      <c r="B42" s="1">
+        <v>45868</v>
+      </c>
+      <c r="C42" s="2">
+        <v>18.795999999999999</v>
+      </c>
+      <c r="D42" s="2">
+        <v>18.873999999999999</v>
+      </c>
+      <c r="E42" s="2">
+        <v>18.756</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>2025</v>
+      </c>
+      <c r="B43" s="1">
+        <v>45869</v>
+      </c>
+      <c r="C43" s="2">
+        <v>18.796299999999999</v>
+      </c>
+      <c r="D43" s="2">
+        <v>18.870999999999999</v>
+      </c>
+      <c r="E43" s="2">
+        <v>18.774999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>2025</v>
+      </c>
+      <c r="B44" s="1">
+        <v>45870</v>
+      </c>
+      <c r="C44" s="2">
+        <v>18.916</v>
+      </c>
+      <c r="D44" s="2">
+        <v>18.959</v>
+      </c>
+      <c r="E44" s="2">
+        <v>18.864000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>2025</v>
+      </c>
+      <c r="B45" s="1">
+        <v>45873</v>
+      </c>
+      <c r="C45" s="2">
+        <v>18.878299999999999</v>
+      </c>
+      <c r="D45" s="2">
+        <v>18.956</v>
+      </c>
+      <c r="E45" s="2">
+        <v>18.829000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>2025</v>
+      </c>
+      <c r="B46" s="1">
+        <v>45874</v>
+      </c>
+      <c r="C46" s="2">
+        <v>18.762</v>
+      </c>
+      <c r="D46" s="2">
+        <v>18.824000000000002</v>
+      </c>
+      <c r="E46" s="2">
+        <v>18.719000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>2025</v>
+      </c>
+      <c r="B47" s="1">
+        <v>45875</v>
+      </c>
+      <c r="C47" s="2">
+        <v>18.619199999999999</v>
+      </c>
+      <c r="D47" s="2">
+        <v>18.654</v>
+      </c>
+      <c r="E47" s="2">
+        <v>18.584</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>2025</v>
+      </c>
+      <c r="B48" s="1">
+        <v>45876</v>
+      </c>
+      <c r="C48" s="2">
+        <v>18.676500000000001</v>
+      </c>
+      <c r="D48" s="2">
+        <v>18.73</v>
+      </c>
+      <c r="E48" s="2">
+        <v>18.635999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>2025</v>
+      </c>
+      <c r="B49" s="1">
+        <v>45877</v>
+      </c>
+      <c r="C49" s="2">
+        <v>18.5518</v>
+      </c>
+      <c r="D49" s="2">
+        <v>18.61</v>
+      </c>
+      <c r="E49" s="2">
+        <v>18.527000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>2025</v>
+      </c>
+      <c r="B50" s="1">
+        <v>45880</v>
+      </c>
+      <c r="C50" s="2">
+        <v>18.668299999999999</v>
+      </c>
+      <c r="D50" s="2">
+        <v>18.696000000000002</v>
+      </c>
+      <c r="E50" s="2">
+        <v>18.646999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>2025</v>
+      </c>
+      <c r="B51" s="1">
+        <v>45881</v>
+      </c>
+      <c r="C51" s="2">
+        <v>18.5657</v>
+      </c>
+      <c r="D51" s="2">
+        <v>18.594000000000001</v>
+      </c>
+      <c r="E51" s="2">
+        <v>18.541</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>2025</v>
+      </c>
+      <c r="B52" s="1">
+        <v>45882</v>
+      </c>
+      <c r="C52" s="2">
+        <v>18.635300000000001</v>
+      </c>
+      <c r="D52" s="2">
+        <v>18.667000000000002</v>
+      </c>
+      <c r="E52" s="2">
+        <v>18.617999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>2025</v>
+      </c>
+      <c r="B53" s="1">
+        <v>45883</v>
+      </c>
+      <c r="C53" s="2">
+        <v>18.813700000000001</v>
+      </c>
+      <c r="D53" s="2">
+        <v>18.853000000000002</v>
+      </c>
+      <c r="E53" s="2">
+        <v>18.779</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>2025</v>
+      </c>
+      <c r="B54" s="1">
+        <v>45884</v>
+      </c>
+      <c r="C54" s="2">
+        <v>18.729500000000002</v>
+      </c>
+      <c r="D54" s="2">
+        <v>18.771999999999998</v>
+      </c>
+      <c r="E54" s="2">
+        <v>18.690999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1726,10 +1962,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394FE10B-CC5B-4887-BA9F-8638E71CB003}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43:F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2519,6 +2755,286 @@
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>2025</v>
+      </c>
+      <c r="B40" s="1">
+        <v>45867</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D40" s="4">
+        <v>8.2299999999999998E-2</v>
+      </c>
+      <c r="E40" s="4">
+        <v>8.2900000000000001E-2</v>
+      </c>
+      <c r="F40" s="4">
+        <v>8.3699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>2025</v>
+      </c>
+      <c r="B41" s="1">
+        <v>45868</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D41" s="4">
+        <v>8.2299999999999998E-2</v>
+      </c>
+      <c r="E41" s="4">
+        <v>8.2900000000000001E-2</v>
+      </c>
+      <c r="F41" s="4">
+        <v>8.3699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>2025</v>
+      </c>
+      <c r="B42" s="1">
+        <v>45869</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D42" s="4">
+        <v>8.2299999999999998E-2</v>
+      </c>
+      <c r="E42" s="4">
+        <v>8.2900000000000001E-2</v>
+      </c>
+      <c r="F42" s="4">
+        <v>8.3699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>2025</v>
+      </c>
+      <c r="B43" s="1">
+        <v>45870</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D43" s="4">
+        <v>8.2400000000000001E-2</v>
+      </c>
+      <c r="E43" s="4">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F43" s="4">
+        <v>8.3799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>2025</v>
+      </c>
+      <c r="B44" s="1">
+        <v>45873</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D44" s="4">
+        <v>8.3099999999999993E-2</v>
+      </c>
+      <c r="E44" s="4">
+        <v>8.3699999999999997E-2</v>
+      </c>
+      <c r="F44" s="4">
+        <v>8.4599999999999995E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>2025</v>
+      </c>
+      <c r="B45" s="1">
+        <v>45874</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D45" s="4">
+        <v>8.2400000000000001E-2</v>
+      </c>
+      <c r="E45" s="4">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F45" s="4">
+        <v>8.3799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>2025</v>
+      </c>
+      <c r="B46" s="1">
+        <v>45875</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D46" s="4">
+        <v>8.2400000000000001E-2</v>
+      </c>
+      <c r="E46" s="4">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F46" s="4">
+        <v>8.3799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>2025</v>
+      </c>
+      <c r="B47" s="1">
+        <v>45876</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D47" s="4">
+        <v>8.2400000000000001E-2</v>
+      </c>
+      <c r="E47" s="4">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F47" s="4">
+        <v>8.3799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>2025</v>
+      </c>
+      <c r="B48" s="1">
+        <v>45877</v>
+      </c>
+      <c r="C48" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D48" s="4">
+        <v>8.2400000000000001E-2</v>
+      </c>
+      <c r="E48" s="4">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F48" s="4">
+        <v>8.3799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>2025</v>
+      </c>
+      <c r="B49" s="1">
+        <v>45880</v>
+      </c>
+      <c r="C49" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="E49" s="4">
+        <v>8.0600000000000005E-2</v>
+      </c>
+      <c r="F49" s="4">
+        <v>8.1299999999999997E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>2025</v>
+      </c>
+      <c r="B50" s="1">
+        <v>45881</v>
+      </c>
+      <c r="C50" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D50" s="4">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E50" s="4">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F50" s="4">
+        <v>8.14E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>2025</v>
+      </c>
+      <c r="B51" s="1">
+        <v>45882</v>
+      </c>
+      <c r="C51" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D51" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="E51" s="4">
+        <v>8.0600000000000005E-2</v>
+      </c>
+      <c r="F51" s="4">
+        <v>8.1299999999999997E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>2025</v>
+      </c>
+      <c r="B52" s="1">
+        <v>45883</v>
+      </c>
+      <c r="C52" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D52" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="E52" s="4">
+        <v>8.0600000000000005E-2</v>
+      </c>
+      <c r="F52" s="4">
+        <v>8.1299999999999997E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>2025</v>
+      </c>
+      <c r="B53" s="1">
+        <v>45884</v>
+      </c>
+      <c r="C53" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D53" s="4">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E53" s="4">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F53" s="4">
+        <v>8.14E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
actualización de noticias e indicadores 8.18
</commit_message>
<xml_diff>
--- a/tipo de cambio y tasas de interés.xlsx
+++ b/tipo de cambio y tasas de interés.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7621B9D-97C9-4BA2-A032-15E661B266D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E9FFBF-A1C1-44F7-820E-D891DFD6D154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
   </bookViews>
@@ -547,7 +547,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -556,6 +556,9 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -698,8 +701,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}" name="Tabla1" displayName="Tabla1" ref="A1:E54" totalsRowShown="0" dataDxfId="5" dataCellStyle="Moneda">
-  <autoFilter ref="A1:E54" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}" name="Tabla1" displayName="Tabla1" ref="A1:E55" totalsRowShown="0" dataDxfId="5" dataCellStyle="Moneda">
+  <autoFilter ref="A1:E55" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8E09B427-5E44-4BBB-89FC-35463079BE46}" name="Año"/>
     <tableColumn id="2" xr3:uid="{3D7466AA-D045-44D9-96B5-BDFB7062F58C}" name="Fecha" dataDxfId="4"/>
@@ -712,8 +715,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}" name="Tabla2" displayName="Tabla2" ref="A1:F53" totalsRowShown="0">
-  <autoFilter ref="A1:F53" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}" name="Tabla2" displayName="Tabla2" ref="A1:F54" totalsRowShown="0">
+  <autoFilter ref="A1:F54" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B700B119-8C38-4F55-BC79-C4D6BC8E0C88}" name="Año"/>
     <tableColumn id="2" xr3:uid="{47E09E7D-A904-4405-9048-49D33EE0E8EB}" name="Fecha" dataDxfId="0"/>
@@ -1023,9 +1026,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892B4731-B44C-4F20-9A44-95C4BD8A73FF}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1952,6 +1957,23 @@
         <v>18.690999999999999</v>
       </c>
     </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>2025</v>
+      </c>
+      <c r="B55" s="1">
+        <v>45887</v>
+      </c>
+      <c r="C55" s="2">
+        <v>18.783999999999999</v>
+      </c>
+      <c r="D55" s="2">
+        <v>18.829999999999998</v>
+      </c>
+      <c r="E55" s="2">
+        <v>18.757999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1962,10 +1984,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394FE10B-CC5B-4887-BA9F-8638E71CB003}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43:F53"/>
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3035,6 +3057,26 @@
         <v>8.14E-2</v>
       </c>
     </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>2025</v>
+      </c>
+      <c r="B54" s="1">
+        <v>45887</v>
+      </c>
+      <c r="C54" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D54" s="5">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E54" s="5">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F54" s="5">
+        <v>8.14E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Hice el cambio para que aparezcan los indicadores nuevos aparezcan en resumen
</commit_message>
<xml_diff>
--- a/tipo de cambio y tasas de interés.xlsx
+++ b/tipo de cambio y tasas de interés.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CF75A1-D987-4881-881D-0C99CD4E7BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AEEDEA-E15D-40B8-AB35-AE2DDE16896B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo de Cambio" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Fecha</t>
   </si>
@@ -107,6 +107,15 @@
   <si>
     <t>Nasdaq</t>
   </si>
+  <si>
+    <t>% Dow Jones</t>
+  </si>
+  <si>
+    <t>% S&amp;P500</t>
+  </si>
+  <si>
+    <t>% Nasdaq</t>
+  </si>
 </sst>
 </file>
 
@@ -115,7 +124,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +262,12 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -602,7 +617,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -616,10 +631,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Énfasis1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -668,7 +680,28 @@
     <cellStyle name="Título 3" xfId="6" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="19" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="27">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
@@ -704,18 +737,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
@@ -815,14 +836,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}" name="Tabla1" displayName="Tabla1" ref="A1:E59" totalsRowShown="0" dataDxfId="23" dataCellStyle="Moneda">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}" name="Tabla1" displayName="Tabla1" ref="A1:E59" totalsRowShown="0" dataDxfId="26" dataCellStyle="Moneda">
   <autoFilter ref="A1:E59" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8E09B427-5E44-4BBB-89FC-35463079BE46}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{3D7466AA-D045-44D9-96B5-BDFB7062F58C}" name="Fecha" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{157C7180-B5CE-4C51-9BD0-3AEECF3B91F1}" name="Tipo de Cambio FIX" dataDxfId="21" dataCellStyle="Moneda"/>
-    <tableColumn id="4" xr3:uid="{74B4BBBC-E72A-423F-B8FA-CE596B4E990E}" name="Nivel máximo" dataDxfId="20" dataCellStyle="Moneda"/>
-    <tableColumn id="5" xr3:uid="{74EB6E0A-1398-4291-8596-80BA6140571D}" name="Nivel mínimo" dataDxfId="19" dataCellStyle="Moneda"/>
+    <tableColumn id="2" xr3:uid="{3D7466AA-D045-44D9-96B5-BDFB7062F58C}" name="Fecha" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{157C7180-B5CE-4C51-9BD0-3AEECF3B91F1}" name="Tipo de Cambio FIX" dataDxfId="24" dataCellStyle="Moneda"/>
+    <tableColumn id="4" xr3:uid="{74B4BBBC-E72A-423F-B8FA-CE596B4E990E}" name="Nivel máximo" dataDxfId="23" dataCellStyle="Moneda"/>
+    <tableColumn id="5" xr3:uid="{74EB6E0A-1398-4291-8596-80BA6140571D}" name="Nivel mínimo" dataDxfId="22" dataCellStyle="Moneda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -833,7 +854,7 @@
   <autoFilter ref="A1:F58" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B700B119-8C38-4F55-BC79-C4D6BC8E0C88}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{47E09E7D-A904-4405-9048-49D33EE0E8EB}" name="Fecha" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{47E09E7D-A904-4405-9048-49D33EE0E8EB}" name="Fecha" dataDxfId="21"/>
     <tableColumn id="3" xr3:uid="{0E168449-32EF-450B-812C-11DC4F0F3A30}" name="Tasa de Interés Objetivo"/>
     <tableColumn id="4" xr3:uid="{EE5A2D13-088C-4226-A754-1A001EC14095}" name="TIIE 28 días"/>
     <tableColumn id="5" xr3:uid="{91C093C9-2029-4DE0-AF73-BB6DB79C251D}" name="TIIE 91 días"/>
@@ -848,33 +869,42 @@
   <autoFilter ref="A1:N161" xr:uid="{41D25D3A-81CA-4450-B7DF-F71343E59E89}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{4B709A46-FEF4-4082-A1C7-4443452E16C3}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{288E25E9-721A-4984-9062-39446AEF10A2}" name="Fecha" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{0B60854E-A304-4A5B-B1BD-17AA07CBA4DD}" name="SOFR" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{BA101BB9-5BDD-49C2-A01D-82F8C1F40DE3}" name="1M Treasury" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{7FE75A9A-7044-4B06-B3A6-F01D3A56E2C5}" name="3M Treasury" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{602D7FBF-E731-4F49-9A0B-6365C780F089}" name="6M Treasury" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{7887EB81-463F-4BB8-9E84-4229D2CAC9A1}" name="1Y Treasury" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{8C5475BF-3FF2-497D-B569-0B378CC77D79}" name="2Y Treasury" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{3B424ABE-EF8F-498A-8F4F-7FDBD990A429}" name="3Y Treasury" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{383F89E5-27BF-4792-BA7B-6E4263B946C9}" name="5Y Treasury" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{A94CC5AD-A6E2-4E44-AAAF-147E46B23BA1}" name="7Y Treasury" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{BA073A53-DD09-4842-A47E-B2F4D2CD2F0B}" name="10Y Treasury" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{0AB1292E-1821-4704-ACB3-22F12D9A1EBD}" name="20Y Treasury" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{FCEEF9DA-C290-458F-AEF1-C46CBE6DCD16}" name="30Y Treasury" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{288E25E9-721A-4984-9062-39446AEF10A2}" name="Fecha" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{0B60854E-A304-4A5B-B1BD-17AA07CBA4DD}" name="SOFR" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{BA101BB9-5BDD-49C2-A01D-82F8C1F40DE3}" name="1M Treasury" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{7FE75A9A-7044-4B06-B3A6-F01D3A56E2C5}" name="3M Treasury" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{602D7FBF-E731-4F49-9A0B-6365C780F089}" name="6M Treasury" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{7887EB81-463F-4BB8-9E84-4229D2CAC9A1}" name="1Y Treasury" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{8C5475BF-3FF2-497D-B569-0B378CC77D79}" name="2Y Treasury" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{3B424ABE-EF8F-498A-8F4F-7FDBD990A429}" name="3Y Treasury" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{383F89E5-27BF-4792-BA7B-6E4263B946C9}" name="5Y Treasury" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{A94CC5AD-A6E2-4E44-AAAF-147E46B23BA1}" name="7Y Treasury" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{BA073A53-DD09-4842-A47E-B2F4D2CD2F0B}" name="10Y Treasury" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{0AB1292E-1821-4704-ACB3-22F12D9A1EBD}" name="20Y Treasury" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{FCEEF9DA-C290-458F-AEF1-C46CBE6DCD16}" name="30Y Treasury" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}" name="Tabla8" displayName="Tabla8" ref="A1:E17" totalsRowShown="0">
-  <autoFilter ref="A1:E17" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}" name="Tabla8" displayName="Tabla8" ref="A1:H17" totalsRowShown="0">
+  <autoFilter ref="A1:H17" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{7676C863-947F-4296-8B2C-4C1C2493E9D9}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{55C318C8-9926-4D62-8294-177D6BC0FE75}" name="Fecha" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{55C318C8-9926-4D62-8294-177D6BC0FE75}" name="Fecha" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{1D145B8D-1465-4EF3-BECF-49ACE623BEC5}" name="Dow Jones"/>
     <tableColumn id="4" xr3:uid="{F2357A84-5C07-4E65-841A-42DAECACF403}" name="S&amp;P 500"/>
     <tableColumn id="5" xr3:uid="{388751CA-0A21-4A09-8009-2BB8B01233CE}" name="Nasdaq"/>
+    <tableColumn id="6" xr3:uid="{DEF693B5-3B7C-424D-8BCC-52947BCEC3CF}" name="% Dow Jones" dataDxfId="2">
+      <calculatedColumnFormula>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C1)/C1,"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{A64DA0F4-44F9-4388-B98F-ED267001BCC9}" name="% S&amp;P500" dataDxfId="1">
+      <calculatedColumnFormula>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D1)/D1,"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{9B8FC688-A5F6-4240-9AD9-64ED7FF46AD3}" name="% Nasdaq" dataDxfId="0">
+      <calculatedColumnFormula>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E1)/E1,"")</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -885,8 +915,8 @@
   <autoFilter ref="A1:C8" xr:uid="{B90FD302-37FE-4F2B-B60B-6A456523923A}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{43F48A9D-2FA0-46A3-84F1-7DEE42E5BF68}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{1AFFE9F5-0B80-4822-A1EA-DB386C299969}" name="Fecha" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{AF83158D-8EA0-4564-B3B9-6FD4F520FAE8}" name="Inflación USA" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{1AFFE9F5-0B80-4822-A1EA-DB386C299969}" name="Fecha" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{AF83158D-8EA0-4564-B3B9-6FD4F520FAE8}" name="Inflación USA" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -897,8 +927,8 @@
   <autoFilter ref="A1:C236" xr:uid="{009B3244-9A58-400B-AA1A-8898DAD1E764}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E37380EC-24C2-4BFF-B1C3-8DCA648F7DEC}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{0FEF90E7-9017-40CF-A119-2A51A7A5DB93}" name="Fecha" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{FC4B62C3-96EC-4423-AE57-348DA8F8FEC3}" name="Inflación México" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{0FEF90E7-9017-40CF-A119-2A51A7A5DB93}" name="Fecha" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{FC4B62C3-96EC-4423-AE57-348DA8F8FEC3}" name="Inflación México" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1203,7 +1233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892B4731-B44C-4F20-9A44-95C4BD8A73FF}">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
@@ -2150,7 +2180,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="10">
+      <c r="A56">
         <v>2025</v>
       </c>
       <c r="B56" s="1">
@@ -2167,7 +2197,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="10">
+      <c r="A57">
         <v>2025</v>
       </c>
       <c r="B57" s="1">
@@ -2184,7 +2214,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="10">
+      <c r="A58">
         <v>2025</v>
       </c>
       <c r="B58" s="1">
@@ -2201,7 +2231,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="10">
+      <c r="A59">
         <v>2025</v>
       </c>
       <c r="B59" s="1">
@@ -3321,7 +3351,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="9">
+      <c r="A55">
         <v>2025</v>
       </c>
       <c r="B55" s="1">
@@ -3341,7 +3371,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="9">
+      <c r="A56">
         <v>2025</v>
       </c>
       <c r="B56" s="1">
@@ -3361,7 +3391,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="9">
+      <c r="A57">
         <v>2025</v>
       </c>
       <c r="B57" s="1">
@@ -3381,7 +3411,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="9">
+      <c r="A58">
         <v>2025</v>
       </c>
       <c r="B58" s="1">
@@ -3412,8 +3442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B7A3E5-7422-42F6-B226-5BFEA691299B}">
   <dimension ref="A1:N161"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:N161"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10518,308 +10548,509 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6F7ED1-F67A-4D3F-B065-CA644B535717}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E17"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="7"/>
     <col min="3" max="3" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>2025</v>
       </c>
       <c r="B2" s="1">
         <v>45870</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2">
         <v>43588.578125</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2">
         <v>6238.009765625</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2">
         <v>20650.130859375</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
+      <c r="F2" t="str">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C1)/C1,"")</f>
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D1)/D1,"")</f>
+        <v/>
+      </c>
+      <c r="H2" t="str">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E1)/E1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>2025</v>
       </c>
       <c r="B3" s="1">
         <v>45873</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3">
         <v>44173.640625</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3">
         <v>6329.93994140625</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3">
         <v>21053.580078125</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
+      <c r="F3" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C2)/C2,"")</f>
+        <v>1.3422380934799074E-2</v>
+      </c>
+      <c r="G3" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D2)/D2,"")</f>
+        <v>1.4737100330916093E-2</v>
+      </c>
+      <c r="H3" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E2)/E2,"")</f>
+        <v>1.9537368624801578E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>2025</v>
       </c>
       <c r="B4" s="1">
         <v>45874</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4">
         <v>44111.73828125</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4">
         <v>6299.18994140625</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4">
         <v>20916.55078125</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+      <c r="F4" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C3)/C3,"")</f>
+        <v>-1.4013412268982527E-3</v>
+      </c>
+      <c r="G4" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D3)/D3,"")</f>
+        <v>-4.8578659963033751E-3</v>
+      </c>
+      <c r="H4" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E3)/E3,"")</f>
+        <v>-6.5085983650531526E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>2025</v>
       </c>
       <c r="B5" s="1">
         <v>45875</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5">
         <v>44193.12109375</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5">
         <v>6345.06005859375</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5">
         <v>21169.419921875</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
+      <c r="F5" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C4)/C4,"")</f>
+        <v>1.8449241782564785E-3</v>
+      </c>
+      <c r="G5" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D4)/D4,"")</f>
+        <v>7.2819072950925838E-3</v>
+      </c>
+      <c r="H5" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E4)/E4,"")</f>
+        <v>1.2089428284307601E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>2025</v>
       </c>
       <c r="B6" s="1">
         <v>45876</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6">
         <v>43968.640625</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6">
         <v>6340</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6">
         <v>21242.69921875</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+      <c r="F6" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C5)/C5,"")</f>
+        <v>-5.0795341717049958E-3</v>
+      </c>
+      <c r="G6" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D5)/D5,"")</f>
+        <v>-7.9748001548017751E-4</v>
+      </c>
+      <c r="H6" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E5)/E5,"")</f>
+        <v>3.4615637625137895E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>2025</v>
       </c>
       <c r="B7" s="1">
         <v>45877</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7">
         <v>44175.609375</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7">
         <v>6389.4501953125</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7">
         <v>21450.01953125</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
+      <c r="F7" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C6)/C6,"")</f>
+        <v>4.7071901031736753E-3</v>
+      </c>
+      <c r="G7" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D6)/D6,"")</f>
+        <v>7.7997153489747636E-3</v>
+      </c>
+      <c r="H7" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E6)/E6,"")</f>
+        <v>9.759603069510462E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>2025</v>
       </c>
       <c r="B8" s="1">
         <v>45880</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8">
         <v>43975.08984375</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8">
         <v>6373.4501953125</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8">
         <v>21385.400390625</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+      <c r="F8" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C7)/C7,"")</f>
+        <v>-4.5391457885237156E-3</v>
+      </c>
+      <c r="G8" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D7)/D7,"")</f>
+        <v>-2.5041278217863092E-3</v>
+      </c>
+      <c r="H8" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E7)/E7,"")</f>
+        <v>-3.012544605419029E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>2025</v>
       </c>
       <c r="B9" s="1">
         <v>45881</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9">
         <v>44458.609375</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9">
         <v>6445.759765625</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9">
         <v>21681.900390625</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
+      <c r="F9" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C8)/C8,"")</f>
+        <v>1.0995305136794864E-2</v>
+      </c>
+      <c r="G9" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D8)/D8,"")</f>
+        <v>1.1345435846612833E-2</v>
+      </c>
+      <c r="H9" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E8)/E8,"")</f>
+        <v>1.3864598959296578E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>2025</v>
       </c>
       <c r="B10" s="1">
         <v>45882</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10">
         <v>44922.26953125</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10">
         <v>6466.580078125</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10">
         <v>21713.140625</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
+      <c r="F10" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C9)/C9,"")</f>
+        <v>1.0429029669801722E-2</v>
+      </c>
+      <c r="G10" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D9)/D9,"")</f>
+        <v>3.2300788824048271E-3</v>
+      </c>
+      <c r="H10" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E9)/E9,"")</f>
+        <v>1.4408439210664354E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>2025</v>
       </c>
       <c r="B11" s="1">
         <v>45883</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11">
         <v>44911.26171875</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11">
         <v>6468.5400390625</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11">
         <v>21710.669921875</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
+      <c r="F11" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C10)/C10,"")</f>
+        <v>-2.4504132615878763E-4</v>
+      </c>
+      <c r="G11" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D10)/D10,"")</f>
+        <v>3.0309080129234172E-4</v>
+      </c>
+      <c r="H11" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E10)/E10,"")</f>
+        <v>-1.1378838131574989E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>2025</v>
       </c>
       <c r="B12" s="1">
         <v>45884</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12">
         <v>44946.12109375</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12">
         <v>6449.7998046875</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12">
         <v>21622.98046875</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
+      <c r="F12" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C11)/C11,"")</f>
+        <v>7.7618338176071685E-4</v>
+      </c>
+      <c r="G12" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D11)/D11,"")</f>
+        <v>-2.8971350972291521E-3</v>
+      </c>
+      <c r="H12" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E11)/E11,"")</f>
+        <v>-4.0390026397410621E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>2025</v>
       </c>
       <c r="B13" s="1">
         <v>45887</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13">
         <v>44911.8203125</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13">
         <v>6449.14990234375</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13">
         <v>21629.76953125</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="8">
+      <c r="F13" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C12)/C12,"")</f>
+        <v>-7.6315331368538737E-4</v>
+      </c>
+      <c r="G13" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D12)/D12,"")</f>
+        <v>-1.0076318078549857E-4</v>
+      </c>
+      <c r="H13" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E12)/E12,"")</f>
+        <v>3.1397440837592673E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>2025</v>
       </c>
       <c r="B14" s="1">
         <v>45888</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14">
         <v>44922.26953125</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14">
         <v>6411.3701171875</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14">
         <v>21314.94921875</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
+      <c r="F14" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C13)/C13,"")</f>
+        <v>2.3266077120218039E-4</v>
+      </c>
+      <c r="G14" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D13)/D13,"")</f>
+        <v>-5.8581031187567951E-3</v>
+      </c>
+      <c r="H14" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E13)/E13,"")</f>
+        <v>-1.4554954552111971E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>2025</v>
       </c>
       <c r="B15" s="1">
         <v>45889</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15">
         <v>44938.30859375</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15">
         <v>6395.77978515625</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15">
         <v>21172.859375</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="8">
+      <c r="F15" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C14)/C14,"")</f>
+        <v>3.5704034251525269E-4</v>
+      </c>
+      <c r="G15" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D14)/D14,"")</f>
+        <v>-2.431669322826284E-3</v>
+      </c>
+      <c r="H15" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E14)/E14,"")</f>
+        <v>-6.6662060646622903E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>2025</v>
       </c>
       <c r="B16" s="1">
         <v>45890</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16">
         <v>44785.5</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16">
         <v>6370.169921875</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16">
         <v>21100.310546875</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="8">
+      <c r="F16" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C15)/C15,"")</f>
+        <v>-3.4004082158813728E-3</v>
+      </c>
+      <c r="G16" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D15)/D15,"")</f>
+        <v>-4.0041815293089152E-3</v>
+      </c>
+      <c r="H16" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E15)/E15,"")</f>
+        <v>-3.4265012032650881E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>2025</v>
       </c>
       <c r="B17" s="1">
         <v>45891</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17">
         <v>45631.73828125</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17">
         <v>6466.91015625</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17">
         <v>21496.5390625</v>
       </c>
+      <c r="F17" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C16)/C16,"")</f>
+        <v>1.8895363036027287E-2</v>
+      </c>
+      <c r="G17" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D16)/D16,"")</f>
+        <v>1.5186444876893553E-2</v>
+      </c>
+      <c r="H17" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E16)/E16,"")</f>
+        <v>1.8778326259453193E-2</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
actualizar indicadores económicos y de noticias hasta el 29 de agosot, así como meter inflación al endpoint de correo
</commit_message>
<xml_diff>
--- a/tipo de cambio y tasas de interés.xlsx
+++ b/tipo de cambio y tasas de interés.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AEEDEA-E15D-40B8-AB35-AE2DDE16896B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB37441D-11BE-4B59-8A9F-31EF5918CC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo de Cambio" sheetId="1" r:id="rId1"/>
@@ -617,7 +617,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -632,6 +632,9 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Énfasis1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -682,15 +685,6 @@
   </cellStyles>
   <dxfs count="27">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
@@ -701,6 +695,15 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -836,8 +839,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}" name="Tabla1" displayName="Tabla1" ref="A1:E59" totalsRowShown="0" dataDxfId="26" dataCellStyle="Moneda">
-  <autoFilter ref="A1:E59" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}" name="Tabla1" displayName="Tabla1" ref="A1:E64" totalsRowShown="0" dataDxfId="26" dataCellStyle="Moneda">
+  <autoFilter ref="A1:E64" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8E09B427-5E44-4BBB-89FC-35463079BE46}" name="Año"/>
     <tableColumn id="2" xr3:uid="{3D7466AA-D045-44D9-96B5-BDFB7062F58C}" name="Fecha" dataDxfId="25"/>
@@ -850,8 +853,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}" name="Tabla2" displayName="Tabla2" ref="A1:F58" totalsRowShown="0">
-  <autoFilter ref="A1:F58" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}" name="Tabla2" displayName="Tabla2" ref="A1:F63" totalsRowShown="0">
+  <autoFilter ref="A1:F63" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B700B119-8C38-4F55-BC79-C4D6BC8E0C88}" name="Año"/>
     <tableColumn id="2" xr3:uid="{47E09E7D-A904-4405-9048-49D33EE0E8EB}" name="Fecha" dataDxfId="21"/>
@@ -865,8 +868,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{41D25D3A-81CA-4450-B7DF-F71343E59E89}" name="Tabla7" displayName="Tabla7" ref="A1:N161" totalsRowShown="0">
-  <autoFilter ref="A1:N161" xr:uid="{41D25D3A-81CA-4450-B7DF-F71343E59E89}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{41D25D3A-81CA-4450-B7DF-F71343E59E89}" name="Tabla7" displayName="Tabla7" ref="A1:N167" totalsRowShown="0">
+  <autoFilter ref="A1:N167" xr:uid="{41D25D3A-81CA-4450-B7DF-F71343E59E89}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{4B709A46-FEF4-4082-A1C7-4443452E16C3}" name="Año"/>
     <tableColumn id="2" xr3:uid="{288E25E9-721A-4984-9062-39446AEF10A2}" name="Fecha" dataDxfId="20"/>
@@ -888,21 +891,21 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}" name="Tabla8" displayName="Tabla8" ref="A1:H17" totalsRowShown="0">
-  <autoFilter ref="A1:H17" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}" name="Tabla8" displayName="Tabla8" ref="A1:H22" totalsRowShown="0">
+  <autoFilter ref="A1:H22" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{7676C863-947F-4296-8B2C-4C1C2493E9D9}" name="Año"/>
     <tableColumn id="2" xr3:uid="{55C318C8-9926-4D62-8294-177D6BC0FE75}" name="Fecha" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{1D145B8D-1465-4EF3-BECF-49ACE623BEC5}" name="Dow Jones"/>
     <tableColumn id="4" xr3:uid="{F2357A84-5C07-4E65-841A-42DAECACF403}" name="S&amp;P 500"/>
     <tableColumn id="5" xr3:uid="{388751CA-0A21-4A09-8009-2BB8B01233CE}" name="Nasdaq"/>
-    <tableColumn id="6" xr3:uid="{DEF693B5-3B7C-424D-8BCC-52947BCEC3CF}" name="% Dow Jones" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{DEF693B5-3B7C-424D-8BCC-52947BCEC3CF}" name="% Dow Jones" dataDxfId="6">
       <calculatedColumnFormula>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C1)/C1,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{A64DA0F4-44F9-4388-B98F-ED267001BCC9}" name="% S&amp;P500" dataDxfId="1">
+    <tableColumn id="7" xr3:uid="{A64DA0F4-44F9-4388-B98F-ED267001BCC9}" name="% S&amp;P500" dataDxfId="5">
       <calculatedColumnFormula>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D1)/D1,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{9B8FC688-A5F6-4240-9AD9-64ED7FF46AD3}" name="% Nasdaq" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{9B8FC688-A5F6-4240-9AD9-64ED7FF46AD3}" name="% Nasdaq" dataDxfId="4">
       <calculatedColumnFormula>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E1)/E1,"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -915,20 +918,23 @@
   <autoFilter ref="A1:C8" xr:uid="{B90FD302-37FE-4F2B-B60B-6A456523923A}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{43F48A9D-2FA0-46A3-84F1-7DEE42E5BF68}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{1AFFE9F5-0B80-4822-A1EA-DB386C299969}" name="Fecha" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{AF83158D-8EA0-4564-B3B9-6FD4F520FAE8}" name="Inflación USA" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{1AFFE9F5-0B80-4822-A1EA-DB386C299969}" name="Fecha" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{AF83158D-8EA0-4564-B3B9-6FD4F520FAE8}" name="Inflación USA" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{009B3244-9A58-400B-AA1A-8898DAD1E764}" name="Tabla26" displayName="Tabla26" ref="A1:C236" totalsRowShown="0">
-  <autoFilter ref="A1:C236" xr:uid="{009B3244-9A58-400B-AA1A-8898DAD1E764}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{009B3244-9A58-400B-AA1A-8898DAD1E764}" name="Tabla26" displayName="Tabla26" ref="A1:C242" totalsRowShown="0">
+  <autoFilter ref="A1:C242" xr:uid="{009B3244-9A58-400B-AA1A-8898DAD1E764}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C236">
+    <sortCondition ref="B1:B236"/>
+  </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E37380EC-24C2-4BFF-B1C3-8DCA648F7DEC}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{0FEF90E7-9017-40CF-A119-2A51A7A5DB93}" name="Fecha" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{FC4B62C3-96EC-4423-AE57-348DA8F8FEC3}" name="Inflación México" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{0FEF90E7-9017-40CF-A119-2A51A7A5DB93}" name="Fecha" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{FC4B62C3-96EC-4423-AE57-348DA8F8FEC3}" name="Inflación México" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1231,10 +1237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892B4731-B44C-4F20-9A44-95C4BD8A73FF}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65:E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2247,6 +2253,91 @@
         <v>18.577999999999999</v>
       </c>
     </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>2025</v>
+      </c>
+      <c r="B60" s="1">
+        <v>45894</v>
+      </c>
+      <c r="C60" s="2">
+        <v>18.636800000000001</v>
+      </c>
+      <c r="D60" s="2">
+        <v>18.696000000000002</v>
+      </c>
+      <c r="E60" s="2">
+        <v>18.574000000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>2025</v>
+      </c>
+      <c r="B61" s="1">
+        <v>45895</v>
+      </c>
+      <c r="C61" s="2">
+        <v>18.6843</v>
+      </c>
+      <c r="D61" s="2">
+        <v>18.704999999999998</v>
+      </c>
+      <c r="E61" s="2">
+        <v>18.655999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>2025</v>
+      </c>
+      <c r="B62" s="1">
+        <v>45896</v>
+      </c>
+      <c r="C62" s="2">
+        <v>18.691199999999998</v>
+      </c>
+      <c r="D62" s="2">
+        <v>18.768000000000001</v>
+      </c>
+      <c r="E62" s="2">
+        <v>18.658999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>2025</v>
+      </c>
+      <c r="B63" s="1">
+        <v>45897</v>
+      </c>
+      <c r="C63" s="2">
+        <v>18.652200000000001</v>
+      </c>
+      <c r="D63" s="2">
+        <v>18.681000000000001</v>
+      </c>
+      <c r="E63" s="2">
+        <v>18.63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>2025</v>
+      </c>
+      <c r="B64" s="1">
+        <v>45898</v>
+      </c>
+      <c r="C64" s="2">
+        <v>18.643999999999998</v>
+      </c>
+      <c r="D64" s="2">
+        <v>18.669</v>
+      </c>
+      <c r="E64" s="2">
+        <v>18.628</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2257,10 +2348,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394FE10B-CC5B-4887-BA9F-8638E71CB003}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64:F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3430,6 +3521,106 @@
         <v>8.1600000000000006E-2</v>
       </c>
     </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>2025</v>
+      </c>
+      <c r="B59" s="8">
+        <v>45894</v>
+      </c>
+      <c r="C59" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D59" s="4">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="E59" s="4">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="F59" s="4">
+        <v>8.1500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>2025</v>
+      </c>
+      <c r="B60" s="8">
+        <v>45895</v>
+      </c>
+      <c r="C60" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D60" s="4">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E60" s="4">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F60" s="4">
+        <v>8.14E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>2025</v>
+      </c>
+      <c r="B61" s="8">
+        <v>45896</v>
+      </c>
+      <c r="C61" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D61" s="4">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="E61" s="4">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="F61" s="4">
+        <v>8.1500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>2025</v>
+      </c>
+      <c r="B62" s="8">
+        <v>45897</v>
+      </c>
+      <c r="C62" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D62" s="4">
+        <v>8.0299999999999996E-2</v>
+      </c>
+      <c r="E62" s="4">
+        <v>8.09E-2</v>
+      </c>
+      <c r="F62" s="4">
+        <v>8.1600000000000006E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>2025</v>
+      </c>
+      <c r="B63" s="8">
+        <v>45898</v>
+      </c>
+      <c r="C63" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D63" s="4">
+        <v>8.0299999999999996E-2</v>
+      </c>
+      <c r="E63" s="4">
+        <v>8.09E-2</v>
+      </c>
+      <c r="F63" s="4">
+        <v>8.1600000000000006E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3440,10 +3631,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B7A3E5-7422-42F6-B226-5BFEA691299B}">
-  <dimension ref="A1:N161"/>
+  <dimension ref="A1:N167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="A168" sqref="A168:N169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10538,6 +10729,270 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
+    <row r="162" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>2025</v>
+      </c>
+      <c r="B162" s="1">
+        <v>45891</v>
+      </c>
+      <c r="C162" s="6">
+        <v>4.36E-2</v>
+      </c>
+      <c r="D162" s="6">
+        <v>4.4699999999999997E-2</v>
+      </c>
+      <c r="E162" s="6">
+        <v>4.2700000000000002E-2</v>
+      </c>
+      <c r="F162" s="6">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="G162" s="6">
+        <v>3.8699999999999998E-2</v>
+      </c>
+      <c r="H162" s="6">
+        <v>3.6799999999999999E-2</v>
+      </c>
+      <c r="I162" s="6">
+        <v>3.6400000000000002E-2</v>
+      </c>
+      <c r="J162" s="6">
+        <v>3.7600000000000001E-2</v>
+      </c>
+      <c r="K162" s="6">
+        <v>3.9800000000000002E-2</v>
+      </c>
+      <c r="L162" s="6">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="M162" s="6">
+        <v>4.8399999999999999E-2</v>
+      </c>
+      <c r="N162" s="6">
+        <v>4.8800000000000003E-2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>2025</v>
+      </c>
+      <c r="B163" s="1">
+        <v>45894</v>
+      </c>
+      <c r="C163" s="6">
+        <v>4.3700000000000003E-2</v>
+      </c>
+      <c r="D163" s="6">
+        <v>4.4499999999999998E-2</v>
+      </c>
+      <c r="E163" s="6">
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="F163" s="6">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="G163" s="6">
+        <v>3.8800000000000001E-2</v>
+      </c>
+      <c r="H163" s="6">
+        <v>3.73E-2</v>
+      </c>
+      <c r="I163" s="6">
+        <v>3.6799999999999999E-2</v>
+      </c>
+      <c r="J163" s="6">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="K163" s="6">
+        <v>4.0099999999999997E-2</v>
+      </c>
+      <c r="L163" s="6">
+        <v>4.2799999999999998E-2</v>
+      </c>
+      <c r="M163" s="6">
+        <v>4.8599999999999997E-2</v>
+      </c>
+      <c r="N163" s="6">
+        <v>4.8899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>2025</v>
+      </c>
+      <c r="B164" s="1">
+        <v>45895</v>
+      </c>
+      <c r="C164" s="6">
+        <v>4.3799999999999999E-2</v>
+      </c>
+      <c r="D164" s="6">
+        <v>4.4200000000000003E-2</v>
+      </c>
+      <c r="E164" s="6">
+        <v>4.2799999999999998E-2</v>
+      </c>
+      <c r="F164" s="6">
+        <v>4.0599999999999997E-2</v>
+      </c>
+      <c r="G164" s="6">
+        <v>3.85E-2</v>
+      </c>
+      <c r="H164" s="6">
+        <v>3.61E-2</v>
+      </c>
+      <c r="I164" s="6">
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="J164" s="6">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="K164" s="6">
+        <v>3.9800000000000002E-2</v>
+      </c>
+      <c r="L164" s="6">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="M164" s="6">
+        <v>4.8599999999999997E-2</v>
+      </c>
+      <c r="N164" s="6">
+        <v>4.9000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>2025</v>
+      </c>
+      <c r="B165" s="1">
+        <v>45896</v>
+      </c>
+      <c r="C165" s="6">
+        <v>4.36E-2</v>
+      </c>
+      <c r="D165" s="6">
+        <v>4.4200000000000003E-2</v>
+      </c>
+      <c r="E165" s="6">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="F165" s="6">
+        <v>4.0399999999999998E-2</v>
+      </c>
+      <c r="G165" s="6">
+        <v>3.8300000000000001E-2</v>
+      </c>
+      <c r="H165" s="6">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="I165" s="6">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="J165" s="6">
+        <v>3.6900000000000002E-2</v>
+      </c>
+      <c r="K165" s="6">
+        <v>3.95E-2</v>
+      </c>
+      <c r="L165" s="6">
+        <v>4.24E-2</v>
+      </c>
+      <c r="M165" s="6">
+        <v>4.87E-2</v>
+      </c>
+      <c r="N165" s="6">
+        <v>4.9099999999999998E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>2025</v>
+      </c>
+      <c r="B166" s="1">
+        <v>45897</v>
+      </c>
+      <c r="C166" s="6">
+        <v>4.3400000000000001E-2</v>
+      </c>
+      <c r="D166" s="6">
+        <v>4.4200000000000003E-2</v>
+      </c>
+      <c r="E166" s="6">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="F166" s="6">
+        <v>4.0399999999999998E-2</v>
+      </c>
+      <c r="G166" s="6">
+        <v>3.85E-2</v>
+      </c>
+      <c r="H166" s="6">
+        <v>3.6200000000000003E-2</v>
+      </c>
+      <c r="I166" s="6">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="J166" s="6">
+        <v>3.6900000000000002E-2</v>
+      </c>
+      <c r="K166" s="6">
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="L166" s="6">
+        <v>4.2200000000000001E-2</v>
+      </c>
+      <c r="M166" s="6">
+        <v>4.8300000000000003E-2</v>
+      </c>
+      <c r="N166" s="6">
+        <v>4.8800000000000003E-2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>2025</v>
+      </c>
+      <c r="B167" s="1">
+        <v>45898</v>
+      </c>
+      <c r="C167" s="6">
+        <v>4.3400000000000001E-2</v>
+      </c>
+      <c r="D167" s="6">
+        <v>4.41E-2</v>
+      </c>
+      <c r="E167" s="6">
+        <v>4.2299999999999997E-2</v>
+      </c>
+      <c r="F167" s="6">
+        <v>4.0099999999999997E-2</v>
+      </c>
+      <c r="G167" s="6">
+        <v>3.8300000000000001E-2</v>
+      </c>
+      <c r="H167" s="6">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="I167" s="6">
+        <v>3.5799999999999998E-2</v>
+      </c>
+      <c r="J167" s="6">
+        <v>3.6799999999999999E-2</v>
+      </c>
+      <c r="K167" s="6">
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="L167" s="6">
+        <v>4.2299999999999997E-2</v>
+      </c>
+      <c r="M167" s="6">
+        <v>4.8599999999999997E-2</v>
+      </c>
+      <c r="N167" s="6">
+        <v>4.9200000000000001E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -10548,10 +11003,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6F7ED1-F67A-4D3F-B065-CA644B535717}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11047,6 +11502,151 @@
       <c r="H17" s="7">
         <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E16)/E16,"")</f>
         <v>1.8778326259453193E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2025</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45894</v>
+      </c>
+      <c r="C18">
+        <v>45282.46875</v>
+      </c>
+      <c r="D18">
+        <v>6439.31982421875</v>
+      </c>
+      <c r="E18">
+        <v>21449.2890625</v>
+      </c>
+      <c r="F18" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C17)/C17,"")</f>
+        <v>-7.6540921824473701E-3</v>
+      </c>
+      <c r="G18" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D17)/D17,"")</f>
+        <v>-4.2663855480634888E-3</v>
+      </c>
+      <c r="H18" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E17)/E17,"")</f>
+        <v>-2.1980282436453251E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2025</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45895</v>
+      </c>
+      <c r="C19">
+        <v>45418.0703125</v>
+      </c>
+      <c r="D19">
+        <v>6465.93994140625</v>
+      </c>
+      <c r="E19">
+        <v>21544.26953125</v>
+      </c>
+      <c r="F19" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C18)/C18,"")</f>
+        <v>2.9945708845655638E-3</v>
+      </c>
+      <c r="G19" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D18)/D18,"")</f>
+        <v>4.1339951911349088E-3</v>
+      </c>
+      <c r="H19" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E18)/E18,"")</f>
+        <v>4.4281406471441175E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2025</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45896</v>
+      </c>
+      <c r="C20">
+        <v>45565.23046875</v>
+      </c>
+      <c r="D20">
+        <v>6481.39990234375</v>
+      </c>
+      <c r="E20">
+        <v>21590.140625</v>
+      </c>
+      <c r="F20" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C19)/C19,"")</f>
+        <v>3.2401234847156961E-3</v>
+      </c>
+      <c r="G20" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D19)/D19,"")</f>
+        <v>2.3909843081743316E-3</v>
+      </c>
+      <c r="H20" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E19)/E19,"")</f>
+        <v>2.129155211480431E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2025</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45897</v>
+      </c>
+      <c r="C21">
+        <v>45636.8984375</v>
+      </c>
+      <c r="D21">
+        <v>6501.85986328125</v>
+      </c>
+      <c r="E21">
+        <v>21705.16015625</v>
+      </c>
+      <c r="F21" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C20)/C20,"")</f>
+        <v>1.5728652749633744E-3</v>
+      </c>
+      <c r="G21" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D20)/D20,"")</f>
+        <v>3.1567194195348813E-3</v>
+      </c>
+      <c r="H21" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E20)/E20,"")</f>
+        <v>5.327410008474644E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2025</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45898</v>
+      </c>
+      <c r="C22">
+        <v>45544.87890625</v>
+      </c>
+      <c r="D22">
+        <v>6460.259765625</v>
+      </c>
+      <c r="E22">
+        <v>21455.55078125</v>
+      </c>
+      <c r="F22" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C21)/C21,"")</f>
+        <v>-2.0163406015862645E-3</v>
+      </c>
+      <c r="G22" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D21)/D21,"")</f>
+        <v>-6.3981842935716482E-3</v>
+      </c>
+      <c r="H22" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E21)/E21,"")</f>
+        <v>-1.1500001529734162E-2</v>
       </c>
     </row>
   </sheetData>
@@ -11063,7 +11663,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11169,10 +11769,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18AC3A63-0138-40B1-8185-B511FBB18C5E}">
-  <dimension ref="A1:C236"/>
+  <dimension ref="A1:C242"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11204,10 +11804,10 @@
         <v>2025</v>
       </c>
       <c r="B3" s="1">
-        <v>45689</v>
+        <v>45659</v>
       </c>
       <c r="C3" s="6">
-        <v>8.3699999999999997E-2</v>
+        <v>8.3500000000000005E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -11215,10 +11815,10 @@
         <v>2025</v>
       </c>
       <c r="B4" s="1">
-        <v>45717</v>
+        <v>45660</v>
       </c>
       <c r="C4" s="6">
-        <v>8.4000000000000005E-2</v>
+        <v>8.3500000000000005E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -11226,10 +11826,10 @@
         <v>2025</v>
       </c>
       <c r="B5" s="1">
-        <v>45748</v>
+        <v>45661</v>
       </c>
       <c r="C5" s="6">
-        <v>8.4199999999999997E-2</v>
+        <v>8.3500000000000005E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -11237,10 +11837,10 @@
         <v>2025</v>
       </c>
       <c r="B6" s="1">
-        <v>45778</v>
+        <v>45662</v>
       </c>
       <c r="C6" s="6">
-        <v>8.4500000000000006E-2</v>
+        <v>8.3500000000000005E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -11248,10 +11848,10 @@
         <v>2025</v>
       </c>
       <c r="B7" s="1">
-        <v>45809</v>
+        <v>45663</v>
       </c>
       <c r="C7" s="6">
-        <v>8.48E-2</v>
+        <v>8.3500000000000005E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -11259,10 +11859,10 @@
         <v>2025</v>
       </c>
       <c r="B8" s="1">
-        <v>45839</v>
+        <v>45664</v>
       </c>
       <c r="C8" s="6">
-        <v>8.5000000000000006E-2</v>
+        <v>8.3599999999999994E-2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -11270,10 +11870,10 @@
         <v>2025</v>
       </c>
       <c r="B9" s="1">
-        <v>45870</v>
+        <v>45665</v>
       </c>
       <c r="C9" s="6">
-        <v>8.5300000000000001E-2</v>
+        <v>8.3599999999999994E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -11281,10 +11881,10 @@
         <v>2025</v>
       </c>
       <c r="B10" s="1">
-        <v>45659</v>
+        <v>45666</v>
       </c>
       <c r="C10" s="6">
-        <v>8.3500000000000005E-2</v>
+        <v>8.3599999999999994E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -11292,10 +11892,10 @@
         <v>2025</v>
       </c>
       <c r="B11" s="1">
-        <v>45690</v>
+        <v>45667</v>
       </c>
       <c r="C11" s="6">
-        <v>8.3699999999999997E-2</v>
+        <v>8.3599999999999994E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -11303,10 +11903,10 @@
         <v>2025</v>
       </c>
       <c r="B12" s="1">
-        <v>45718</v>
+        <v>45668</v>
       </c>
       <c r="C12" s="6">
-        <v>8.4000000000000005E-2</v>
+        <v>8.3599999999999994E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -11314,10 +11914,10 @@
         <v>2025</v>
       </c>
       <c r="B13" s="1">
-        <v>45749</v>
+        <v>45669</v>
       </c>
       <c r="C13" s="6">
-        <v>8.4199999999999997E-2</v>
+        <v>8.3599999999999994E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -11325,10 +11925,10 @@
         <v>2025</v>
       </c>
       <c r="B14" s="1">
-        <v>45779</v>
+        <v>45670</v>
       </c>
       <c r="C14" s="6">
-        <v>8.4500000000000006E-2</v>
+        <v>8.3599999999999994E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -11336,10 +11936,10 @@
         <v>2025</v>
       </c>
       <c r="B15" s="1">
-        <v>45810</v>
+        <v>45671</v>
       </c>
       <c r="C15" s="6">
-        <v>8.48E-2</v>
+        <v>8.3599999999999994E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -11347,10 +11947,10 @@
         <v>2025</v>
       </c>
       <c r="B16" s="1">
-        <v>45840</v>
+        <v>45672</v>
       </c>
       <c r="C16" s="6">
-        <v>8.5000000000000006E-2</v>
+        <v>8.3599999999999994E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -11358,10 +11958,10 @@
         <v>2025</v>
       </c>
       <c r="B17" s="1">
-        <v>45871</v>
+        <v>45673</v>
       </c>
       <c r="C17" s="6">
-        <v>8.5300000000000001E-2</v>
+        <v>8.3599999999999994E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -11369,10 +11969,10 @@
         <v>2025</v>
       </c>
       <c r="B18" s="1">
-        <v>45660</v>
+        <v>45674</v>
       </c>
       <c r="C18" s="6">
-        <v>8.3500000000000005E-2</v>
+        <v>8.3599999999999994E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -11380,10 +11980,10 @@
         <v>2025</v>
       </c>
       <c r="B19" s="1">
-        <v>45691</v>
+        <v>45675</v>
       </c>
       <c r="C19" s="6">
-        <v>8.3799999999999999E-2</v>
+        <v>8.3599999999999994E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -11391,10 +11991,10 @@
         <v>2025</v>
       </c>
       <c r="B20" s="1">
-        <v>45719</v>
+        <v>45676</v>
       </c>
       <c r="C20" s="6">
-        <v>8.4000000000000005E-2</v>
+        <v>8.3699999999999997E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -11402,10 +12002,10 @@
         <v>2025</v>
       </c>
       <c r="B21" s="1">
-        <v>45750</v>
+        <v>45677</v>
       </c>
       <c r="C21" s="6">
-        <v>8.4199999999999997E-2</v>
+        <v>8.3699999999999997E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -11413,10 +12013,10 @@
         <v>2025</v>
       </c>
       <c r="B22" s="1">
-        <v>45780</v>
+        <v>45678</v>
       </c>
       <c r="C22" s="6">
-        <v>8.4500000000000006E-2</v>
+        <v>8.3699999999999997E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -11424,10 +12024,10 @@
         <v>2025</v>
       </c>
       <c r="B23" s="1">
-        <v>45811</v>
+        <v>45679</v>
       </c>
       <c r="C23" s="6">
-        <v>8.48E-2</v>
+        <v>8.3699999999999997E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -11435,10 +12035,10 @@
         <v>2025</v>
       </c>
       <c r="B24" s="1">
-        <v>45841</v>
+        <v>45680</v>
       </c>
       <c r="C24" s="6">
-        <v>8.5000000000000006E-2</v>
+        <v>8.3699999999999997E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -11446,10 +12046,10 @@
         <v>2025</v>
       </c>
       <c r="B25" s="1">
-        <v>45872</v>
+        <v>45681</v>
       </c>
       <c r="C25" s="6">
-        <v>8.5300000000000001E-2</v>
+        <v>8.3699999999999997E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -11457,10 +12057,10 @@
         <v>2025</v>
       </c>
       <c r="B26" s="1">
-        <v>45661</v>
+        <v>45682</v>
       </c>
       <c r="C26" s="6">
-        <v>8.3500000000000005E-2</v>
+        <v>8.3699999999999997E-2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -11468,10 +12068,10 @@
         <v>2025</v>
       </c>
       <c r="B27" s="1">
-        <v>45692</v>
+        <v>45683</v>
       </c>
       <c r="C27" s="6">
-        <v>8.3799999999999999E-2</v>
+        <v>8.3699999999999997E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -11479,10 +12079,10 @@
         <v>2025</v>
       </c>
       <c r="B28" s="1">
-        <v>45720</v>
+        <v>45684</v>
       </c>
       <c r="C28" s="6">
-        <v>8.4000000000000005E-2</v>
+        <v>8.3699999999999997E-2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -11490,10 +12090,10 @@
         <v>2025</v>
       </c>
       <c r="B29" s="1">
-        <v>45751</v>
+        <v>45685</v>
       </c>
       <c r="C29" s="6">
-        <v>8.4199999999999997E-2</v>
+        <v>8.3699999999999997E-2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -11501,10 +12101,10 @@
         <v>2025</v>
       </c>
       <c r="B30" s="1">
-        <v>45781</v>
+        <v>45686</v>
       </c>
       <c r="C30" s="6">
-        <v>8.4500000000000006E-2</v>
+        <v>8.3699999999999997E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -11512,10 +12112,10 @@
         <v>2025</v>
       </c>
       <c r="B31" s="1">
-        <v>45812</v>
+        <v>45687</v>
       </c>
       <c r="C31" s="6">
-        <v>8.48E-2</v>
+        <v>8.3699999999999997E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -11523,10 +12123,10 @@
         <v>2025</v>
       </c>
       <c r="B32" s="1">
-        <v>45842</v>
+        <v>45688</v>
       </c>
       <c r="C32" s="6">
-        <v>8.5000000000000006E-2</v>
+        <v>8.3699999999999997E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -11534,10 +12134,10 @@
         <v>2025</v>
       </c>
       <c r="B33" s="1">
-        <v>45873</v>
+        <v>45689</v>
       </c>
       <c r="C33" s="6">
-        <v>8.5300000000000001E-2</v>
+        <v>8.3699999999999997E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -11545,10 +12145,10 @@
         <v>2025</v>
       </c>
       <c r="B34" s="1">
-        <v>45662</v>
+        <v>45690</v>
       </c>
       <c r="C34" s="6">
-        <v>8.3500000000000005E-2</v>
+        <v>8.3699999999999997E-2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -11556,7 +12156,7 @@
         <v>2025</v>
       </c>
       <c r="B35" s="1">
-        <v>45693</v>
+        <v>45691</v>
       </c>
       <c r="C35" s="6">
         <v>8.3799999999999999E-2</v>
@@ -11567,10 +12167,10 @@
         <v>2025</v>
       </c>
       <c r="B36" s="1">
-        <v>45721</v>
+        <v>45692</v>
       </c>
       <c r="C36" s="6">
-        <v>8.4000000000000005E-2</v>
+        <v>8.3799999999999999E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -11578,10 +12178,10 @@
         <v>2025</v>
       </c>
       <c r="B37" s="1">
-        <v>45752</v>
+        <v>45693</v>
       </c>
       <c r="C37" s="6">
-        <v>8.43E-2</v>
+        <v>8.3799999999999999E-2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -11589,10 +12189,10 @@
         <v>2025</v>
       </c>
       <c r="B38" s="1">
-        <v>45782</v>
+        <v>45694</v>
       </c>
       <c r="C38" s="6">
-        <v>8.4500000000000006E-2</v>
+        <v>8.3799999999999999E-2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -11600,10 +12200,10 @@
         <v>2025</v>
       </c>
       <c r="B39" s="1">
-        <v>45813</v>
+        <v>45695</v>
       </c>
       <c r="C39" s="6">
-        <v>8.48E-2</v>
+        <v>8.3799999999999999E-2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -11611,10 +12211,10 @@
         <v>2025</v>
       </c>
       <c r="B40" s="1">
-        <v>45843</v>
+        <v>45696</v>
       </c>
       <c r="C40" s="6">
-        <v>8.5000000000000006E-2</v>
+        <v>8.3799999999999999E-2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -11622,10 +12222,10 @@
         <v>2025</v>
       </c>
       <c r="B41" s="1">
-        <v>45874</v>
+        <v>45697</v>
       </c>
       <c r="C41" s="6">
-        <v>8.5300000000000001E-2</v>
+        <v>8.3799999999999999E-2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -11633,10 +12233,10 @@
         <v>2025</v>
       </c>
       <c r="B42" s="1">
-        <v>45663</v>
+        <v>45698</v>
       </c>
       <c r="C42" s="6">
-        <v>8.3500000000000005E-2</v>
+        <v>8.3799999999999999E-2</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -11644,7 +12244,7 @@
         <v>2025</v>
       </c>
       <c r="B43" s="1">
-        <v>45694</v>
+        <v>45699</v>
       </c>
       <c r="C43" s="6">
         <v>8.3799999999999999E-2</v>
@@ -11655,10 +12255,10 @@
         <v>2025</v>
       </c>
       <c r="B44" s="1">
-        <v>45722</v>
+        <v>45700</v>
       </c>
       <c r="C44" s="6">
-        <v>8.4000000000000005E-2</v>
+        <v>8.3799999999999999E-2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -11666,10 +12266,10 @@
         <v>2025</v>
       </c>
       <c r="B45" s="1">
-        <v>45753</v>
+        <v>45701</v>
       </c>
       <c r="C45" s="6">
-        <v>8.43E-2</v>
+        <v>8.3900000000000002E-2</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -11677,10 +12277,10 @@
         <v>2025</v>
       </c>
       <c r="B46" s="1">
-        <v>45783</v>
+        <v>45702</v>
       </c>
       <c r="C46" s="6">
-        <v>8.4500000000000006E-2</v>
+        <v>8.3900000000000002E-2</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -11688,10 +12288,10 @@
         <v>2025</v>
       </c>
       <c r="B47" s="1">
-        <v>45814</v>
+        <v>45703</v>
       </c>
       <c r="C47" s="6">
-        <v>8.48E-2</v>
+        <v>8.3900000000000002E-2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -11699,10 +12299,10 @@
         <v>2025</v>
       </c>
       <c r="B48" s="1">
-        <v>45844</v>
+        <v>45704</v>
       </c>
       <c r="C48" s="6">
-        <v>8.5000000000000006E-2</v>
+        <v>8.3900000000000002E-2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -11710,10 +12310,10 @@
         <v>2025</v>
       </c>
       <c r="B49" s="1">
-        <v>45875</v>
+        <v>45705</v>
       </c>
       <c r="C49" s="6">
-        <v>8.5300000000000001E-2</v>
+        <v>8.3900000000000002E-2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -11721,10 +12321,10 @@
         <v>2025</v>
       </c>
       <c r="B50" s="1">
-        <v>45664</v>
+        <v>45706</v>
       </c>
       <c r="C50" s="6">
-        <v>8.3599999999999994E-2</v>
+        <v>8.3900000000000002E-2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -11732,10 +12332,10 @@
         <v>2025</v>
       </c>
       <c r="B51" s="1">
-        <v>45695</v>
+        <v>45707</v>
       </c>
       <c r="C51" s="6">
-        <v>8.3799999999999999E-2</v>
+        <v>8.3900000000000002E-2</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -11743,10 +12343,10 @@
         <v>2025</v>
       </c>
       <c r="B52" s="1">
-        <v>45723</v>
+        <v>45708</v>
       </c>
       <c r="C52" s="6">
-        <v>8.4000000000000005E-2</v>
+        <v>8.3900000000000002E-2</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -11754,10 +12354,10 @@
         <v>2025</v>
       </c>
       <c r="B53" s="1">
-        <v>45754</v>
+        <v>45709</v>
       </c>
       <c r="C53" s="6">
-        <v>8.43E-2</v>
+        <v>8.3900000000000002E-2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -11765,10 +12365,10 @@
         <v>2025</v>
       </c>
       <c r="B54" s="1">
-        <v>45784</v>
+        <v>45710</v>
       </c>
       <c r="C54" s="6">
-        <v>8.4599999999999995E-2</v>
+        <v>8.3900000000000002E-2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -11776,10 +12376,10 @@
         <v>2025</v>
       </c>
       <c r="B55" s="1">
-        <v>45815</v>
+        <v>45711</v>
       </c>
       <c r="C55" s="6">
-        <v>8.48E-2</v>
+        <v>8.3900000000000002E-2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -11787,10 +12387,10 @@
         <v>2025</v>
       </c>
       <c r="B56" s="1">
-        <v>45845</v>
+        <v>45712</v>
       </c>
       <c r="C56" s="6">
-        <v>8.5000000000000006E-2</v>
+        <v>8.3900000000000002E-2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -11798,10 +12398,10 @@
         <v>2025</v>
       </c>
       <c r="B57" s="1">
-        <v>45876</v>
+        <v>45713</v>
       </c>
       <c r="C57" s="6">
-        <v>8.5300000000000001E-2</v>
+        <v>8.3900000000000002E-2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -11809,10 +12409,10 @@
         <v>2025</v>
       </c>
       <c r="B58" s="1">
-        <v>45665</v>
+        <v>45714</v>
       </c>
       <c r="C58" s="6">
-        <v>8.3599999999999994E-2</v>
+        <v>8.3900000000000002E-2</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -11820,10 +12420,10 @@
         <v>2025</v>
       </c>
       <c r="B59" s="1">
-        <v>45696</v>
+        <v>45715</v>
       </c>
       <c r="C59" s="6">
-        <v>8.3799999999999999E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -11831,7 +12431,7 @@
         <v>2025</v>
       </c>
       <c r="B60" s="1">
-        <v>45724</v>
+        <v>45716</v>
       </c>
       <c r="C60" s="6">
         <v>8.4000000000000005E-2</v>
@@ -11842,10 +12442,10 @@
         <v>2025</v>
       </c>
       <c r="B61" s="1">
-        <v>45755</v>
+        <v>45717</v>
       </c>
       <c r="C61" s="6">
-        <v>8.43E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -11853,10 +12453,10 @@
         <v>2025</v>
       </c>
       <c r="B62" s="1">
-        <v>45785</v>
+        <v>45718</v>
       </c>
       <c r="C62" s="6">
-        <v>8.4599999999999995E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -11864,10 +12464,10 @@
         <v>2025</v>
       </c>
       <c r="B63" s="1">
-        <v>45816</v>
+        <v>45719</v>
       </c>
       <c r="C63" s="6">
-        <v>8.48E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -11875,10 +12475,10 @@
         <v>2025</v>
       </c>
       <c r="B64" s="1">
-        <v>45846</v>
+        <v>45720</v>
       </c>
       <c r="C64" s="6">
-        <v>8.5099999999999995E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -11886,10 +12486,10 @@
         <v>2025</v>
       </c>
       <c r="B65" s="1">
-        <v>45877</v>
+        <v>45721</v>
       </c>
       <c r="C65" s="6">
-        <v>8.5300000000000001E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -11897,10 +12497,10 @@
         <v>2025</v>
       </c>
       <c r="B66" s="1">
-        <v>45666</v>
+        <v>45722</v>
       </c>
       <c r="C66" s="6">
-        <v>8.3599999999999994E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -11908,10 +12508,10 @@
         <v>2025</v>
       </c>
       <c r="B67" s="1">
-        <v>45697</v>
+        <v>45723</v>
       </c>
       <c r="C67" s="6">
-        <v>8.3799999999999999E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -11919,10 +12519,10 @@
         <v>2025</v>
       </c>
       <c r="B68" s="1">
-        <v>45725</v>
+        <v>45724</v>
       </c>
       <c r="C68" s="6">
-        <v>8.4099999999999994E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -11930,10 +12530,10 @@
         <v>2025</v>
       </c>
       <c r="B69" s="1">
-        <v>45756</v>
+        <v>45725</v>
       </c>
       <c r="C69" s="6">
-        <v>8.43E-2</v>
+        <v>8.4099999999999994E-2</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -11941,10 +12541,10 @@
         <v>2025</v>
       </c>
       <c r="B70" s="1">
-        <v>45786</v>
+        <v>45726</v>
       </c>
       <c r="C70" s="6">
-        <v>8.4599999999999995E-2</v>
+        <v>8.4099999999999994E-2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -11952,10 +12552,10 @@
         <v>2025</v>
       </c>
       <c r="B71" s="1">
-        <v>45817</v>
+        <v>45727</v>
       </c>
       <c r="C71" s="6">
-        <v>8.48E-2</v>
+        <v>8.4099999999999994E-2</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -11963,10 +12563,10 @@
         <v>2025</v>
       </c>
       <c r="B72" s="1">
-        <v>45847</v>
+        <v>45728</v>
       </c>
       <c r="C72" s="6">
-        <v>8.5099999999999995E-2</v>
+        <v>8.4099999999999994E-2</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -11974,10 +12574,10 @@
         <v>2025</v>
       </c>
       <c r="B73" s="1">
-        <v>45878</v>
+        <v>45729</v>
       </c>
       <c r="C73" s="6">
-        <v>8.5300000000000001E-2</v>
+        <v>8.4099999999999994E-2</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
@@ -11985,10 +12585,10 @@
         <v>2025</v>
       </c>
       <c r="B74" s="1">
-        <v>45667</v>
+        <v>45730</v>
       </c>
       <c r="C74" s="6">
-        <v>8.3599999999999994E-2</v>
+        <v>8.4099999999999994E-2</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -11996,10 +12596,10 @@
         <v>2025</v>
       </c>
       <c r="B75" s="1">
-        <v>45698</v>
+        <v>45731</v>
       </c>
       <c r="C75" s="6">
-        <v>8.3799999999999999E-2</v>
+        <v>8.4099999999999994E-2</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -12007,7 +12607,7 @@
         <v>2025</v>
       </c>
       <c r="B76" s="1">
-        <v>45726</v>
+        <v>45732</v>
       </c>
       <c r="C76" s="6">
         <v>8.4099999999999994E-2</v>
@@ -12018,10 +12618,10 @@
         <v>2025</v>
       </c>
       <c r="B77" s="1">
-        <v>45757</v>
+        <v>45733</v>
       </c>
       <c r="C77" s="6">
-        <v>8.43E-2</v>
+        <v>8.4099999999999994E-2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
@@ -12029,10 +12629,10 @@
         <v>2025</v>
       </c>
       <c r="B78" s="1">
-        <v>45787</v>
+        <v>45734</v>
       </c>
       <c r="C78" s="6">
-        <v>8.4599999999999995E-2</v>
+        <v>8.4099999999999994E-2</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
@@ -12040,10 +12640,10 @@
         <v>2025</v>
       </c>
       <c r="B79" s="1">
-        <v>45818</v>
+        <v>45735</v>
       </c>
       <c r="C79" s="6">
-        <v>8.48E-2</v>
+        <v>8.4099999999999994E-2</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
@@ -12051,10 +12651,10 @@
         <v>2025</v>
       </c>
       <c r="B80" s="1">
-        <v>45848</v>
+        <v>45736</v>
       </c>
       <c r="C80" s="6">
-        <v>8.5099999999999995E-2</v>
+        <v>8.4099999999999994E-2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -12062,10 +12662,10 @@
         <v>2025</v>
       </c>
       <c r="B81" s="1">
-        <v>45879</v>
+        <v>45737</v>
       </c>
       <c r="C81" s="6">
-        <v>8.5300000000000001E-2</v>
+        <v>8.4099999999999994E-2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -12073,10 +12673,10 @@
         <v>2025</v>
       </c>
       <c r="B82" s="1">
-        <v>45668</v>
+        <v>45738</v>
       </c>
       <c r="C82" s="6">
-        <v>8.3599999999999994E-2</v>
+        <v>8.4199999999999997E-2</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
@@ -12084,10 +12684,10 @@
         <v>2025</v>
       </c>
       <c r="B83" s="1">
-        <v>45699</v>
+        <v>45739</v>
       </c>
       <c r="C83" s="6">
-        <v>8.3799999999999999E-2</v>
+        <v>8.4199999999999997E-2</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
@@ -12095,10 +12695,10 @@
         <v>2025</v>
       </c>
       <c r="B84" s="1">
-        <v>45727</v>
+        <v>45740</v>
       </c>
       <c r="C84" s="6">
-        <v>8.4099999999999994E-2</v>
+        <v>8.4199999999999997E-2</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
@@ -12106,10 +12706,10 @@
         <v>2025</v>
       </c>
       <c r="B85" s="1">
-        <v>45758</v>
+        <v>45741</v>
       </c>
       <c r="C85" s="6">
-        <v>8.43E-2</v>
+        <v>8.4199999999999997E-2</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
@@ -12117,10 +12717,10 @@
         <v>2025</v>
       </c>
       <c r="B86" s="1">
-        <v>45788</v>
+        <v>45742</v>
       </c>
       <c r="C86" s="6">
-        <v>8.4599999999999995E-2</v>
+        <v>8.4199999999999997E-2</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
@@ -12128,10 +12728,10 @@
         <v>2025</v>
       </c>
       <c r="B87" s="1">
-        <v>45819</v>
+        <v>45743</v>
       </c>
       <c r="C87" s="6">
-        <v>8.48E-2</v>
+        <v>8.4199999999999997E-2</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
@@ -12139,10 +12739,10 @@
         <v>2025</v>
       </c>
       <c r="B88" s="1">
-        <v>45849</v>
+        <v>45744</v>
       </c>
       <c r="C88" s="6">
-        <v>8.5099999999999995E-2</v>
+        <v>8.4199999999999997E-2</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
@@ -12150,10 +12750,10 @@
         <v>2025</v>
       </c>
       <c r="B89" s="1">
-        <v>45880</v>
+        <v>45745</v>
       </c>
       <c r="C89" s="6">
-        <v>8.5300000000000001E-2</v>
+        <v>8.4199999999999997E-2</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
@@ -12161,10 +12761,10 @@
         <v>2025</v>
       </c>
       <c r="B90" s="1">
-        <v>45669</v>
+        <v>45746</v>
       </c>
       <c r="C90" s="6">
-        <v>8.3599999999999994E-2</v>
+        <v>8.4199999999999997E-2</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -12172,10 +12772,10 @@
         <v>2025</v>
       </c>
       <c r="B91" s="1">
-        <v>45700</v>
+        <v>45747</v>
       </c>
       <c r="C91" s="6">
-        <v>8.3799999999999999E-2</v>
+        <v>8.4199999999999997E-2</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
@@ -12183,10 +12783,10 @@
         <v>2025</v>
       </c>
       <c r="B92" s="1">
-        <v>45728</v>
+        <v>45748</v>
       </c>
       <c r="C92" s="6">
-        <v>8.4099999999999994E-2</v>
+        <v>8.4199999999999997E-2</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
@@ -12194,10 +12794,10 @@
         <v>2025</v>
       </c>
       <c r="B93" s="1">
-        <v>45759</v>
+        <v>45749</v>
       </c>
       <c r="C93" s="6">
-        <v>8.43E-2</v>
+        <v>8.4199999999999997E-2</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
@@ -12205,10 +12805,10 @@
         <v>2025</v>
       </c>
       <c r="B94" s="1">
-        <v>45789</v>
+        <v>45750</v>
       </c>
       <c r="C94" s="6">
-        <v>8.4599999999999995E-2</v>
+        <v>8.4199999999999997E-2</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
@@ -12216,10 +12816,10 @@
         <v>2025</v>
       </c>
       <c r="B95" s="1">
-        <v>45820</v>
+        <v>45751</v>
       </c>
       <c r="C95" s="6">
-        <v>8.48E-2</v>
+        <v>8.4199999999999997E-2</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
@@ -12227,10 +12827,10 @@
         <v>2025</v>
       </c>
       <c r="B96" s="1">
-        <v>45850</v>
+        <v>45752</v>
       </c>
       <c r="C96" s="6">
-        <v>8.5099999999999995E-2</v>
+        <v>8.43E-2</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -12238,10 +12838,10 @@
         <v>2025</v>
       </c>
       <c r="B97" s="1">
-        <v>45881</v>
+        <v>45753</v>
       </c>
       <c r="C97" s="6">
-        <v>8.5300000000000001E-2</v>
+        <v>8.43E-2</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
@@ -12249,10 +12849,10 @@
         <v>2025</v>
       </c>
       <c r="B98" s="1">
-        <v>45670</v>
+        <v>45754</v>
       </c>
       <c r="C98" s="6">
-        <v>8.3599999999999994E-2</v>
+        <v>8.43E-2</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
@@ -12260,10 +12860,10 @@
         <v>2025</v>
       </c>
       <c r="B99" s="1">
-        <v>45701</v>
+        <v>45755</v>
       </c>
       <c r="C99" s="6">
-        <v>8.3900000000000002E-2</v>
+        <v>8.43E-2</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
@@ -12271,10 +12871,10 @@
         <v>2025</v>
       </c>
       <c r="B100" s="1">
-        <v>45729</v>
+        <v>45756</v>
       </c>
       <c r="C100" s="6">
-        <v>8.4099999999999994E-2</v>
+        <v>8.43E-2</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -12282,7 +12882,7 @@
         <v>2025</v>
       </c>
       <c r="B101" s="1">
-        <v>45760</v>
+        <v>45757</v>
       </c>
       <c r="C101" s="6">
         <v>8.43E-2</v>
@@ -12293,10 +12893,10 @@
         <v>2025</v>
       </c>
       <c r="B102" s="1">
-        <v>45790</v>
+        <v>45758</v>
       </c>
       <c r="C102" s="6">
-        <v>8.4599999999999995E-2</v>
+        <v>8.43E-2</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
@@ -12304,10 +12904,10 @@
         <v>2025</v>
       </c>
       <c r="B103" s="1">
-        <v>45821</v>
+        <v>45759</v>
       </c>
       <c r="C103" s="6">
-        <v>8.48E-2</v>
+        <v>8.43E-2</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
@@ -12315,10 +12915,10 @@
         <v>2025</v>
       </c>
       <c r="B104" s="1">
-        <v>45851</v>
+        <v>45760</v>
       </c>
       <c r="C104" s="6">
-        <v>8.5099999999999995E-2</v>
+        <v>8.43E-2</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
@@ -12326,10 +12926,10 @@
         <v>2025</v>
       </c>
       <c r="B105" s="1">
-        <v>45882</v>
+        <v>45761</v>
       </c>
       <c r="C105" s="6">
-        <v>8.5300000000000001E-2</v>
+        <v>8.43E-2</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
@@ -12337,10 +12937,10 @@
         <v>2025</v>
       </c>
       <c r="B106" s="1">
-        <v>45671</v>
+        <v>45762</v>
       </c>
       <c r="C106" s="6">
-        <v>8.3599999999999994E-2</v>
+        <v>8.4400000000000003E-2</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
@@ -12348,10 +12948,10 @@
         <v>2025</v>
       </c>
       <c r="B107" s="1">
-        <v>45702</v>
+        <v>45763</v>
       </c>
       <c r="C107" s="6">
-        <v>8.3900000000000002E-2</v>
+        <v>8.4400000000000003E-2</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
@@ -12359,10 +12959,10 @@
         <v>2025</v>
       </c>
       <c r="B108" s="1">
-        <v>45730</v>
+        <v>45764</v>
       </c>
       <c r="C108" s="6">
-        <v>8.4099999999999994E-2</v>
+        <v>8.4400000000000003E-2</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
@@ -12370,10 +12970,10 @@
         <v>2025</v>
       </c>
       <c r="B109" s="1">
-        <v>45761</v>
+        <v>45765</v>
       </c>
       <c r="C109" s="6">
-        <v>8.43E-2</v>
+        <v>8.4400000000000003E-2</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
@@ -12381,10 +12981,10 @@
         <v>2025</v>
       </c>
       <c r="B110" s="1">
-        <v>45791</v>
+        <v>45766</v>
       </c>
       <c r="C110" s="6">
-        <v>8.4599999999999995E-2</v>
+        <v>8.4400000000000003E-2</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
@@ -12392,10 +12992,10 @@
         <v>2025</v>
       </c>
       <c r="B111" s="1">
-        <v>45822</v>
+        <v>45767</v>
       </c>
       <c r="C111" s="6">
-        <v>8.4900000000000003E-2</v>
+        <v>8.4400000000000003E-2</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
@@ -12403,10 +13003,10 @@
         <v>2025</v>
       </c>
       <c r="B112" s="1">
-        <v>45852</v>
+        <v>45768</v>
       </c>
       <c r="C112" s="6">
-        <v>8.5099999999999995E-2</v>
+        <v>8.4400000000000003E-2</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
@@ -12414,10 +13014,10 @@
         <v>2025</v>
       </c>
       <c r="B113" s="1">
-        <v>45883</v>
+        <v>45769</v>
       </c>
       <c r="C113" s="6">
-        <v>8.5300000000000001E-2</v>
+        <v>8.4400000000000003E-2</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
@@ -12425,10 +13025,10 @@
         <v>2025</v>
       </c>
       <c r="B114" s="1">
-        <v>45672</v>
+        <v>45770</v>
       </c>
       <c r="C114" s="6">
-        <v>8.3599999999999994E-2</v>
+        <v>8.4400000000000003E-2</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
@@ -12436,10 +13036,10 @@
         <v>2025</v>
       </c>
       <c r="B115" s="1">
-        <v>45703</v>
+        <v>45771</v>
       </c>
       <c r="C115" s="6">
-        <v>8.3900000000000002E-2</v>
+        <v>8.4500000000000006E-2</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
@@ -12447,10 +13047,10 @@
         <v>2025</v>
       </c>
       <c r="B116" s="1">
-        <v>45731</v>
+        <v>45772</v>
       </c>
       <c r="C116" s="6">
-        <v>8.4099999999999994E-2</v>
+        <v>8.4500000000000006E-2</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
@@ -12458,10 +13058,10 @@
         <v>2025</v>
       </c>
       <c r="B117" s="1">
-        <v>45762</v>
+        <v>45773</v>
       </c>
       <c r="C117" s="6">
-        <v>8.4400000000000003E-2</v>
+        <v>8.4500000000000006E-2</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
@@ -12469,10 +13069,10 @@
         <v>2025</v>
       </c>
       <c r="B118" s="1">
-        <v>45792</v>
+        <v>45774</v>
       </c>
       <c r="C118" s="6">
-        <v>8.4599999999999995E-2</v>
+        <v>8.4500000000000006E-2</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
@@ -12480,10 +13080,10 @@
         <v>2025</v>
       </c>
       <c r="B119" s="1">
-        <v>45823</v>
+        <v>45775</v>
       </c>
       <c r="C119" s="6">
-        <v>8.4900000000000003E-2</v>
+        <v>8.4500000000000006E-2</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
@@ -12491,10 +13091,10 @@
         <v>2025</v>
       </c>
       <c r="B120" s="1">
-        <v>45853</v>
+        <v>45776</v>
       </c>
       <c r="C120" s="6">
-        <v>8.5099999999999995E-2</v>
+        <v>8.4500000000000006E-2</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
@@ -12502,10 +13102,10 @@
         <v>2025</v>
       </c>
       <c r="B121" s="1">
-        <v>45884</v>
+        <v>45777</v>
       </c>
       <c r="C121" s="6">
-        <v>8.5400000000000004E-2</v>
+        <v>8.4500000000000006E-2</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
@@ -12513,10 +13113,10 @@
         <v>2025</v>
       </c>
       <c r="B122" s="1">
-        <v>45673</v>
+        <v>45778</v>
       </c>
       <c r="C122" s="6">
-        <v>8.3599999999999994E-2</v>
+        <v>8.4500000000000006E-2</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
@@ -12524,10 +13124,10 @@
         <v>2025</v>
       </c>
       <c r="B123" s="1">
-        <v>45704</v>
+        <v>45779</v>
       </c>
       <c r="C123" s="6">
-        <v>8.3900000000000002E-2</v>
+        <v>8.4500000000000006E-2</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
@@ -12535,10 +13135,10 @@
         <v>2025</v>
       </c>
       <c r="B124" s="1">
-        <v>45732</v>
+        <v>45780</v>
       </c>
       <c r="C124" s="6">
-        <v>8.4099999999999994E-2</v>
+        <v>8.4500000000000006E-2</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -12546,10 +13146,10 @@
         <v>2025</v>
       </c>
       <c r="B125" s="1">
-        <v>45763</v>
+        <v>45781</v>
       </c>
       <c r="C125" s="6">
-        <v>8.4400000000000003E-2</v>
+        <v>8.4500000000000006E-2</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
@@ -12557,10 +13157,10 @@
         <v>2025</v>
       </c>
       <c r="B126" s="1">
-        <v>45793</v>
+        <v>45782</v>
       </c>
       <c r="C126" s="6">
-        <v>8.4599999999999995E-2</v>
+        <v>8.4500000000000006E-2</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
@@ -12568,10 +13168,10 @@
         <v>2025</v>
       </c>
       <c r="B127" s="1">
-        <v>45824</v>
+        <v>45783</v>
       </c>
       <c r="C127" s="6">
-        <v>8.4900000000000003E-2</v>
+        <v>8.4500000000000006E-2</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
@@ -12579,10 +13179,10 @@
         <v>2025</v>
       </c>
       <c r="B128" s="1">
-        <v>45854</v>
+        <v>45784</v>
       </c>
       <c r="C128" s="6">
-        <v>8.5099999999999995E-2</v>
+        <v>8.4599999999999995E-2</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
@@ -12590,10 +13190,10 @@
         <v>2025</v>
       </c>
       <c r="B129" s="1">
-        <v>45885</v>
+        <v>45785</v>
       </c>
       <c r="C129" s="6">
-        <v>8.5400000000000004E-2</v>
+        <v>8.4599999999999995E-2</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
@@ -12601,10 +13201,10 @@
         <v>2025</v>
       </c>
       <c r="B130" s="1">
-        <v>45674</v>
+        <v>45786</v>
       </c>
       <c r="C130" s="6">
-        <v>8.3599999999999994E-2</v>
+        <v>8.4599999999999995E-2</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
@@ -12612,10 +13212,10 @@
         <v>2025</v>
       </c>
       <c r="B131" s="1">
-        <v>45705</v>
+        <v>45787</v>
       </c>
       <c r="C131" s="6">
-        <v>8.3900000000000002E-2</v>
+        <v>8.4599999999999995E-2</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
@@ -12623,10 +13223,10 @@
         <v>2025</v>
       </c>
       <c r="B132" s="1">
-        <v>45733</v>
+        <v>45788</v>
       </c>
       <c r="C132" s="6">
-        <v>8.4099999999999994E-2</v>
+        <v>8.4599999999999995E-2</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
@@ -12634,10 +13234,10 @@
         <v>2025</v>
       </c>
       <c r="B133" s="1">
-        <v>45764</v>
+        <v>45789</v>
       </c>
       <c r="C133" s="6">
-        <v>8.4400000000000003E-2</v>
+        <v>8.4599999999999995E-2</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
@@ -12645,10 +13245,10 @@
         <v>2025</v>
       </c>
       <c r="B134" s="1">
-        <v>45794</v>
+        <v>45790</v>
       </c>
       <c r="C134" s="6">
-        <v>8.4699999999999998E-2</v>
+        <v>8.4599999999999995E-2</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
@@ -12656,10 +13256,10 @@
         <v>2025</v>
       </c>
       <c r="B135" s="1">
-        <v>45825</v>
+        <v>45791</v>
       </c>
       <c r="C135" s="6">
-        <v>8.4900000000000003E-2</v>
+        <v>8.4599999999999995E-2</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
@@ -12667,10 +13267,10 @@
         <v>2025</v>
       </c>
       <c r="B136" s="1">
-        <v>45855</v>
+        <v>45792</v>
       </c>
       <c r="C136" s="6">
-        <v>8.5099999999999995E-2</v>
+        <v>8.4599999999999995E-2</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
@@ -12678,10 +13278,10 @@
         <v>2025</v>
       </c>
       <c r="B137" s="1">
-        <v>45886</v>
+        <v>45793</v>
       </c>
       <c r="C137" s="6">
-        <v>8.5400000000000004E-2</v>
+        <v>8.4599999999999995E-2</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
@@ -12689,10 +13289,10 @@
         <v>2025</v>
       </c>
       <c r="B138" s="1">
-        <v>45675</v>
+        <v>45794</v>
       </c>
       <c r="C138" s="6">
-        <v>8.3599999999999994E-2</v>
+        <v>8.4699999999999998E-2</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
@@ -12700,10 +13300,10 @@
         <v>2025</v>
       </c>
       <c r="B139" s="1">
-        <v>45706</v>
+        <v>45795</v>
       </c>
       <c r="C139" s="6">
-        <v>8.3900000000000002E-2</v>
+        <v>8.4699999999999998E-2</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
@@ -12711,10 +13311,10 @@
         <v>2025</v>
       </c>
       <c r="B140" s="1">
-        <v>45734</v>
+        <v>45796</v>
       </c>
       <c r="C140" s="6">
-        <v>8.4099999999999994E-2</v>
+        <v>8.4699999999999998E-2</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
@@ -12722,10 +13322,10 @@
         <v>2025</v>
       </c>
       <c r="B141" s="1">
-        <v>45765</v>
+        <v>45797</v>
       </c>
       <c r="C141" s="6">
-        <v>8.4400000000000003E-2</v>
+        <v>8.4699999999999998E-2</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
@@ -12733,7 +13333,7 @@
         <v>2025</v>
       </c>
       <c r="B142" s="1">
-        <v>45795</v>
+        <v>45798</v>
       </c>
       <c r="C142" s="6">
         <v>8.4699999999999998E-2</v>
@@ -12744,10 +13344,10 @@
         <v>2025</v>
       </c>
       <c r="B143" s="1">
-        <v>45826</v>
+        <v>45799</v>
       </c>
       <c r="C143" s="6">
-        <v>8.4900000000000003E-2</v>
+        <v>8.4699999999999998E-2</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
@@ -12755,10 +13355,10 @@
         <v>2025</v>
       </c>
       <c r="B144" s="1">
-        <v>45856</v>
+        <v>45800</v>
       </c>
       <c r="C144" s="6">
-        <v>8.5099999999999995E-2</v>
+        <v>8.4699999999999998E-2</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
@@ -12766,10 +13366,10 @@
         <v>2025</v>
       </c>
       <c r="B145" s="1">
-        <v>45887</v>
+        <v>45801</v>
       </c>
       <c r="C145" s="6">
-        <v>8.5400000000000004E-2</v>
+        <v>8.4699999999999998E-2</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
@@ -12777,10 +13377,10 @@
         <v>2025</v>
       </c>
       <c r="B146" s="1">
-        <v>45676</v>
+        <v>45802</v>
       </c>
       <c r="C146" s="6">
-        <v>8.3699999999999997E-2</v>
+        <v>8.4699999999999998E-2</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
@@ -12788,10 +13388,10 @@
         <v>2025</v>
       </c>
       <c r="B147" s="1">
-        <v>45707</v>
+        <v>45803</v>
       </c>
       <c r="C147" s="6">
-        <v>8.3900000000000002E-2</v>
+        <v>8.4699999999999998E-2</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
@@ -12799,10 +13399,10 @@
         <v>2025</v>
       </c>
       <c r="B148" s="1">
-        <v>45735</v>
+        <v>45804</v>
       </c>
       <c r="C148" s="6">
-        <v>8.4099999999999994E-2</v>
+        <v>8.48E-2</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
@@ -12810,10 +13410,10 @@
         <v>2025</v>
       </c>
       <c r="B149" s="1">
-        <v>45766</v>
+        <v>45805</v>
       </c>
       <c r="C149" s="6">
-        <v>8.4400000000000003E-2</v>
+        <v>8.48E-2</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
@@ -12821,10 +13421,10 @@
         <v>2025</v>
       </c>
       <c r="B150" s="1">
-        <v>45796</v>
+        <v>45806</v>
       </c>
       <c r="C150" s="6">
-        <v>8.4699999999999998E-2</v>
+        <v>8.48E-2</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
@@ -12832,10 +13432,10 @@
         <v>2025</v>
       </c>
       <c r="B151" s="1">
-        <v>45827</v>
+        <v>45807</v>
       </c>
       <c r="C151" s="6">
-        <v>8.4900000000000003E-2</v>
+        <v>8.48E-2</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
@@ -12843,10 +13443,10 @@
         <v>2025</v>
       </c>
       <c r="B152" s="1">
-        <v>45857</v>
+        <v>45808</v>
       </c>
       <c r="C152" s="6">
-        <v>8.5199999999999998E-2</v>
+        <v>8.48E-2</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
@@ -12854,10 +13454,10 @@
         <v>2025</v>
       </c>
       <c r="B153" s="1">
-        <v>45888</v>
+        <v>45809</v>
       </c>
       <c r="C153" s="6">
-        <v>8.5400000000000004E-2</v>
+        <v>8.48E-2</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
@@ -12865,10 +13465,10 @@
         <v>2025</v>
       </c>
       <c r="B154" s="1">
-        <v>45677</v>
+        <v>45810</v>
       </c>
       <c r="C154" s="6">
-        <v>8.3699999999999997E-2</v>
+        <v>8.48E-2</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
@@ -12876,10 +13476,10 @@
         <v>2025</v>
       </c>
       <c r="B155" s="1">
-        <v>45708</v>
+        <v>45811</v>
       </c>
       <c r="C155" s="6">
-        <v>8.3900000000000002E-2</v>
+        <v>8.48E-2</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
@@ -12887,10 +13487,10 @@
         <v>2025</v>
       </c>
       <c r="B156" s="1">
-        <v>45736</v>
+        <v>45812</v>
       </c>
       <c r="C156" s="6">
-        <v>8.4099999999999994E-2</v>
+        <v>8.48E-2</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
@@ -12898,10 +13498,10 @@
         <v>2025</v>
       </c>
       <c r="B157" s="1">
-        <v>45767</v>
+        <v>45813</v>
       </c>
       <c r="C157" s="6">
-        <v>8.4400000000000003E-2</v>
+        <v>8.48E-2</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
@@ -12909,10 +13509,10 @@
         <v>2025</v>
       </c>
       <c r="B158" s="1">
-        <v>45797</v>
+        <v>45814</v>
       </c>
       <c r="C158" s="6">
-        <v>8.4699999999999998E-2</v>
+        <v>8.48E-2</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
@@ -12920,10 +13520,10 @@
         <v>2025</v>
       </c>
       <c r="B159" s="1">
-        <v>45828</v>
+        <v>45815</v>
       </c>
       <c r="C159" s="6">
-        <v>8.4900000000000003E-2</v>
+        <v>8.48E-2</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
@@ -12931,10 +13531,10 @@
         <v>2025</v>
       </c>
       <c r="B160" s="1">
-        <v>45858</v>
+        <v>45816</v>
       </c>
       <c r="C160" s="6">
-        <v>8.5199999999999998E-2</v>
+        <v>8.48E-2</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
@@ -12942,10 +13542,10 @@
         <v>2025</v>
       </c>
       <c r="B161" s="1">
-        <v>45889</v>
+        <v>45817</v>
       </c>
       <c r="C161" s="6">
-        <v>8.5400000000000004E-2</v>
+        <v>8.48E-2</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
@@ -12953,10 +13553,10 @@
         <v>2025</v>
       </c>
       <c r="B162" s="1">
-        <v>45678</v>
+        <v>45818</v>
       </c>
       <c r="C162" s="6">
-        <v>8.3699999999999997E-2</v>
+        <v>8.48E-2</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
@@ -12964,10 +13564,10 @@
         <v>2025</v>
       </c>
       <c r="B163" s="1">
-        <v>45709</v>
+        <v>45819</v>
       </c>
       <c r="C163" s="6">
-        <v>8.3900000000000002E-2</v>
+        <v>8.48E-2</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
@@ -12975,10 +13575,10 @@
         <v>2025</v>
       </c>
       <c r="B164" s="1">
-        <v>45737</v>
+        <v>45820</v>
       </c>
       <c r="C164" s="6">
-        <v>8.4099999999999994E-2</v>
+        <v>8.48E-2</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
@@ -12986,10 +13586,10 @@
         <v>2025</v>
       </c>
       <c r="B165" s="1">
-        <v>45768</v>
+        <v>45821</v>
       </c>
       <c r="C165" s="6">
-        <v>8.4400000000000003E-2</v>
+        <v>8.48E-2</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
@@ -12997,10 +13597,10 @@
         <v>2025</v>
       </c>
       <c r="B166" s="1">
-        <v>45798</v>
+        <v>45822</v>
       </c>
       <c r="C166" s="6">
-        <v>8.4699999999999998E-2</v>
+        <v>8.4900000000000003E-2</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
@@ -13008,7 +13608,7 @@
         <v>2025</v>
       </c>
       <c r="B167" s="1">
-        <v>45829</v>
+        <v>45823</v>
       </c>
       <c r="C167" s="6">
         <v>8.4900000000000003E-2</v>
@@ -13019,10 +13619,10 @@
         <v>2025</v>
       </c>
       <c r="B168" s="1">
-        <v>45859</v>
+        <v>45824</v>
       </c>
       <c r="C168" s="6">
-        <v>8.5199999999999998E-2</v>
+        <v>8.4900000000000003E-2</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
@@ -13030,10 +13630,10 @@
         <v>2025</v>
       </c>
       <c r="B169" s="1">
-        <v>45890</v>
+        <v>45825</v>
       </c>
       <c r="C169" s="6">
-        <v>8.5400000000000004E-2</v>
+        <v>8.4900000000000003E-2</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
@@ -13041,10 +13641,10 @@
         <v>2025</v>
       </c>
       <c r="B170" s="1">
-        <v>45679</v>
+        <v>45826</v>
       </c>
       <c r="C170" s="6">
-        <v>8.3699999999999997E-2</v>
+        <v>8.4900000000000003E-2</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
@@ -13052,10 +13652,10 @@
         <v>2025</v>
       </c>
       <c r="B171" s="1">
-        <v>45710</v>
+        <v>45827</v>
       </c>
       <c r="C171" s="6">
-        <v>8.3900000000000002E-2</v>
+        <v>8.4900000000000003E-2</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
@@ -13063,10 +13663,10 @@
         <v>2025</v>
       </c>
       <c r="B172" s="1">
-        <v>45738</v>
+        <v>45828</v>
       </c>
       <c r="C172" s="6">
-        <v>8.4199999999999997E-2</v>
+        <v>8.4900000000000003E-2</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
@@ -13074,10 +13674,10 @@
         <v>2025</v>
       </c>
       <c r="B173" s="1">
-        <v>45769</v>
+        <v>45829</v>
       </c>
       <c r="C173" s="6">
-        <v>8.4400000000000003E-2</v>
+        <v>8.4900000000000003E-2</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
@@ -13085,10 +13685,10 @@
         <v>2025</v>
       </c>
       <c r="B174" s="1">
-        <v>45799</v>
+        <v>45830</v>
       </c>
       <c r="C174" s="6">
-        <v>8.4699999999999998E-2</v>
+        <v>8.4900000000000003E-2</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
@@ -13096,10 +13696,10 @@
         <v>2025</v>
       </c>
       <c r="B175" s="1">
-        <v>45830</v>
+        <v>45831</v>
       </c>
       <c r="C175" s="6">
-        <v>8.4900000000000003E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
@@ -13107,10 +13707,10 @@
         <v>2025</v>
       </c>
       <c r="B176" s="1">
-        <v>45860</v>
+        <v>45832</v>
       </c>
       <c r="C176" s="6">
-        <v>8.5199999999999998E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
@@ -13118,10 +13718,10 @@
         <v>2025</v>
       </c>
       <c r="B177" s="1">
-        <v>45891</v>
+        <v>45833</v>
       </c>
       <c r="C177" s="6">
-        <v>8.5400000000000004E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
@@ -13129,10 +13729,10 @@
         <v>2025</v>
       </c>
       <c r="B178" s="1">
-        <v>45680</v>
+        <v>45834</v>
       </c>
       <c r="C178" s="6">
-        <v>8.3699999999999997E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
@@ -13140,10 +13740,10 @@
         <v>2025</v>
       </c>
       <c r="B179" s="1">
-        <v>45711</v>
+        <v>45835</v>
       </c>
       <c r="C179" s="6">
-        <v>8.3900000000000002E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
@@ -13151,10 +13751,10 @@
         <v>2025</v>
       </c>
       <c r="B180" s="1">
-        <v>45739</v>
+        <v>45836</v>
       </c>
       <c r="C180" s="6">
-        <v>8.4199999999999997E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
@@ -13162,10 +13762,10 @@
         <v>2025</v>
       </c>
       <c r="B181" s="1">
-        <v>45770</v>
+        <v>45837</v>
       </c>
       <c r="C181" s="6">
-        <v>8.4400000000000003E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
@@ -13173,10 +13773,10 @@
         <v>2025</v>
       </c>
       <c r="B182" s="1">
-        <v>45800</v>
+        <v>45838</v>
       </c>
       <c r="C182" s="6">
-        <v>8.4699999999999998E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
@@ -13184,7 +13784,7 @@
         <v>2025</v>
       </c>
       <c r="B183" s="1">
-        <v>45831</v>
+        <v>45839</v>
       </c>
       <c r="C183" s="6">
         <v>8.5000000000000006E-2</v>
@@ -13195,10 +13795,10 @@
         <v>2025</v>
       </c>
       <c r="B184" s="1">
-        <v>45861</v>
+        <v>45840</v>
       </c>
       <c r="C184" s="6">
-        <v>8.5199999999999998E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
@@ -13206,10 +13806,10 @@
         <v>2025</v>
       </c>
       <c r="B185" s="1">
-        <v>45892</v>
+        <v>45841</v>
       </c>
       <c r="C185" s="6">
-        <v>8.5400000000000004E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
@@ -13217,10 +13817,10 @@
         <v>2025</v>
       </c>
       <c r="B186" s="1">
-        <v>45681</v>
+        <v>45842</v>
       </c>
       <c r="C186" s="6">
-        <v>8.3699999999999997E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
@@ -13228,10 +13828,10 @@
         <v>2025</v>
       </c>
       <c r="B187" s="1">
-        <v>45712</v>
+        <v>45843</v>
       </c>
       <c r="C187" s="6">
-        <v>8.3900000000000002E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
@@ -13239,10 +13839,10 @@
         <v>2025</v>
       </c>
       <c r="B188" s="1">
-        <v>45740</v>
+        <v>45844</v>
       </c>
       <c r="C188" s="6">
-        <v>8.4199999999999997E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
@@ -13250,10 +13850,10 @@
         <v>2025</v>
       </c>
       <c r="B189" s="1">
-        <v>45771</v>
+        <v>45845</v>
       </c>
       <c r="C189" s="6">
-        <v>8.4500000000000006E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
@@ -13261,10 +13861,10 @@
         <v>2025</v>
       </c>
       <c r="B190" s="1">
-        <v>45801</v>
+        <v>45846</v>
       </c>
       <c r="C190" s="6">
-        <v>8.4699999999999998E-2</v>
+        <v>8.5099999999999995E-2</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
@@ -13272,10 +13872,10 @@
         <v>2025</v>
       </c>
       <c r="B191" s="1">
-        <v>45832</v>
+        <v>45847</v>
       </c>
       <c r="C191" s="6">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5099999999999995E-2</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
@@ -13283,10 +13883,10 @@
         <v>2025</v>
       </c>
       <c r="B192" s="1">
-        <v>45862</v>
+        <v>45848</v>
       </c>
       <c r="C192" s="6">
-        <v>8.5199999999999998E-2</v>
+        <v>8.5099999999999995E-2</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
@@ -13294,10 +13894,10 @@
         <v>2025</v>
       </c>
       <c r="B193" s="1">
-        <v>45682</v>
+        <v>45849</v>
       </c>
       <c r="C193" s="6">
-        <v>8.3699999999999997E-2</v>
+        <v>8.5099999999999995E-2</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
@@ -13305,10 +13905,10 @@
         <v>2025</v>
       </c>
       <c r="B194" s="1">
-        <v>45713</v>
+        <v>45850</v>
       </c>
       <c r="C194" s="6">
-        <v>8.3900000000000002E-2</v>
+        <v>8.5099999999999995E-2</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
@@ -13316,10 +13916,10 @@
         <v>2025</v>
       </c>
       <c r="B195" s="1">
-        <v>45741</v>
+        <v>45851</v>
       </c>
       <c r="C195" s="6">
-        <v>8.4199999999999997E-2</v>
+        <v>8.5099999999999995E-2</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
@@ -13327,10 +13927,10 @@
         <v>2025</v>
       </c>
       <c r="B196" s="1">
-        <v>45772</v>
+        <v>45852</v>
       </c>
       <c r="C196" s="6">
-        <v>8.4500000000000006E-2</v>
+        <v>8.5099999999999995E-2</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
@@ -13338,10 +13938,10 @@
         <v>2025</v>
       </c>
       <c r="B197" s="1">
-        <v>45802</v>
+        <v>45853</v>
       </c>
       <c r="C197" s="6">
-        <v>8.4699999999999998E-2</v>
+        <v>8.5099999999999995E-2</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
@@ -13349,10 +13949,10 @@
         <v>2025</v>
       </c>
       <c r="B198" s="1">
-        <v>45833</v>
+        <v>45854</v>
       </c>
       <c r="C198" s="6">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5099999999999995E-2</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
@@ -13360,10 +13960,10 @@
         <v>2025</v>
       </c>
       <c r="B199" s="1">
-        <v>45863</v>
+        <v>45855</v>
       </c>
       <c r="C199" s="6">
-        <v>8.5199999999999998E-2</v>
+        <v>8.5099999999999995E-2</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
@@ -13371,10 +13971,10 @@
         <v>2025</v>
       </c>
       <c r="B200" s="1">
-        <v>45683</v>
+        <v>45856</v>
       </c>
       <c r="C200" s="6">
-        <v>8.3699999999999997E-2</v>
+        <v>8.5099999999999995E-2</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
@@ -13382,10 +13982,10 @@
         <v>2025</v>
       </c>
       <c r="B201" s="1">
-        <v>45714</v>
+        <v>45857</v>
       </c>
       <c r="C201" s="6">
-        <v>8.3900000000000002E-2</v>
+        <v>8.5199999999999998E-2</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
@@ -13393,10 +13993,10 @@
         <v>2025</v>
       </c>
       <c r="B202" s="1">
-        <v>45742</v>
+        <v>45858</v>
       </c>
       <c r="C202" s="6">
-        <v>8.4199999999999997E-2</v>
+        <v>8.5199999999999998E-2</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
@@ -13404,10 +14004,10 @@
         <v>2025</v>
       </c>
       <c r="B203" s="1">
-        <v>45773</v>
+        <v>45859</v>
       </c>
       <c r="C203" s="6">
-        <v>8.4500000000000006E-2</v>
+        <v>8.5199999999999998E-2</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
@@ -13415,10 +14015,10 @@
         <v>2025</v>
       </c>
       <c r="B204" s="1">
-        <v>45803</v>
+        <v>45860</v>
       </c>
       <c r="C204" s="6">
-        <v>8.4699999999999998E-2</v>
+        <v>8.5199999999999998E-2</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
@@ -13426,10 +14026,10 @@
         <v>2025</v>
       </c>
       <c r="B205" s="1">
-        <v>45834</v>
+        <v>45861</v>
       </c>
       <c r="C205" s="6">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5199999999999998E-2</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
@@ -13437,7 +14037,7 @@
         <v>2025</v>
       </c>
       <c r="B206" s="1">
-        <v>45864</v>
+        <v>45862</v>
       </c>
       <c r="C206" s="6">
         <v>8.5199999999999998E-2</v>
@@ -13448,10 +14048,10 @@
         <v>2025</v>
       </c>
       <c r="B207" s="1">
-        <v>45684</v>
+        <v>45863</v>
       </c>
       <c r="C207" s="6">
-        <v>8.3699999999999997E-2</v>
+        <v>8.5199999999999998E-2</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
@@ -13459,10 +14059,10 @@
         <v>2025</v>
       </c>
       <c r="B208" s="1">
-        <v>45715</v>
+        <v>45864</v>
       </c>
       <c r="C208" s="6">
-        <v>8.4000000000000005E-2</v>
+        <v>8.5199999999999998E-2</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
@@ -13470,10 +14070,10 @@
         <v>2025</v>
       </c>
       <c r="B209" s="1">
-        <v>45743</v>
+        <v>45865</v>
       </c>
       <c r="C209" s="6">
-        <v>8.4199999999999997E-2</v>
+        <v>8.5199999999999998E-2</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
@@ -13481,10 +14081,10 @@
         <v>2025</v>
       </c>
       <c r="B210" s="1">
-        <v>45774</v>
+        <v>45866</v>
       </c>
       <c r="C210" s="6">
-        <v>8.4500000000000006E-2</v>
+        <v>8.5199999999999998E-2</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
@@ -13492,10 +14092,10 @@
         <v>2025</v>
       </c>
       <c r="B211" s="1">
-        <v>45804</v>
+        <v>45867</v>
       </c>
       <c r="C211" s="6">
-        <v>8.48E-2</v>
+        <v>8.5199999999999998E-2</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
@@ -13503,10 +14103,10 @@
         <v>2025</v>
       </c>
       <c r="B212" s="1">
-        <v>45835</v>
+        <v>45868</v>
       </c>
       <c r="C212" s="6">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5199999999999998E-2</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
@@ -13514,10 +14114,10 @@
         <v>2025</v>
       </c>
       <c r="B213" s="1">
-        <v>45865</v>
+        <v>45869</v>
       </c>
       <c r="C213" s="6">
-        <v>8.5199999999999998E-2</v>
+        <v>8.5300000000000001E-2</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
@@ -13525,10 +14125,10 @@
         <v>2025</v>
       </c>
       <c r="B214" s="1">
-        <v>45685</v>
+        <v>45870</v>
       </c>
       <c r="C214" s="6">
-        <v>8.3699999999999997E-2</v>
+        <v>8.5300000000000001E-2</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
@@ -13536,10 +14136,10 @@
         <v>2025</v>
       </c>
       <c r="B215" s="1">
-        <v>45716</v>
+        <v>45871</v>
       </c>
       <c r="C215" s="6">
-        <v>8.4000000000000005E-2</v>
+        <v>8.5300000000000001E-2</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
@@ -13547,10 +14147,10 @@
         <v>2025</v>
       </c>
       <c r="B216" s="1">
-        <v>45744</v>
+        <v>45872</v>
       </c>
       <c r="C216" s="6">
-        <v>8.4199999999999997E-2</v>
+        <v>8.5300000000000001E-2</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
@@ -13558,10 +14158,10 @@
         <v>2025</v>
       </c>
       <c r="B217" s="1">
-        <v>45775</v>
+        <v>45873</v>
       </c>
       <c r="C217" s="6">
-        <v>8.4500000000000006E-2</v>
+        <v>8.5300000000000001E-2</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
@@ -13569,10 +14169,10 @@
         <v>2025</v>
       </c>
       <c r="B218" s="1">
-        <v>45805</v>
+        <v>45874</v>
       </c>
       <c r="C218" s="6">
-        <v>8.48E-2</v>
+        <v>8.5300000000000001E-2</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
@@ -13580,10 +14180,10 @@
         <v>2025</v>
       </c>
       <c r="B219" s="1">
-        <v>45836</v>
+        <v>45875</v>
       </c>
       <c r="C219" s="6">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5300000000000001E-2</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
@@ -13591,10 +14191,10 @@
         <v>2025</v>
       </c>
       <c r="B220" s="1">
-        <v>45866</v>
+        <v>45876</v>
       </c>
       <c r="C220" s="6">
-        <v>8.5199999999999998E-2</v>
+        <v>8.5300000000000001E-2</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
@@ -13602,10 +14202,10 @@
         <v>2025</v>
       </c>
       <c r="B221" s="1">
-        <v>45686</v>
+        <v>45877</v>
       </c>
       <c r="C221" s="6">
-        <v>8.3699999999999997E-2</v>
+        <v>8.5300000000000001E-2</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
@@ -13613,10 +14213,10 @@
         <v>2025</v>
       </c>
       <c r="B222" s="1">
-        <v>45745</v>
+        <v>45878</v>
       </c>
       <c r="C222" s="6">
-        <v>8.4199999999999997E-2</v>
+        <v>8.5300000000000001E-2</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
@@ -13624,10 +14224,10 @@
         <v>2025</v>
       </c>
       <c r="B223" s="1">
-        <v>45776</v>
+        <v>45879</v>
       </c>
       <c r="C223" s="6">
-        <v>8.4500000000000006E-2</v>
+        <v>8.5300000000000001E-2</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
@@ -13635,10 +14235,10 @@
         <v>2025</v>
       </c>
       <c r="B224" s="1">
-        <v>45806</v>
+        <v>45880</v>
       </c>
       <c r="C224" s="6">
-        <v>8.48E-2</v>
+        <v>8.5300000000000001E-2</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
@@ -13646,10 +14246,10 @@
         <v>2025</v>
       </c>
       <c r="B225" s="1">
-        <v>45837</v>
+        <v>45881</v>
       </c>
       <c r="C225" s="6">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5300000000000001E-2</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
@@ -13657,10 +14257,10 @@
         <v>2025</v>
       </c>
       <c r="B226" s="1">
-        <v>45867</v>
+        <v>45882</v>
       </c>
       <c r="C226" s="6">
-        <v>8.5199999999999998E-2</v>
+        <v>8.5300000000000001E-2</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
@@ -13668,10 +14268,10 @@
         <v>2025</v>
       </c>
       <c r="B227" s="1">
-        <v>45687</v>
+        <v>45883</v>
       </c>
       <c r="C227" s="6">
-        <v>8.3699999999999997E-2</v>
+        <v>8.5300000000000001E-2</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
@@ -13679,10 +14279,10 @@
         <v>2025</v>
       </c>
       <c r="B228" s="1">
-        <v>45746</v>
+        <v>45884</v>
       </c>
       <c r="C228" s="6">
-        <v>8.4199999999999997E-2</v>
+        <v>8.5400000000000004E-2</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
@@ -13690,10 +14290,10 @@
         <v>2025</v>
       </c>
       <c r="B229" s="1">
-        <v>45777</v>
+        <v>45885</v>
       </c>
       <c r="C229" s="6">
-        <v>8.4500000000000006E-2</v>
+        <v>8.5400000000000004E-2</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
@@ -13701,10 +14301,10 @@
         <v>2025</v>
       </c>
       <c r="B230" s="1">
-        <v>45807</v>
+        <v>45886</v>
       </c>
       <c r="C230" s="6">
-        <v>8.48E-2</v>
+        <v>8.5400000000000004E-2</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
@@ -13712,10 +14312,10 @@
         <v>2025</v>
       </c>
       <c r="B231" s="1">
-        <v>45838</v>
+        <v>45887</v>
       </c>
       <c r="C231" s="6">
-        <v>8.5000000000000006E-2</v>
+        <v>8.5400000000000004E-2</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
@@ -13723,10 +14323,10 @@
         <v>2025</v>
       </c>
       <c r="B232" s="1">
-        <v>45868</v>
+        <v>45888</v>
       </c>
       <c r="C232" s="6">
-        <v>8.5199999999999998E-2</v>
+        <v>8.5400000000000004E-2</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
@@ -13734,10 +14334,10 @@
         <v>2025</v>
       </c>
       <c r="B233" s="1">
-        <v>45688</v>
+        <v>45889</v>
       </c>
       <c r="C233" s="6">
-        <v>8.3699999999999997E-2</v>
+        <v>8.5400000000000004E-2</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
@@ -13745,10 +14345,10 @@
         <v>2025</v>
       </c>
       <c r="B234" s="1">
-        <v>45747</v>
+        <v>45890</v>
       </c>
       <c r="C234" s="6">
-        <v>8.4199999999999997E-2</v>
+        <v>8.5400000000000004E-2</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
@@ -13756,10 +14356,10 @@
         <v>2025</v>
       </c>
       <c r="B235" s="1">
-        <v>45808</v>
+        <v>45891</v>
       </c>
       <c r="C235" s="6">
-        <v>8.48E-2</v>
+        <v>8.5400000000000004E-2</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
@@ -13767,10 +14367,76 @@
         <v>2025</v>
       </c>
       <c r="B236" s="1">
-        <v>45869</v>
+        <v>45892</v>
       </c>
       <c r="C236" s="6">
-        <v>8.5300000000000001E-2</v>
+        <v>8.5400000000000004E-2</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A237">
+        <v>2025</v>
+      </c>
+      <c r="B237" s="1">
+        <v>45893</v>
+      </c>
+      <c r="C237" s="6">
+        <v>8.5400000000000004E-2</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A238">
+        <v>2025</v>
+      </c>
+      <c r="B238" s="1">
+        <v>45894</v>
+      </c>
+      <c r="C238" s="6">
+        <v>8.5400000000000004E-2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A239">
+        <v>2025</v>
+      </c>
+      <c r="B239" s="1">
+        <v>45895</v>
+      </c>
+      <c r="C239" s="6">
+        <v>8.5400000000000004E-2</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A240">
+        <v>2025</v>
+      </c>
+      <c r="B240" s="1">
+        <v>45896</v>
+      </c>
+      <c r="C240" s="6">
+        <v>8.5400000000000004E-2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A241">
+        <v>2025</v>
+      </c>
+      <c r="B241" s="1">
+        <v>45897</v>
+      </c>
+      <c r="C241" s="6">
+        <v>8.5400000000000004E-2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A242">
+        <v>2025</v>
+      </c>
+      <c r="B242" s="1">
+        <v>45898</v>
+      </c>
+      <c r="C242" s="6">
+        <v>8.5400000000000004E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizar /pregunta y commit para el file de indicadores_v2
</commit_message>
<xml_diff>
--- a/tipo de cambio y tasas de interés.xlsx
+++ b/tipo de cambio y tasas de interés.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA31B18-9A34-4E98-9053-D2AB15881819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8D67F8-3F20-4733-9EF9-1D428724F74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="7" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo de Cambio" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="Wallstreet" sheetId="6" r:id="rId5"/>
     <sheet name="InflaciónUS" sheetId="4" r:id="rId6"/>
     <sheet name="InflaciónMex2" sheetId="8" r:id="rId7"/>
-    <sheet name="InflaciónUS2" sheetId="9" r:id="rId8"/>
+    <sheet name="InflaciónMex" sheetId="10" r:id="rId8"/>
+    <sheet name="InflaciónUS2" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Tasas de interés'!$D$1:$F$30</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>Fecha</t>
   </si>
@@ -93,9 +94,6 @@
   </si>
   <si>
     <t>30Y Treasury</t>
-  </si>
-  <si>
-    <t>Inflación USA</t>
   </si>
   <si>
     <t>Dow Jones</t>
@@ -658,7 +656,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -684,9 +682,6 @@
     <xf numFmtId="10" fontId="0" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Énfasis1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -735,13 +730,7 @@
     <cellStyle name="Título 3" xfId="6" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="19" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -897,14 +886,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}" name="Tabla1" displayName="Tabla1" ref="A1:E64" totalsRowShown="0" dataDxfId="24" dataCellStyle="Moneda">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}" name="Tabla1" displayName="Tabla1" ref="A1:E64" totalsRowShown="0" dataDxfId="22" dataCellStyle="Moneda">
   <autoFilter ref="A1:E64" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8E09B427-5E44-4BBB-89FC-35463079BE46}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{3D7466AA-D045-44D9-96B5-BDFB7062F58C}" name="Fecha" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{157C7180-B5CE-4C51-9BD0-3AEECF3B91F1}" name="Tipo de Cambio FIX" dataDxfId="22" dataCellStyle="Moneda"/>
-    <tableColumn id="4" xr3:uid="{74B4BBBC-E72A-423F-B8FA-CE596B4E990E}" name="Nivel máximo" dataDxfId="21" dataCellStyle="Moneda"/>
-    <tableColumn id="5" xr3:uid="{74EB6E0A-1398-4291-8596-80BA6140571D}" name="Nivel mínimo" dataDxfId="20" dataCellStyle="Moneda"/>
+    <tableColumn id="2" xr3:uid="{3D7466AA-D045-44D9-96B5-BDFB7062F58C}" name="Fecha" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{157C7180-B5CE-4C51-9BD0-3AEECF3B91F1}" name="Tipo de Cambio FIX" dataDxfId="20" dataCellStyle="Moneda"/>
+    <tableColumn id="4" xr3:uid="{74B4BBBC-E72A-423F-B8FA-CE596B4E990E}" name="Nivel máximo" dataDxfId="19" dataCellStyle="Moneda"/>
+    <tableColumn id="5" xr3:uid="{74EB6E0A-1398-4291-8596-80BA6140571D}" name="Nivel mínimo" dataDxfId="18" dataCellStyle="Moneda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -915,7 +904,7 @@
   <autoFilter ref="A1:F63" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B700B119-8C38-4F55-BC79-C4D6BC8E0C88}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{47E09E7D-A904-4405-9048-49D33EE0E8EB}" name="Fecha" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{47E09E7D-A904-4405-9048-49D33EE0E8EB}" name="Fecha" dataDxfId="17"/>
     <tableColumn id="3" xr3:uid="{0E168449-32EF-450B-812C-11DC4F0F3A30}" name="Tasa de Interés Objetivo"/>
     <tableColumn id="4" xr3:uid="{EE5A2D13-088C-4226-A754-1A001EC14095}" name="TIIE 28 días"/>
     <tableColumn id="5" xr3:uid="{91C093C9-2029-4DE0-AF73-BB6DB79C251D}" name="TIIE 91 días"/>
@@ -930,19 +919,19 @@
   <autoFilter ref="A1:N167" xr:uid="{41D25D3A-81CA-4450-B7DF-F71343E59E89}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{4B709A46-FEF4-4082-A1C7-4443452E16C3}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{288E25E9-721A-4984-9062-39446AEF10A2}" name="Fecha" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{B14E5478-3494-4D1C-8F7A-C3666CA59C27}" name="SOFR" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{BA101BB9-5BDD-49C2-A01D-82F8C1F40DE3}" name="1M Treasury" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{7FE75A9A-7044-4B06-B3A6-F01D3A56E2C5}" name="3M Treasury" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{602D7FBF-E731-4F49-9A0B-6365C780F089}" name="6M Treasury" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{7887EB81-463F-4BB8-9E84-4229D2CAC9A1}" name="1Y Treasury" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{8C5475BF-3FF2-497D-B569-0B378CC77D79}" name="2Y Treasury" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{3B424ABE-EF8F-498A-8F4F-7FDBD990A429}" name="3Y Treasury" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{383F89E5-27BF-4792-BA7B-6E4263B946C9}" name="5Y Treasury" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{A94CC5AD-A6E2-4E44-AAAF-147E46B23BA1}" name="7Y Treasury" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{BA073A53-DD09-4842-A47E-B2F4D2CD2F0B}" name="10Y Treasury" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{0AB1292E-1821-4704-ACB3-22F12D9A1EBD}" name="20Y Treasury" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{FCEEF9DA-C290-458F-AEF1-C46CBE6DCD16}" name="30Y Treasury" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{288E25E9-721A-4984-9062-39446AEF10A2}" name="Fecha" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{B14E5478-3494-4D1C-8F7A-C3666CA59C27}" name="SOFR" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{BA101BB9-5BDD-49C2-A01D-82F8C1F40DE3}" name="1M Treasury" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{7FE75A9A-7044-4B06-B3A6-F01D3A56E2C5}" name="3M Treasury" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{602D7FBF-E731-4F49-9A0B-6365C780F089}" name="6M Treasury" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{7887EB81-463F-4BB8-9E84-4229D2CAC9A1}" name="1Y Treasury" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{8C5475BF-3FF2-497D-B569-0B378CC77D79}" name="2Y Treasury" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{3B424ABE-EF8F-498A-8F4F-7FDBD990A429}" name="3Y Treasury" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{383F89E5-27BF-4792-BA7B-6E4263B946C9}" name="5Y Treasury" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{A94CC5AD-A6E2-4E44-AAAF-147E46B23BA1}" name="7Y Treasury" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{BA073A53-DD09-4842-A47E-B2F4D2CD2F0B}" name="10Y Treasury" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{0AB1292E-1821-4704-ACB3-22F12D9A1EBD}" name="20Y Treasury" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{FCEEF9DA-C290-458F-AEF1-C46CBE6DCD16}" name="30Y Treasury" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -953,31 +942,19 @@
   <autoFilter ref="A1:H22" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{7676C863-947F-4296-8B2C-4C1C2493E9D9}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{55C318C8-9926-4D62-8294-177D6BC0FE75}" name="Fecha" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{55C318C8-9926-4D62-8294-177D6BC0FE75}" name="Fecha" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{1D145B8D-1465-4EF3-BECF-49ACE623BEC5}" name="Dow Jones"/>
     <tableColumn id="4" xr3:uid="{F2357A84-5C07-4E65-841A-42DAECACF403}" name="S&amp;P 500"/>
     <tableColumn id="5" xr3:uid="{388751CA-0A21-4A09-8009-2BB8B01233CE}" name="Nasdaq"/>
-    <tableColumn id="6" xr3:uid="{DEF693B5-3B7C-424D-8BCC-52947BCEC3CF}" name="% Dow Jones" dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{DEF693B5-3B7C-424D-8BCC-52947BCEC3CF}" name="% Dow Jones" dataDxfId="2">
       <calculatedColumnFormula>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C1)/C1,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{A64DA0F4-44F9-4388-B98F-ED267001BCC9}" name="% S&amp;P500" dataDxfId="3">
+    <tableColumn id="7" xr3:uid="{A64DA0F4-44F9-4388-B98F-ED267001BCC9}" name="% S&amp;P500" dataDxfId="1">
       <calculatedColumnFormula>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D1)/D1,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{9B8FC688-A5F6-4240-9AD9-64ED7FF46AD3}" name="% Nasdaq" dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{9B8FC688-A5F6-4240-9AD9-64ED7FF46AD3}" name="% Nasdaq" dataDxfId="0">
       <calculatedColumnFormula>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E1)/E1,"")</calculatedColumnFormula>
     </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B90FD302-37FE-4F2B-B60B-6A456523923A}" name="Tabla6" displayName="Tabla6" ref="A1:C8" totalsRowShown="0">
-  <autoFilter ref="A1:C8" xr:uid="{B90FD302-37FE-4F2B-B60B-6A456523923A}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{43F48A9D-2FA0-46A3-84F1-7DEE42E5BF68}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{1AFFE9F5-0B80-4822-A1EA-DB386C299969}" name="Fecha" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{AF83158D-8EA0-4564-B3B9-6FD4F520FAE8}" name="Inflación USA" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12917,22 +12894,22 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -13555,10 +13532,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D941C0-37A8-48F7-8F55-1334D82BCF20}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13566,7 +13543,7 @@
     <col min="3" max="3" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -13574,91 +13551,42 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2025</v>
       </c>
       <c r="B2" s="1">
-        <v>45658</v>
+        <v>45809</v>
       </c>
       <c r="C2" s="6">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2.6700000000000002E-2</v>
+      </c>
+      <c r="D2" s="6">
+        <v>2.9100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2025</v>
       </c>
       <c r="B3" s="1">
-        <v>45689</v>
+        <v>45839</v>
       </c>
       <c r="C3" s="6">
-        <v>2.81E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2025</v>
-      </c>
-      <c r="B4" s="1">
-        <v>45717</v>
-      </c>
-      <c r="C4" s="6">
-        <v>2.41E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2025</v>
-      </c>
-      <c r="B5" s="1">
-        <v>45748</v>
-      </c>
-      <c r="C5" s="6">
-        <v>2.3300000000000001E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2025</v>
-      </c>
-      <c r="B6" s="1">
-        <v>45778</v>
-      </c>
-      <c r="C6" s="6">
-        <v>2.3800000000000002E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2025</v>
-      </c>
-      <c r="B7" s="1">
-        <v>45809</v>
-      </c>
-      <c r="C7" s="6">
-        <v>2.6700000000000002E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2025</v>
-      </c>
-      <c r="B8" s="1">
-        <v>45839</v>
-      </c>
-      <c r="C8" s="6">
         <v>2.7300000000000001E-2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3.0499999999999999E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -13667,7 +13595,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+      <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13680,10 +13608,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -13762,57 +13690,153 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9B52AB-9F4D-4048-B6BB-4409FE75ED91}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2025</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45824</v>
+      </c>
+      <c r="C2" s="6">
+        <v>4.1300000000000003E-2</v>
+      </c>
+      <c r="D2" s="6">
+        <v>4.2799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45839</v>
+      </c>
+      <c r="C3" s="6">
+        <v>3.5499999999999997E-2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2025</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45854</v>
+      </c>
+      <c r="C4" s="6">
+        <v>3.4799999999999998E-2</v>
+      </c>
+      <c r="D4" s="6">
+        <v>4.2200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2025</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45870</v>
+      </c>
+      <c r="C5" s="6">
+        <v>3.49E-2</v>
+      </c>
+      <c r="D5" s="6">
+        <v>4.2099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2025</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45885</v>
+      </c>
+      <c r="C6" s="6">
+        <v>3.5699999999999996E-2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>4.2299999999999997E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8447025A-DEDD-4B7D-9DDD-6B1F377112FD}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.5546875" style="17"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="17" t="s">
+      <c r="C1" t="s">
         <v>28</v>
       </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="17">
-        <v>2025</v>
-      </c>
-      <c r="B2" s="18">
+      <c r="A2">
+        <v>2025</v>
+      </c>
+      <c r="B2" s="1">
         <v>45809</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C2" s="6">
         <v>2.6700000000000002E-2</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="6">
         <v>2.9100000000000001E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="17">
-        <v>2025</v>
-      </c>
-      <c r="B3" s="18">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3" s="1">
         <v>45839</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="6">
         <v>2.7300000000000001E-2</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="6">
         <v>3.0499999999999999E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
actualizar /pregunta y commit para el file de indicadores_v3
</commit_message>
<xml_diff>
--- a/tipo de cambio y tasas de interés.xlsx
+++ b/tipo de cambio y tasas de interés.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8D67F8-3F20-4733-9EF9-1D428724F74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB1BDE2-B518-4155-84C1-9BEBEB1604CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="7" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo de Cambio" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Wallstreet" sheetId="6" r:id="rId5"/>
     <sheet name="InflaciónUS" sheetId="4" r:id="rId6"/>
     <sheet name="InflaciónMex2" sheetId="8" r:id="rId7"/>
-    <sheet name="InflaciónMex" sheetId="10" r:id="rId8"/>
+    <sheet name="InflaciónMEX" sheetId="10" r:id="rId8"/>
     <sheet name="InflaciónUS2" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
@@ -13534,7 +13534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D941C0-37A8-48F7-8F55-1334D82BCF20}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -13693,8 +13693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9B52AB-9F4D-4048-B6BB-4409FE75ED91}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
actualizar /pregunta y commit para el file de indicadores_v4
</commit_message>
<xml_diff>
--- a/tipo de cambio y tasas de interés.xlsx
+++ b/tipo de cambio y tasas de interés.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB1BDE2-B518-4155-84C1-9BEBEB1604CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5BB237-CE45-40A3-A2E3-8E71196AF081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="7" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="6" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo de Cambio" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,7 @@
     <sheet name="SOFR" sheetId="7" r:id="rId4"/>
     <sheet name="Wallstreet" sheetId="6" r:id="rId5"/>
     <sheet name="InflaciónUS" sheetId="4" r:id="rId6"/>
-    <sheet name="InflaciónMex2" sheetId="8" r:id="rId7"/>
-    <sheet name="InflaciónMEX" sheetId="10" r:id="rId8"/>
-    <sheet name="InflaciónUS2" sheetId="9" r:id="rId9"/>
+    <sheet name="InflaciónMEX" sheetId="10" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Tasas de interés'!$D$1:$F$30</definedName>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>Fecha</t>
   </si>
@@ -13591,11 +13589,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60E746B7-63E8-4974-AE98-EF30EFE65B70}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9B52AB-9F4D-4048-B6BB-4409FE75ED91}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13687,160 +13685,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9B52AB-9F4D-4048-B6BB-4409FE75ED91}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2025</v>
-      </c>
-      <c r="B2" s="1">
-        <v>45824</v>
-      </c>
-      <c r="C2" s="6">
-        <v>4.1300000000000003E-2</v>
-      </c>
-      <c r="D2" s="6">
-        <v>4.2799999999999998E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2025</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45839</v>
-      </c>
-      <c r="C3" s="6">
-        <v>3.5499999999999997E-2</v>
-      </c>
-      <c r="D3" s="6">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2025</v>
-      </c>
-      <c r="B4" s="1">
-        <v>45854</v>
-      </c>
-      <c r="C4" s="6">
-        <v>3.4799999999999998E-2</v>
-      </c>
-      <c r="D4" s="6">
-        <v>4.2200000000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2025</v>
-      </c>
-      <c r="B5" s="1">
-        <v>45870</v>
-      </c>
-      <c r="C5" s="6">
-        <v>3.49E-2</v>
-      </c>
-      <c r="D5" s="6">
-        <v>4.2099999999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2025</v>
-      </c>
-      <c r="B6" s="1">
-        <v>45885</v>
-      </c>
-      <c r="C6" s="6">
-        <v>3.5699999999999996E-2</v>
-      </c>
-      <c r="D6" s="6">
-        <v>4.2299999999999997E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8447025A-DEDD-4B7D-9DDD-6B1F377112FD}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2025</v>
-      </c>
-      <c r="B2" s="1">
-        <v>45809</v>
-      </c>
-      <c r="C2" s="6">
-        <v>2.6700000000000002E-2</v>
-      </c>
-      <c r="D2" s="6">
-        <v>2.9100000000000001E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2025</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45839</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2.7300000000000001E-2</v>
-      </c>
-      <c r="D3" s="6">
-        <v>3.0499999999999999E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
actualizar /pregunta y commit para el file de indicadores_v5
</commit_message>
<xml_diff>
--- a/tipo de cambio y tasas de interés.xlsx
+++ b/tipo de cambio y tasas de interés.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5BB237-CE45-40A3-A2E3-8E71196AF081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EE7819-852F-4BF6-8B03-93A763BCCA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="6" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="7" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo de Cambio" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="Wallstreet" sheetId="6" r:id="rId5"/>
     <sheet name="InflaciónUS" sheetId="4" r:id="rId6"/>
     <sheet name="InflaciónMEX" sheetId="10" r:id="rId7"/>
+    <sheet name="InflaciónMex2" sheetId="11" r:id="rId8"/>
+    <sheet name="InflaciónUS2" sheetId="12" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Tasas de interés'!$D$1:$F$30</definedName>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>Fecha</t>
   </si>
@@ -13533,7 +13535,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13592,8 +13594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9B52AB-9F4D-4048-B6BB-4409FE75ED91}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13685,4 +13687,160 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F297D930-9524-46E0-8AFD-08F86DED9AB1}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2025</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45824</v>
+      </c>
+      <c r="C2" s="6">
+        <v>4.1300000000000003E-2</v>
+      </c>
+      <c r="D2" s="6">
+        <v>4.2799999999999998E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45839</v>
+      </c>
+      <c r="C3" s="6">
+        <v>3.5499999999999997E-2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2025</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45854</v>
+      </c>
+      <c r="C4" s="6">
+        <v>3.4799999999999998E-2</v>
+      </c>
+      <c r="D4" s="6">
+        <v>4.2200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2025</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45870</v>
+      </c>
+      <c r="C5" s="6">
+        <v>3.49E-2</v>
+      </c>
+      <c r="D5" s="6">
+        <v>4.2099999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2025</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45885</v>
+      </c>
+      <c r="C6" s="6">
+        <v>3.5699999999999996E-2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>4.2299999999999997E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A5D771-451F-4EF7-BDF0-50D2827A27CA}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2025</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45809</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2.6700000000000002E-2</v>
+      </c>
+      <c r="D2" s="6">
+        <v>2.9100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45839</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2.7300000000000001E-2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3.0499999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
meter nuevo dato de inflación de us
</commit_message>
<xml_diff>
--- a/tipo de cambio y tasas de interés.xlsx
+++ b/tipo de cambio y tasas de interés.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EE7819-852F-4BF6-8B03-93A763BCCA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1FAC32-A76A-41D3-BFE4-732969D08671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="7" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo de Cambio" sheetId="1" r:id="rId1"/>
@@ -656,7 +656,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -682,6 +682,8 @@
     <xf numFmtId="10" fontId="0" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Énfasis1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -13532,10 +13534,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D941C0-37A8-48F7-8F55-1334D82BCF20}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13583,6 +13585,20 @@
       </c>
       <c r="D3" s="6">
         <v>3.0499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2025</v>
+      </c>
+      <c r="B4" s="17">
+        <v>45870</v>
+      </c>
+      <c r="C4" s="18">
+        <v>2.9399999999999999E-2</v>
+      </c>
+      <c r="D4" s="18">
+        <v>3.1099999999999999E-2</v>
       </c>
     </row>
   </sheetData>
@@ -13693,7 +13709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F297D930-9524-46E0-8AFD-08F86DED9AB1}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
agregar tasas de interés US
</commit_message>
<xml_diff>
--- a/tipo de cambio y tasas de interés.xlsx
+++ b/tipo de cambio y tasas de interés.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1FAC32-A76A-41D3-BFE4-732969D08671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8082AABE-D427-4094-80A3-56147C1C15B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="7" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo de Cambio" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,7 @@
     <sheet name="Wallstreet" sheetId="6" r:id="rId5"/>
     <sheet name="InflaciónUS" sheetId="4" r:id="rId6"/>
     <sheet name="InflaciónMEX" sheetId="10" r:id="rId7"/>
-    <sheet name="InflaciónMex2" sheetId="11" r:id="rId8"/>
-    <sheet name="InflaciónUS2" sheetId="12" r:id="rId9"/>
+    <sheet name="Tasas de interés US" sheetId="13" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Tasas de interés'!$D$1:$F$30</definedName>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Fecha</t>
   </si>
@@ -119,15 +118,25 @@
   <si>
     <t>Inflación Anual</t>
   </si>
+  <si>
+    <t>Tasa efectiva de fondos FED</t>
+  </si>
+  <si>
+    <t>Rango objetivo superior FED</t>
+  </si>
+  <si>
+    <t>Rango objetivo inferior FED</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="0.0_)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +283,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Courier"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="35">
@@ -469,7 +490,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -608,8 +629,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -655,8 +685,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -682,10 +718,19 @@
     <xf numFmtId="10" fontId="0" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="48">
     <cellStyle name="20% - Énfasis1" xfId="21" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="25" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="29" builtinId="38" customBuiltin="1"/>
@@ -717,11 +762,14 @@
     <cellStyle name="Énfasis5" xfId="36" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Énfasis6" xfId="40" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="11" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo 2" xfId="47" xr:uid="{3CEDA4A3-9976-4188-924C-8989FB7703CE}"/>
     <cellStyle name="Incorrecto" xfId="9" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Neutral" xfId="10" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="44" xr:uid="{74F88E50-E0AE-4555-9F58-C9E5156B0A26}"/>
+    <cellStyle name="Normal 3 2 2" xfId="46" xr:uid="{EEF2FD27-9350-43C8-82B2-061DBF4D6720}"/>
+    <cellStyle name="Normal 8" xfId="45" xr:uid="{7C74F38C-7988-470E-BE4C-4F91532008DF}"/>
     <cellStyle name="Notas" xfId="17" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
     <cellStyle name="Salida" xfId="12" builtinId="21" customBuiltin="1"/>
@@ -888,8 +936,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}" name="Tabla1" displayName="Tabla1" ref="A1:E64" totalsRowShown="0" dataDxfId="22" dataCellStyle="Moneda">
-  <autoFilter ref="A1:E64" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}" name="Tabla1" displayName="Tabla1" ref="A1:E78" totalsRowShown="0" dataDxfId="22" dataCellStyle="Moneda">
+  <autoFilter ref="A1:E78" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8E09B427-5E44-4BBB-89FC-35463079BE46}" name="Año"/>
     <tableColumn id="2" xr3:uid="{3D7466AA-D045-44D9-96B5-BDFB7062F58C}" name="Fecha" dataDxfId="21"/>
@@ -902,8 +950,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}" name="Tabla2" displayName="Tabla2" ref="A1:F63" totalsRowShown="0">
-  <autoFilter ref="A1:F63" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}" name="Tabla2" displayName="Tabla2" ref="A1:F77" totalsRowShown="0">
+  <autoFilter ref="A1:F77" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B700B119-8C38-4F55-BC79-C4D6BC8E0C88}" name="Año"/>
     <tableColumn id="2" xr3:uid="{47E09E7D-A904-4405-9048-49D33EE0E8EB}" name="Fecha" dataDxfId="17"/>
@@ -917,8 +965,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{41D25D3A-81CA-4450-B7DF-F71343E59E89}" name="Tabla7" displayName="Tabla7" ref="A1:N167" totalsRowShown="0">
-  <autoFilter ref="A1:N167" xr:uid="{41D25D3A-81CA-4450-B7DF-F71343E59E89}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{41D25D3A-81CA-4450-B7DF-F71343E59E89}" name="Tabla7" displayName="Tabla7" ref="A1:N180" totalsRowShown="0">
+  <autoFilter ref="A1:N180" xr:uid="{41D25D3A-81CA-4450-B7DF-F71343E59E89}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{4B709A46-FEF4-4082-A1C7-4443452E16C3}" name="Año"/>
     <tableColumn id="2" xr3:uid="{288E25E9-721A-4984-9062-39446AEF10A2}" name="Fecha" dataDxfId="16"/>
@@ -940,8 +988,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}" name="Tabla8" displayName="Tabla8" ref="A1:H22" totalsRowShown="0">
-  <autoFilter ref="A1:H22" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}" name="Tabla8" displayName="Tabla8" ref="A1:H36" totalsRowShown="0">
+  <autoFilter ref="A1:H36" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{7676C863-947F-4296-8B2C-4C1C2493E9D9}" name="Año"/>
     <tableColumn id="2" xr3:uid="{55C318C8-9926-4D62-8294-177D6BC0FE75}" name="Fecha" dataDxfId="3"/>
@@ -1259,10 +1307,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892B4731-B44C-4F20-9A44-95C4BD8A73FF}">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2360,6 +2408,244 @@
         <v>18.628</v>
       </c>
     </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="26">
+        <v>2025</v>
+      </c>
+      <c r="B65" s="27">
+        <v>45901</v>
+      </c>
+      <c r="C65" s="2">
+        <v>18.646000000000001</v>
+      </c>
+      <c r="D65" s="2">
+        <v>18.664000000000001</v>
+      </c>
+      <c r="E65" s="2">
+        <v>18.616</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="26">
+        <v>2025</v>
+      </c>
+      <c r="B66" s="27">
+        <v>45902</v>
+      </c>
+      <c r="C66" s="2">
+        <v>18.7072</v>
+      </c>
+      <c r="D66" s="2">
+        <v>18.760000000000002</v>
+      </c>
+      <c r="E66" s="2">
+        <v>18.687999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="26">
+        <v>2025</v>
+      </c>
+      <c r="B67" s="27">
+        <v>45903</v>
+      </c>
+      <c r="C67" s="2">
+        <v>18.6873</v>
+      </c>
+      <c r="D67" s="2">
+        <v>18.728999999999999</v>
+      </c>
+      <c r="E67" s="2">
+        <v>18.672999999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="26">
+        <v>2025</v>
+      </c>
+      <c r="B68" s="27">
+        <v>45904</v>
+      </c>
+      <c r="C68" s="2">
+        <v>18.7577</v>
+      </c>
+      <c r="D68" s="2">
+        <v>18.78</v>
+      </c>
+      <c r="E68" s="2">
+        <v>18.734999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="26">
+        <v>2025</v>
+      </c>
+      <c r="B69" s="27">
+        <v>45905</v>
+      </c>
+      <c r="C69" s="2">
+        <v>18.679200000000002</v>
+      </c>
+      <c r="D69" s="2">
+        <v>18.739999999999998</v>
+      </c>
+      <c r="E69" s="2">
+        <v>18.664999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="26">
+        <v>2025</v>
+      </c>
+      <c r="B70" s="27">
+        <v>45908</v>
+      </c>
+      <c r="C70" s="2">
+        <v>18.655000000000001</v>
+      </c>
+      <c r="D70" s="2">
+        <v>18.690000000000001</v>
+      </c>
+      <c r="E70" s="2">
+        <v>18.623999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="26">
+        <v>2025</v>
+      </c>
+      <c r="B71" s="27">
+        <v>45909</v>
+      </c>
+      <c r="C71" s="2">
+        <v>18.635300000000001</v>
+      </c>
+      <c r="D71" s="2">
+        <v>18.655999999999999</v>
+      </c>
+      <c r="E71" s="2">
+        <v>18.616</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="26">
+        <v>2025</v>
+      </c>
+      <c r="B72" s="27">
+        <v>45910</v>
+      </c>
+      <c r="C72" s="2">
+        <v>18.591999999999999</v>
+      </c>
+      <c r="D72" s="2">
+        <v>18.605</v>
+      </c>
+      <c r="E72" s="2">
+        <v>18.571000000000002</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="26">
+        <v>2025</v>
+      </c>
+      <c r="B73" s="27">
+        <v>45911</v>
+      </c>
+      <c r="C73" s="2">
+        <v>18.528700000000001</v>
+      </c>
+      <c r="D73" s="2">
+        <v>18.545999999999999</v>
+      </c>
+      <c r="E73" s="2">
+        <v>18.478000000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="26">
+        <v>2025</v>
+      </c>
+      <c r="B74" s="27">
+        <v>45912</v>
+      </c>
+      <c r="C74" s="2">
+        <v>18.4757</v>
+      </c>
+      <c r="D74" s="2">
+        <v>18.509</v>
+      </c>
+      <c r="E74" s="2">
+        <v>18.439</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="26">
+        <v>2025</v>
+      </c>
+      <c r="B75" s="27">
+        <v>45915</v>
+      </c>
+      <c r="C75" s="2">
+        <v>18.363499999999998</v>
+      </c>
+      <c r="D75" s="2">
+        <v>18.382999999999999</v>
+      </c>
+      <c r="E75" s="2">
+        <v>18.335000000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="26">
+        <v>2025</v>
+      </c>
+      <c r="B76" s="27">
+        <v>45917</v>
+      </c>
+      <c r="C76" s="2">
+        <v>18.325700000000001</v>
+      </c>
+      <c r="D76" s="2">
+        <v>18.353000000000002</v>
+      </c>
+      <c r="E76" s="2">
+        <v>18.202000000000002</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="26">
+        <v>2025</v>
+      </c>
+      <c r="B77" s="27">
+        <v>45918</v>
+      </c>
+      <c r="C77" s="2">
+        <v>18.361000000000001</v>
+      </c>
+      <c r="D77" s="2">
+        <v>18.388000000000002</v>
+      </c>
+      <c r="E77" s="2">
+        <v>18.321999999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="26">
+        <v>2025</v>
+      </c>
+      <c r="B78" s="27">
+        <v>45919</v>
+      </c>
+      <c r="C78" s="2">
+        <v>18.389199999999999</v>
+      </c>
+      <c r="D78" s="2">
+        <v>18.423999999999999</v>
+      </c>
+      <c r="E78" s="2">
+        <v>18.358000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2370,10 +2656,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394FE10B-CC5B-4887-BA9F-8638E71CB003}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3643,6 +3929,286 @@
         <v>8.1600000000000006E-2</v>
       </c>
     </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>2025</v>
+      </c>
+      <c r="B64" s="25">
+        <v>45901</v>
+      </c>
+      <c r="C64" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D64" s="5">
+        <v>8.0399999999999999E-2</v>
+      </c>
+      <c r="E64" s="5">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="F64" s="5">
+        <v>8.1699999999999995E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="24">
+        <v>2025</v>
+      </c>
+      <c r="B65" s="25">
+        <v>45902</v>
+      </c>
+      <c r="C65" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D65" s="5">
+        <v>8.1100000000000005E-2</v>
+      </c>
+      <c r="E65" s="5">
+        <v>8.1699999999999995E-2</v>
+      </c>
+      <c r="F65" s="5">
+        <v>8.2500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="24">
+        <v>2025</v>
+      </c>
+      <c r="B66" s="25">
+        <v>45903</v>
+      </c>
+      <c r="C66" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D66" s="5">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="E66" s="5">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="F66" s="5">
+        <v>8.1500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="24">
+        <v>2025</v>
+      </c>
+      <c r="B67" s="25">
+        <v>45904</v>
+      </c>
+      <c r="C67" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D67" s="5">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="E67" s="5">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="F67" s="5">
+        <v>8.1500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="24">
+        <v>2025</v>
+      </c>
+      <c r="B68" s="25">
+        <v>45905</v>
+      </c>
+      <c r="C68" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D68" s="5">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="E68" s="5">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="F68" s="5">
+        <v>8.1500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="24">
+        <v>2025</v>
+      </c>
+      <c r="B69" s="25">
+        <v>45908</v>
+      </c>
+      <c r="C69" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D69" s="5">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="E69" s="5">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="F69" s="5">
+        <v>8.1500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="24">
+        <v>2025</v>
+      </c>
+      <c r="B70" s="25">
+        <v>45909</v>
+      </c>
+      <c r="C70" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D70" s="5">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E70" s="5">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F70" s="5">
+        <v>8.14E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="24">
+        <v>2025</v>
+      </c>
+      <c r="B71" s="25">
+        <v>45910</v>
+      </c>
+      <c r="C71" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D71" s="5">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E71" s="5">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F71" s="5">
+        <v>8.14E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="24">
+        <v>2025</v>
+      </c>
+      <c r="B72" s="25">
+        <v>45911</v>
+      </c>
+      <c r="C72" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D72" s="5">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E72" s="5">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F72" s="5">
+        <v>8.14E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="24">
+        <v>2025</v>
+      </c>
+      <c r="B73" s="25">
+        <v>45912</v>
+      </c>
+      <c r="C73" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D73" s="5">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E73" s="5">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F73" s="5">
+        <v>8.14E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="24">
+        <v>2025</v>
+      </c>
+      <c r="B74" s="25">
+        <v>45915</v>
+      </c>
+      <c r="C74" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D74" s="5">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E74" s="5">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F74" s="5">
+        <v>8.14E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="24">
+        <v>2025</v>
+      </c>
+      <c r="B75" s="25">
+        <v>45917</v>
+      </c>
+      <c r="C75" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D75" s="5">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="E75" s="5">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="F75" s="5">
+        <v>8.1500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="24">
+        <v>2025</v>
+      </c>
+      <c r="B76" s="25">
+        <v>45918</v>
+      </c>
+      <c r="C76" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D76" s="5">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="E76" s="5">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="F76" s="5">
+        <v>8.1500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="24">
+        <v>2025</v>
+      </c>
+      <c r="B77" s="25">
+        <v>45919</v>
+      </c>
+      <c r="C77" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D77" s="5">
+        <v>8.0299999999999996E-2</v>
+      </c>
+      <c r="E77" s="5">
+        <v>8.09E-2</v>
+      </c>
+      <c r="F77" s="5">
+        <v>8.1600000000000006E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3653,10 +4219,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B7A3E5-7422-42F6-B226-5BFEA691299B}">
-  <dimension ref="A1:N167"/>
+  <dimension ref="A1:N180"/>
   <sheetViews>
-    <sheetView topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C167"/>
+    <sheetView topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="G182" sqref="G182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11015,6 +11581,578 @@
         <v>4.9200000000000001E-2</v>
       </c>
     </row>
+    <row r="168" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A168" s="21">
+        <v>2025</v>
+      </c>
+      <c r="B168" s="20">
+        <v>45902</v>
+      </c>
+      <c r="C168" s="16">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="D168" s="19">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E168" s="19">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F168" s="19">
+        <v>3.9899999999999998E-2</v>
+      </c>
+      <c r="G168" s="19">
+        <v>3.8199999999999998E-2</v>
+      </c>
+      <c r="H168" s="19">
+        <v>3.6600000000000001E-2</v>
+      </c>
+      <c r="I168" s="19">
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="J168" s="19">
+        <v>3.7400000000000003E-2</v>
+      </c>
+      <c r="K168" s="19">
+        <v>3.9800000000000002E-2</v>
+      </c>
+      <c r="L168" s="19">
+        <v>4.2799999999999998E-2</v>
+      </c>
+      <c r="M168" s="19">
+        <v>4.9200000000000001E-2</v>
+      </c>
+      <c r="N168" s="19">
+        <v>4.9700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A169" s="21">
+        <v>2025</v>
+      </c>
+      <c r="B169" s="20">
+        <v>45903</v>
+      </c>
+      <c r="C169" s="16">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="D169" s="19">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="E169" s="19">
+        <v>4.1799999999999997E-2</v>
+      </c>
+      <c r="F169" s="19">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="G169" s="19">
+        <v>3.7699999999999997E-2</v>
+      </c>
+      <c r="H169" s="19">
+        <v>3.61E-2</v>
+      </c>
+      <c r="I169" s="19">
+        <v>3.5799999999999998E-2</v>
+      </c>
+      <c r="J169" s="19">
+        <v>3.6900000000000002E-2</v>
+      </c>
+      <c r="K169" s="19">
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="L169" s="19">
+        <v>4.2200000000000001E-2</v>
+      </c>
+      <c r="M169" s="19">
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="N169" s="19">
+        <v>4.9000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A170" s="21">
+        <v>2025</v>
+      </c>
+      <c r="B170" s="20">
+        <v>45904</v>
+      </c>
+      <c r="C170" s="16">
+        <v>4.41E-2</v>
+      </c>
+      <c r="D170" s="19">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="E170" s="19">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="F170" s="19">
+        <v>3.9399999999999998E-2</v>
+      </c>
+      <c r="G170" s="19">
+        <v>3.7600000000000001E-2</v>
+      </c>
+      <c r="H170" s="19">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="I170" s="19">
+        <v>3.5499999999999997E-2</v>
+      </c>
+      <c r="J170" s="19">
+        <v>3.6499999999999998E-2</v>
+      </c>
+      <c r="K170" s="19">
+        <v>3.8699999999999998E-2</v>
+      </c>
+      <c r="L170" s="19">
+        <v>4.1700000000000001E-2</v>
+      </c>
+      <c r="M170" s="19">
+        <v>4.8099999999999997E-2</v>
+      </c>
+      <c r="N170" s="19">
+        <v>4.8599999999999997E-2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A171" s="21">
+        <v>2025</v>
+      </c>
+      <c r="B171" s="20">
+        <v>45905</v>
+      </c>
+      <c r="C171" s="16">
+        <v>4.4200000000000003E-2</v>
+      </c>
+      <c r="D171" s="19">
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="E171" s="19">
+        <v>4.07E-2</v>
+      </c>
+      <c r="F171" s="19">
+        <v>3.85E-2</v>
+      </c>
+      <c r="G171" s="19">
+        <v>3.6499999999999998E-2</v>
+      </c>
+      <c r="H171" s="19">
+        <v>3.5099999999999999E-2</v>
+      </c>
+      <c r="I171" s="19">
+        <v>3.4799999999999998E-2</v>
+      </c>
+      <c r="J171" s="19">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="K171" s="19">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="L171" s="19">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="M171" s="19">
+        <v>4.7199999999999999E-2</v>
+      </c>
+      <c r="N171" s="19">
+        <v>4.7800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A172" s="21">
+        <v>2025</v>
+      </c>
+      <c r="B172" s="20">
+        <v>45908</v>
+      </c>
+      <c r="C172" s="16">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D172" s="19">
+        <v>4.2599999999999999E-2</v>
+      </c>
+      <c r="E172" s="19">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="F172" s="19">
+        <v>3.8399999999999997E-2</v>
+      </c>
+      <c r="G172" s="19">
+        <v>3.6400000000000002E-2</v>
+      </c>
+      <c r="H172" s="19">
+        <v>3.49E-2</v>
+      </c>
+      <c r="I172" s="19">
+        <v>3.4700000000000002E-2</v>
+      </c>
+      <c r="J172" s="19">
+        <v>3.5700000000000003E-2</v>
+      </c>
+      <c r="K172" s="19">
+        <v>3.7699999999999997E-2</v>
+      </c>
+      <c r="L172" s="19">
+        <v>4.0500000000000001E-2</v>
+      </c>
+      <c r="M172" s="19">
+        <v>4.65E-2</v>
+      </c>
+      <c r="N172" s="19">
+        <v>4.6899999999999997E-2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A173" s="21">
+        <v>2025</v>
+      </c>
+      <c r="B173" s="20">
+        <v>45909</v>
+      </c>
+      <c r="C173" s="16">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D173" s="19">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="E173" s="19">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="F173" s="19">
+        <v>3.85E-2</v>
+      </c>
+      <c r="G173" s="19">
+        <v>3.6799999999999999E-2</v>
+      </c>
+      <c r="H173" s="19">
+        <v>3.5400000000000001E-2</v>
+      </c>
+      <c r="I173" s="19">
+        <v>3.4799999999999998E-2</v>
+      </c>
+      <c r="J173" s="19">
+        <v>3.61E-2</v>
+      </c>
+      <c r="K173" s="19">
+        <v>3.8100000000000002E-2</v>
+      </c>
+      <c r="L173" s="19">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="M173" s="19">
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="N173" s="19">
+        <v>4.7199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A174" s="21">
+        <v>2025</v>
+      </c>
+      <c r="B174" s="20">
+        <v>45910</v>
+      </c>
+      <c r="C174" s="16">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="D174" s="19">
+        <v>4.2299999999999997E-2</v>
+      </c>
+      <c r="E174" s="19">
+        <v>4.0899999999999999E-2</v>
+      </c>
+      <c r="F174" s="19">
+        <v>3.8300000000000001E-2</v>
+      </c>
+      <c r="G174" s="19">
+        <v>3.6600000000000001E-2</v>
+      </c>
+      <c r="H174" s="19">
+        <v>3.5400000000000001E-2</v>
+      </c>
+      <c r="I174" s="19">
+        <v>3.4700000000000002E-2</v>
+      </c>
+      <c r="J174" s="19">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="K174" s="19">
+        <v>3.78E-2</v>
+      </c>
+      <c r="L174" s="19">
+        <v>4.0399999999999998E-2</v>
+      </c>
+      <c r="M174" s="19">
+        <v>4.65E-2</v>
+      </c>
+      <c r="N174" s="19">
+        <v>4.6899999999999997E-2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A175" s="21">
+        <v>2025</v>
+      </c>
+      <c r="B175" s="20">
+        <v>45911</v>
+      </c>
+      <c r="C175" s="16">
+        <v>4.41E-2</v>
+      </c>
+      <c r="D175" s="19">
+        <v>4.2200000000000001E-2</v>
+      </c>
+      <c r="E175" s="19">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="F175" s="19">
+        <v>3.8199999999999998E-2</v>
+      </c>
+      <c r="G175" s="19">
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="H175" s="19">
+        <v>3.5200000000000002E-2</v>
+      </c>
+      <c r="I175" s="19">
+        <v>3.4700000000000002E-2</v>
+      </c>
+      <c r="J175" s="19">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="K175" s="19">
+        <v>3.7600000000000001E-2</v>
+      </c>
+      <c r="L175" s="19">
+        <v>4.0099999999999997E-2</v>
+      </c>
+      <c r="M175" s="19">
+        <v>4.6100000000000002E-2</v>
+      </c>
+      <c r="N175" s="19">
+        <v>4.65E-2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A176" s="21">
+        <v>2025</v>
+      </c>
+      <c r="B176" s="20">
+        <v>45912</v>
+      </c>
+      <c r="C176" s="16">
+        <v>4.4200000000000003E-2</v>
+      </c>
+      <c r="D176" s="19">
+        <v>4.24E-2</v>
+      </c>
+      <c r="E176" s="19">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="F176" s="19">
+        <v>3.8300000000000001E-2</v>
+      </c>
+      <c r="G176" s="19">
+        <v>3.6600000000000001E-2</v>
+      </c>
+      <c r="H176" s="19">
+        <v>3.56E-2</v>
+      </c>
+      <c r="I176" s="19">
+        <v>3.5200000000000002E-2</v>
+      </c>
+      <c r="J176" s="19">
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="K176" s="19">
+        <v>3.8100000000000002E-2</v>
+      </c>
+      <c r="L176" s="19">
+        <v>4.0599999999999997E-2</v>
+      </c>
+      <c r="M176" s="19">
+        <v>4.65E-2</v>
+      </c>
+      <c r="N176" s="19">
+        <v>4.6800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A177" s="21">
+        <v>2025</v>
+      </c>
+      <c r="B177" s="20">
+        <v>45915</v>
+      </c>
+      <c r="C177" s="16">
+        <v>4.5100000000000001E-2</v>
+      </c>
+      <c r="D177" s="19">
+        <v>4.2200000000000001E-2</v>
+      </c>
+      <c r="E177" s="19">
+        <v>4.0599999999999997E-2</v>
+      </c>
+      <c r="F177" s="19">
+        <v>3.8100000000000002E-2</v>
+      </c>
+      <c r="G177" s="19">
+        <v>3.6400000000000002E-2</v>
+      </c>
+      <c r="H177" s="19">
+        <v>3.5400000000000001E-2</v>
+      </c>
+      <c r="I177" s="19">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="J177" s="19">
+        <v>3.61E-2</v>
+      </c>
+      <c r="K177" s="19">
+        <v>3.7900000000000003E-2</v>
+      </c>
+      <c r="L177" s="19">
+        <v>4.0500000000000001E-2</v>
+      </c>
+      <c r="M177" s="19">
+        <v>4.6300000000000001E-2</v>
+      </c>
+      <c r="N177" s="19">
+        <v>4.6600000000000003E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A178" s="21">
+        <v>2025</v>
+      </c>
+      <c r="B178" s="20">
+        <v>45916</v>
+      </c>
+      <c r="C178" s="16">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="D178" s="19">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="E178" s="19">
+        <v>4.0399999999999998E-2</v>
+      </c>
+      <c r="F178" s="19">
+        <v>3.8100000000000002E-2</v>
+      </c>
+      <c r="G178" s="19">
+        <v>3.6200000000000003E-2</v>
+      </c>
+      <c r="H178" s="19">
+        <v>3.5099999999999999E-2</v>
+      </c>
+      <c r="I178" s="19">
+        <v>3.4700000000000002E-2</v>
+      </c>
+      <c r="J178" s="19">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="K178" s="19">
+        <v>3.78E-2</v>
+      </c>
+      <c r="L178" s="19">
+        <v>4.0399999999999998E-2</v>
+      </c>
+      <c r="M178" s="19">
+        <v>4.6100000000000002E-2</v>
+      </c>
+      <c r="N178" s="19">
+        <v>4.65E-2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A179" s="21">
+        <v>2025</v>
+      </c>
+      <c r="B179" s="20">
+        <v>45917</v>
+      </c>
+      <c r="C179" s="16">
+        <v>4.3799999999999999E-2</v>
+      </c>
+      <c r="D179" s="19">
+        <v>4.1700000000000001E-2</v>
+      </c>
+      <c r="E179" s="19">
+        <v>4.02E-2</v>
+      </c>
+      <c r="F179" s="19">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="G179" s="19">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="H179" s="19">
+        <v>3.5200000000000002E-2</v>
+      </c>
+      <c r="I179" s="19">
+        <v>3.5099999999999999E-2</v>
+      </c>
+      <c r="J179" s="19">
+        <v>3.6200000000000003E-2</v>
+      </c>
+      <c r="K179" s="19">
+        <v>3.8100000000000002E-2</v>
+      </c>
+      <c r="L179" s="19">
+        <v>4.0599999999999997E-2</v>
+      </c>
+      <c r="M179" s="19">
+        <v>4.6199999999999998E-2</v>
+      </c>
+      <c r="N179" s="19">
+        <v>4.6600000000000003E-2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A180" s="21">
+        <v>2025</v>
+      </c>
+      <c r="B180" s="20">
+        <v>45918</v>
+      </c>
+      <c r="C180" s="18">
+        <v>4.1399999999999999E-2</v>
+      </c>
+      <c r="D180" s="17">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="E180" s="17">
+        <v>4.0300000000000002E-2</v>
+      </c>
+      <c r="F180" s="17">
+        <v>3.8100000000000002E-2</v>
+      </c>
+      <c r="G180" s="17">
+        <v>3.61E-2</v>
+      </c>
+      <c r="H180" s="17">
+        <v>3.5700000000000003E-2</v>
+      </c>
+      <c r="I180" s="17">
+        <v>3.5499999999999997E-2</v>
+      </c>
+      <c r="J180" s="17">
+        <v>3.6700000000000003E-2</v>
+      </c>
+      <c r="K180" s="17">
+        <v>3.8600000000000002E-2</v>
+      </c>
+      <c r="L180" s="17">
+        <v>4.1099999999999998E-2</v>
+      </c>
+      <c r="M180" s="17">
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="N180" s="17">
+        <v>4.7199999999999999E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -11027,7 +12165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A0379E-1221-4F1B-BC4B-DB7651DB87BC}">
   <dimension ref="A1:C167"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
+    <sheetView topLeftCell="A80" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C167"/>
     </sheetView>
   </sheetViews>
@@ -12877,10 +14015,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6F7ED1-F67A-4D3F-B065-CA644B535717}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:H25"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13521,6 +14659,412 @@
       <c r="H22" s="7">
         <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E21)/E21,"")</f>
         <v>-1.1500001529734162E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="22">
+        <v>2025</v>
+      </c>
+      <c r="B23" s="23">
+        <v>45902</v>
+      </c>
+      <c r="C23" s="22">
+        <v>45295.80859375</v>
+      </c>
+      <c r="D23" s="22">
+        <v>6415.5400390625</v>
+      </c>
+      <c r="E23" s="22">
+        <v>21279.630859375</v>
+      </c>
+      <c r="F23" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C22)/C22,"")</f>
+        <v>-5.4686787731434887E-3</v>
+      </c>
+      <c r="G23" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D22)/D22,"")</f>
+        <v>-6.9222799368615752E-3</v>
+      </c>
+      <c r="H23" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E22)/E22,"")</f>
+        <v>-8.1992731703134075E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="22">
+        <v>2025</v>
+      </c>
+      <c r="B24" s="23">
+        <v>45903</v>
+      </c>
+      <c r="C24" s="22">
+        <v>45271.23046875</v>
+      </c>
+      <c r="D24" s="22">
+        <v>6448.259765625</v>
+      </c>
+      <c r="E24" s="22">
+        <v>21497.73046875</v>
+      </c>
+      <c r="F24" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C23)/C23,"")</f>
+        <v>-5.4261367139809343E-4</v>
+      </c>
+      <c r="G24" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D23)/D23,"")</f>
+        <v>5.1000736279842966E-3</v>
+      </c>
+      <c r="H24" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E23)/E23,"")</f>
+        <v>1.0249219585447535E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="22">
+        <v>2025</v>
+      </c>
+      <c r="B25" s="23">
+        <v>45904</v>
+      </c>
+      <c r="C25" s="22">
+        <v>45621.2890625</v>
+      </c>
+      <c r="D25" s="22">
+        <v>6502.080078125</v>
+      </c>
+      <c r="E25" s="22">
+        <v>21707.689453125</v>
+      </c>
+      <c r="F25" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C24)/C24,"")</f>
+        <v>7.7324735847778599E-3</v>
+      </c>
+      <c r="G25" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D24)/D24,"")</f>
+        <v>8.3464864096993215E-3</v>
+      </c>
+      <c r="H25" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E24)/E24,"")</f>
+        <v>9.7665651116151612E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="22">
+        <v>2025</v>
+      </c>
+      <c r="B26" s="23">
+        <v>45905</v>
+      </c>
+      <c r="C26" s="22">
+        <v>45400.859375</v>
+      </c>
+      <c r="D26" s="22">
+        <v>6481.5</v>
+      </c>
+      <c r="E26" s="22">
+        <v>21700.390625</v>
+      </c>
+      <c r="F26" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C25)/C25,"")</f>
+        <v>-4.8317286080631558E-3</v>
+      </c>
+      <c r="G26" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D25)/D25,"")</f>
+        <v>-3.1651529783888271E-3</v>
+      </c>
+      <c r="H26" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E25)/E25,"")</f>
+        <v>-3.3623238165263479E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="22">
+        <v>2025</v>
+      </c>
+      <c r="B27" s="23">
+        <v>45908</v>
+      </c>
+      <c r="C27" s="22">
+        <v>45514.94921875</v>
+      </c>
+      <c r="D27" s="22">
+        <v>6495.14990234375</v>
+      </c>
+      <c r="E27" s="22">
+        <v>21798.69921875</v>
+      </c>
+      <c r="F27" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C26)/C26,"")</f>
+        <v>2.5129445856442007E-3</v>
+      </c>
+      <c r="G27" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D26)/D26,"")</f>
+        <v>2.1059789159530973E-3</v>
+      </c>
+      <c r="H27" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E26)/E26,"")</f>
+        <v>4.5302683923460476E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="22">
+        <v>2025</v>
+      </c>
+      <c r="B28" s="23">
+        <v>45909</v>
+      </c>
+      <c r="C28" s="22">
+        <v>45711.33984375</v>
+      </c>
+      <c r="D28" s="22">
+        <v>6512.60986328125</v>
+      </c>
+      <c r="E28" s="22">
+        <v>21879.490234375</v>
+      </c>
+      <c r="F28" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C27)/C27,"")</f>
+        <v>4.3148598069641785E-3</v>
+      </c>
+      <c r="G28" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D27)/D27,"")</f>
+        <v>2.688153653112708E-3</v>
+      </c>
+      <c r="H28" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E27)/E27,"")</f>
+        <v>3.7062310376533006E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="22">
+        <v>2025</v>
+      </c>
+      <c r="B29" s="23">
+        <v>45910</v>
+      </c>
+      <c r="C29" s="22">
+        <v>45490.921875</v>
+      </c>
+      <c r="D29" s="22">
+        <v>6532.0400390625</v>
+      </c>
+      <c r="E29" s="22">
+        <v>21886.060546875</v>
+      </c>
+      <c r="F29" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C28)/C28,"")</f>
+        <v>-4.8219537975353662E-3</v>
+      </c>
+      <c r="G29" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D28)/D28,"")</f>
+        <v>2.9834699435627621E-3</v>
+      </c>
+      <c r="H29" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E28)/E28,"")</f>
+        <v>3.0029550184296991E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="22">
+        <v>2025</v>
+      </c>
+      <c r="B30" s="23">
+        <v>45911</v>
+      </c>
+      <c r="C30" s="22">
+        <v>46108</v>
+      </c>
+      <c r="D30" s="22">
+        <v>6587.47021484375</v>
+      </c>
+      <c r="E30" s="22">
+        <v>22043.0703125</v>
+      </c>
+      <c r="F30" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C29)/C29,"")</f>
+        <v>1.3564863044446712E-2</v>
+      </c>
+      <c r="G30" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D29)/D29,"")</f>
+        <v>8.48589038795995E-3</v>
+      </c>
+      <c r="H30" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E29)/E29,"")</f>
+        <v>7.173961951202709E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="22">
+        <v>2025</v>
+      </c>
+      <c r="B31" s="23">
+        <v>45912</v>
+      </c>
+      <c r="C31" s="22">
+        <v>45834.21875</v>
+      </c>
+      <c r="D31" s="22">
+        <v>6584.2900390625</v>
+      </c>
+      <c r="E31" s="22">
+        <v>22141.099609375</v>
+      </c>
+      <c r="F31" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C30)/C30,"")</f>
+        <v>-5.937825323154333E-3</v>
+      </c>
+      <c r="G31" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D30)/D30,"")</f>
+        <v>-4.8276131466735316E-4</v>
+      </c>
+      <c r="H31" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E30)/E30,"")</f>
+        <v>4.4471707201065528E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="22">
+        <v>2025</v>
+      </c>
+      <c r="B32" s="23">
+        <v>45915</v>
+      </c>
+      <c r="C32" s="22">
+        <v>45883.44921875</v>
+      </c>
+      <c r="D32" s="22">
+        <v>6615.27978515625</v>
+      </c>
+      <c r="E32" s="22">
+        <v>22348.75</v>
+      </c>
+      <c r="F32" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C31)/C31,"")</f>
+        <v>1.0740985685503803E-3</v>
+      </c>
+      <c r="G32" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D31)/D31,"")</f>
+        <v>4.7066192269626167E-3</v>
+      </c>
+      <c r="H32" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E31)/E31,"")</f>
+        <v>9.3785039717303158E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="22">
+        <v>2025</v>
+      </c>
+      <c r="B33" s="23">
+        <v>45916</v>
+      </c>
+      <c r="C33" s="22">
+        <v>45757.8984375</v>
+      </c>
+      <c r="D33" s="22">
+        <v>6606.759765625</v>
+      </c>
+      <c r="E33" s="22">
+        <v>22333.9609375</v>
+      </c>
+      <c r="F33" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C32)/C32,"")</f>
+        <v>-2.7362978020992897E-3</v>
+      </c>
+      <c r="G33" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D32)/D32,"")</f>
+        <v>-1.2879303382402232E-3</v>
+      </c>
+      <c r="H33" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E32)/E32,"")</f>
+        <v>-6.6174003020303144E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="22">
+        <v>2025</v>
+      </c>
+      <c r="B34" s="23">
+        <v>45917</v>
+      </c>
+      <c r="C34" s="22">
+        <v>46018.3203125</v>
+      </c>
+      <c r="D34" s="22">
+        <v>6600.35009765625</v>
+      </c>
+      <c r="E34" s="22">
+        <v>22261.330078125</v>
+      </c>
+      <c r="F34" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C33)/C33,"")</f>
+        <v>5.6912988553376453E-3</v>
+      </c>
+      <c r="G34" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D33)/D33,"")</f>
+        <v>-9.7016816051032008E-4</v>
+      </c>
+      <c r="H34" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E33)/E33,"")</f>
+        <v>-3.2520366440262115E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="22">
+        <v>2025</v>
+      </c>
+      <c r="B35" s="23">
+        <v>45918</v>
+      </c>
+      <c r="C35" s="22">
+        <v>46142.421875</v>
+      </c>
+      <c r="D35" s="22">
+        <v>6631.9599609375</v>
+      </c>
+      <c r="E35" s="22">
+        <v>22470.720703125</v>
+      </c>
+      <c r="F35" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C34)/C34,"")</f>
+        <v>2.696786011685224E-3</v>
+      </c>
+      <c r="G35" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D34)/D34,"")</f>
+        <v>4.7891191851284522E-3</v>
+      </c>
+      <c r="H35" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E34)/E34,"")</f>
+        <v>9.4060248990134147E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="22">
+        <v>2025</v>
+      </c>
+      <c r="B36" s="23">
+        <v>45919</v>
+      </c>
+      <c r="C36" s="22">
+        <v>46315.26953125</v>
+      </c>
+      <c r="D36" s="22">
+        <v>6664.35986328125</v>
+      </c>
+      <c r="E36" s="22">
+        <v>22631.48046875</v>
+      </c>
+      <c r="F36" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C35)/C35,"")</f>
+        <v>3.7459597746786022E-3</v>
+      </c>
+      <c r="G36" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D35)/D35,"")</f>
+        <v>4.8854188708295394E-3</v>
+      </c>
+      <c r="H36" s="7">
+        <f>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E35)/E35,"")</f>
+        <v>7.1541882322734389E-3</v>
       </c>
     </row>
   </sheetData>
@@ -13536,7 +15080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D941C0-37A8-48F7-8F55-1334D82BCF20}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -13591,13 +15135,13 @@
       <c r="A4">
         <v>2025</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="1">
         <v>45870</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="6">
         <v>2.9399999999999999E-2</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="6">
         <v>3.1099999999999999E-2</v>
       </c>
     </row>
@@ -13608,10 +15152,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9B52AB-9F4D-4048-B6BB-4409FE75ED91}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D6"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13635,13 +15179,13 @@
         <v>2025</v>
       </c>
       <c r="B2" s="1">
-        <v>45824</v>
+        <v>45809</v>
       </c>
       <c r="C2" s="6">
-        <v>4.1300000000000003E-2</v>
+        <v>4.3200000000000002E-2</v>
       </c>
       <c r="D2" s="6">
-        <v>4.2799999999999998E-2</v>
+        <v>4.24E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -13652,10 +15196,10 @@
         <v>45839</v>
       </c>
       <c r="C3" s="6">
-        <v>3.5499999999999997E-2</v>
+        <v>3.5099999999999999E-2</v>
       </c>
       <c r="D3" s="6">
-        <v>4.2500000000000003E-2</v>
+        <v>4.2299999999999997E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -13663,40 +15207,12 @@
         <v>2025</v>
       </c>
       <c r="B4" s="1">
-        <v>45854</v>
+        <v>45870</v>
       </c>
       <c r="C4" s="6">
-        <v>3.4799999999999998E-2</v>
+        <v>3.5700000000000003E-2</v>
       </c>
       <c r="D4" s="6">
-        <v>4.2200000000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2025</v>
-      </c>
-      <c r="B5" s="1">
-        <v>45870</v>
-      </c>
-      <c r="C5" s="6">
-        <v>3.49E-2</v>
-      </c>
-      <c r="D5" s="6">
-        <v>4.2099999999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2025</v>
-      </c>
-      <c r="B6" s="1">
-        <v>45885</v>
-      </c>
-      <c r="C6" s="6">
-        <v>3.5699999999999996E-2</v>
-      </c>
-      <c r="D6" s="6">
         <v>4.2299999999999997E-2</v>
       </c>
     </row>
@@ -13706,154 +15222,746 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F297D930-9524-46E0-8AFD-08F86DED9AB1}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE3EAA2-8F6D-45D1-94CD-1021786505AF}">
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2025</v>
-      </c>
-      <c r="B2" s="1">
-        <v>45824</v>
-      </c>
-      <c r="C2" s="6">
-        <v>4.1300000000000003E-2</v>
-      </c>
-      <c r="D2" s="6">
-        <v>4.2799999999999998E-2</v>
+      <c r="A2" s="1">
+        <v>45870</v>
+      </c>
+      <c r="B2" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C2" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D2" s="7">
+        <v>4.2500000000000003E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2025</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45839</v>
-      </c>
-      <c r="C3" s="6">
-        <v>3.5499999999999997E-2</v>
-      </c>
-      <c r="D3" s="6">
+      <c r="A3" s="1">
+        <v>45871</v>
+      </c>
+      <c r="B3" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C3" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D3" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2025</v>
-      </c>
-      <c r="B4" s="1">
-        <v>45854</v>
-      </c>
-      <c r="C4" s="6">
-        <v>3.4799999999999998E-2</v>
-      </c>
-      <c r="D4" s="6">
-        <v>4.2200000000000001E-2</v>
+      <c r="A4" s="1">
+        <v>45872</v>
+      </c>
+      <c r="B4" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C4" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>4.2500000000000003E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2025</v>
-      </c>
-      <c r="B5" s="1">
-        <v>45870</v>
-      </c>
-      <c r="C5" s="6">
-        <v>3.49E-2</v>
-      </c>
-      <c r="D5" s="6">
-        <v>4.2099999999999999E-2</v>
+      <c r="A5" s="1">
+        <v>45873</v>
+      </c>
+      <c r="B5" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C5" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D5" s="7">
+        <v>4.2500000000000003E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2025</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="A6" s="1">
+        <v>45874</v>
+      </c>
+      <c r="B6" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C6" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D6" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>45875</v>
+      </c>
+      <c r="B7" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C7" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D7" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>45876</v>
+      </c>
+      <c r="B8" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C8" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D8" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>45877</v>
+      </c>
+      <c r="B9" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C9" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D9" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>45878</v>
+      </c>
+      <c r="B10" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C10" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D10" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>45879</v>
+      </c>
+      <c r="B11" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C11" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D11" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>45880</v>
+      </c>
+      <c r="B12" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C12" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D12" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>45881</v>
+      </c>
+      <c r="B13" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C13" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D13" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>45882</v>
+      </c>
+      <c r="B14" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C14" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D14" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>45883</v>
+      </c>
+      <c r="B15" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C15" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D15" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>45884</v>
+      </c>
+      <c r="B16" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C16" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D16" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>45885</v>
       </c>
-      <c r="C6" s="6">
-        <v>3.5699999999999996E-2</v>
-      </c>
-      <c r="D6" s="6">
-        <v>4.2299999999999997E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A5D771-451F-4EF7-BDF0-50D2827A27CA}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2025</v>
-      </c>
-      <c r="B2" s="1">
-        <v>45809</v>
-      </c>
-      <c r="C2" s="6">
-        <v>2.6700000000000002E-2</v>
-      </c>
-      <c r="D2" s="6">
-        <v>2.9100000000000001E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2025</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45839</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2.7300000000000001E-2</v>
-      </c>
-      <c r="D3" s="6">
-        <v>3.0499999999999999E-2</v>
+      <c r="B17" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C17" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D17" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>45886</v>
+      </c>
+      <c r="B18" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C18" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D18" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>45887</v>
+      </c>
+      <c r="B19" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C19" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D19" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>45888</v>
+      </c>
+      <c r="B20" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C20" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D20" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>45889</v>
+      </c>
+      <c r="B21" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C21" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D21" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>45890</v>
+      </c>
+      <c r="B22" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C22" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D22" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>45891</v>
+      </c>
+      <c r="B23" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C23" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D23" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>45892</v>
+      </c>
+      <c r="B24" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C24" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D24" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>45893</v>
+      </c>
+      <c r="B25" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C25" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D25" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>45894</v>
+      </c>
+      <c r="B26" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C26" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D26" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>45895</v>
+      </c>
+      <c r="B27" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C27" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D27" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>45896</v>
+      </c>
+      <c r="B28" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C28" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D28" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>45897</v>
+      </c>
+      <c r="B29" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C29" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D29" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>45898</v>
+      </c>
+      <c r="B30" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C30" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D30" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>45899</v>
+      </c>
+      <c r="B31" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C31" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D31" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>45900</v>
+      </c>
+      <c r="B32" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C32" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D32" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>45901</v>
+      </c>
+      <c r="B33" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C33" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D33" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>45902</v>
+      </c>
+      <c r="B34" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C34" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D34" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>45903</v>
+      </c>
+      <c r="B35" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C35" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D35" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>45904</v>
+      </c>
+      <c r="B36" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C36" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D36" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>45905</v>
+      </c>
+      <c r="B37" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C37" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D37" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>45906</v>
+      </c>
+      <c r="B38" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C38" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D38" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>45907</v>
+      </c>
+      <c r="B39" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C39" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D39" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>45908</v>
+      </c>
+      <c r="B40" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C40" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D40" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>45909</v>
+      </c>
+      <c r="B41" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C41" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D41" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>45910</v>
+      </c>
+      <c r="B42" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C42" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D42" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>45911</v>
+      </c>
+      <c r="B43" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C43" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D43" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>45912</v>
+      </c>
+      <c r="B44" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C44" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D44" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>45913</v>
+      </c>
+      <c r="B45" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C45" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D45" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>45914</v>
+      </c>
+      <c r="B46" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C46" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D46" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>45915</v>
+      </c>
+      <c r="B47" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C47" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D47" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>45916</v>
+      </c>
+      <c r="B48" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C48" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D48" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>45917</v>
+      </c>
+      <c r="B49" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="C49" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D49" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>45918</v>
+      </c>
+      <c r="B50" s="7">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="C50" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="D50" s="7">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>45919</v>
+      </c>
+      <c r="B51" s="7">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="C51" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="D51" s="7">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>45920</v>
+      </c>
+      <c r="B52" s="7">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="C52" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="D52" s="7">
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregar tasas de interés US_v3
</commit_message>
<xml_diff>
--- a/tipo de cambio y tasas de interés.xlsx
+++ b/tipo de cambio y tasas de interés.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8082AABE-D427-4094-80A3-56147C1C15B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1586D41E-D4B9-4D70-8E12-E6C15689B6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="7" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
   </bookViews>
@@ -119,13 +119,13 @@
     <t>Inflación Anual</t>
   </si>
   <si>
-    <t>Tasa efectiva de fondos FED</t>
-  </si>
-  <si>
     <t>Rango objetivo superior FED</t>
   </si>
   <si>
     <t>Rango objetivo inferior FED</t>
+  </si>
+  <si>
+    <t>Tasa efectiva FED</t>
   </si>
 </sst>
 </file>
@@ -15225,8 +15225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE3EAA2-8F6D-45D1-94CD-1021786505AF}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15241,13 +15241,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
agregar tasas de interés US_v4
</commit_message>
<xml_diff>
--- a/tipo de cambio y tasas de interés.xlsx
+++ b/tipo de cambio y tasas de interés.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1586D41E-D4B9-4D70-8E12-E6C15689B6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA52D60-F3A9-4587-9EFF-B7C827993408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="7" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>Fecha</t>
   </si>
@@ -134,7 +134,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="0.0_)"/>
+    <numFmt numFmtId="164" formatCode="0.0_)"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -685,14 +685,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="169" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="169" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -718,17 +718,7 @@
     <xf numFmtId="10" fontId="0" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="48">
     <cellStyle name="20% - Énfasis1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -2409,10 +2399,10 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="26">
-        <v>2025</v>
-      </c>
-      <c r="B65" s="27">
+      <c r="A65">
+        <v>2025</v>
+      </c>
+      <c r="B65" s="1">
         <v>45901</v>
       </c>
       <c r="C65" s="2">
@@ -2426,10 +2416,10 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="26">
-        <v>2025</v>
-      </c>
-      <c r="B66" s="27">
+      <c r="A66">
+        <v>2025</v>
+      </c>
+      <c r="B66" s="1">
         <v>45902</v>
       </c>
       <c r="C66" s="2">
@@ -2443,10 +2433,10 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="26">
-        <v>2025</v>
-      </c>
-      <c r="B67" s="27">
+      <c r="A67">
+        <v>2025</v>
+      </c>
+      <c r="B67" s="1">
         <v>45903</v>
       </c>
       <c r="C67" s="2">
@@ -2460,10 +2450,10 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="26">
-        <v>2025</v>
-      </c>
-      <c r="B68" s="27">
+      <c r="A68">
+        <v>2025</v>
+      </c>
+      <c r="B68" s="1">
         <v>45904</v>
       </c>
       <c r="C68" s="2">
@@ -2477,10 +2467,10 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="26">
-        <v>2025</v>
-      </c>
-      <c r="B69" s="27">
+      <c r="A69">
+        <v>2025</v>
+      </c>
+      <c r="B69" s="1">
         <v>45905</v>
       </c>
       <c r="C69" s="2">
@@ -2494,10 +2484,10 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="26">
-        <v>2025</v>
-      </c>
-      <c r="B70" s="27">
+      <c r="A70">
+        <v>2025</v>
+      </c>
+      <c r="B70" s="1">
         <v>45908</v>
       </c>
       <c r="C70" s="2">
@@ -2511,10 +2501,10 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="26">
-        <v>2025</v>
-      </c>
-      <c r="B71" s="27">
+      <c r="A71">
+        <v>2025</v>
+      </c>
+      <c r="B71" s="1">
         <v>45909</v>
       </c>
       <c r="C71" s="2">
@@ -2528,10 +2518,10 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="26">
-        <v>2025</v>
-      </c>
-      <c r="B72" s="27">
+      <c r="A72">
+        <v>2025</v>
+      </c>
+      <c r="B72" s="1">
         <v>45910</v>
       </c>
       <c r="C72" s="2">
@@ -2545,10 +2535,10 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A73" s="26">
-        <v>2025</v>
-      </c>
-      <c r="B73" s="27">
+      <c r="A73">
+        <v>2025</v>
+      </c>
+      <c r="B73" s="1">
         <v>45911</v>
       </c>
       <c r="C73" s="2">
@@ -2562,10 +2552,10 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" s="26">
-        <v>2025</v>
-      </c>
-      <c r="B74" s="27">
+      <c r="A74">
+        <v>2025</v>
+      </c>
+      <c r="B74" s="1">
         <v>45912</v>
       </c>
       <c r="C74" s="2">
@@ -2579,10 +2569,10 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="26">
-        <v>2025</v>
-      </c>
-      <c r="B75" s="27">
+      <c r="A75">
+        <v>2025</v>
+      </c>
+      <c r="B75" s="1">
         <v>45915</v>
       </c>
       <c r="C75" s="2">
@@ -2596,10 +2586,10 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="26">
-        <v>2025</v>
-      </c>
-      <c r="B76" s="27">
+      <c r="A76">
+        <v>2025</v>
+      </c>
+      <c r="B76" s="1">
         <v>45917</v>
       </c>
       <c r="C76" s="2">
@@ -2613,10 +2603,10 @@
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A77" s="26">
-        <v>2025</v>
-      </c>
-      <c r="B77" s="27">
+      <c r="A77">
+        <v>2025</v>
+      </c>
+      <c r="B77" s="1">
         <v>45918</v>
       </c>
       <c r="C77" s="2">
@@ -2630,10 +2620,10 @@
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" s="26">
-        <v>2025</v>
-      </c>
-      <c r="B78" s="27">
+      <c r="A78">
+        <v>2025</v>
+      </c>
+      <c r="B78" s="1">
         <v>45919</v>
       </c>
       <c r="C78" s="2">
@@ -3933,7 +3923,7 @@
       <c r="A64">
         <v>2025</v>
       </c>
-      <c r="B64" s="25">
+      <c r="B64" s="1">
         <v>45901</v>
       </c>
       <c r="C64" s="5">
@@ -3950,10 +3940,10 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="24">
-        <v>2025</v>
-      </c>
-      <c r="B65" s="25">
+      <c r="A65">
+        <v>2025</v>
+      </c>
+      <c r="B65" s="1">
         <v>45902</v>
       </c>
       <c r="C65" s="5">
@@ -3970,10 +3960,10 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="24">
-        <v>2025</v>
-      </c>
-      <c r="B66" s="25">
+      <c r="A66">
+        <v>2025</v>
+      </c>
+      <c r="B66" s="1">
         <v>45903</v>
       </c>
       <c r="C66" s="5">
@@ -3990,10 +3980,10 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="24">
-        <v>2025</v>
-      </c>
-      <c r="B67" s="25">
+      <c r="A67">
+        <v>2025</v>
+      </c>
+      <c r="B67" s="1">
         <v>45904</v>
       </c>
       <c r="C67" s="5">
@@ -4010,10 +4000,10 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="24">
-        <v>2025</v>
-      </c>
-      <c r="B68" s="25">
+      <c r="A68">
+        <v>2025</v>
+      </c>
+      <c r="B68" s="1">
         <v>45905</v>
       </c>
       <c r="C68" s="5">
@@ -4030,10 +4020,10 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="24">
-        <v>2025</v>
-      </c>
-      <c r="B69" s="25">
+      <c r="A69">
+        <v>2025</v>
+      </c>
+      <c r="B69" s="1">
         <v>45908</v>
       </c>
       <c r="C69" s="5">
@@ -4050,10 +4040,10 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="24">
-        <v>2025</v>
-      </c>
-      <c r="B70" s="25">
+      <c r="A70">
+        <v>2025</v>
+      </c>
+      <c r="B70" s="1">
         <v>45909</v>
       </c>
       <c r="C70" s="5">
@@ -4070,10 +4060,10 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="24">
-        <v>2025</v>
-      </c>
-      <c r="B71" s="25">
+      <c r="A71">
+        <v>2025</v>
+      </c>
+      <c r="B71" s="1">
         <v>45910</v>
       </c>
       <c r="C71" s="5">
@@ -4090,10 +4080,10 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="24">
-        <v>2025</v>
-      </c>
-      <c r="B72" s="25">
+      <c r="A72">
+        <v>2025</v>
+      </c>
+      <c r="B72" s="1">
         <v>45911</v>
       </c>
       <c r="C72" s="5">
@@ -4110,10 +4100,10 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="24">
-        <v>2025</v>
-      </c>
-      <c r="B73" s="25">
+      <c r="A73">
+        <v>2025</v>
+      </c>
+      <c r="B73" s="1">
         <v>45912</v>
       </c>
       <c r="C73" s="5">
@@ -4130,10 +4120,10 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="24">
-        <v>2025</v>
-      </c>
-      <c r="B74" s="25">
+      <c r="A74">
+        <v>2025</v>
+      </c>
+      <c r="B74" s="1">
         <v>45915</v>
       </c>
       <c r="C74" s="5">
@@ -4150,10 +4140,10 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="24">
-        <v>2025</v>
-      </c>
-      <c r="B75" s="25">
+      <c r="A75">
+        <v>2025</v>
+      </c>
+      <c r="B75" s="1">
         <v>45917</v>
       </c>
       <c r="C75" s="5">
@@ -4170,10 +4160,10 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="24">
-        <v>2025</v>
-      </c>
-      <c r="B76" s="25">
+      <c r="A76">
+        <v>2025</v>
+      </c>
+      <c r="B76" s="1">
         <v>45918</v>
       </c>
       <c r="C76" s="5">
@@ -4190,10 +4180,10 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="24">
-        <v>2025</v>
-      </c>
-      <c r="B77" s="25">
+      <c r="A77">
+        <v>2025</v>
+      </c>
+      <c r="B77" s="1">
         <v>45919</v>
       </c>
       <c r="C77" s="5">
@@ -11582,574 +11572,574 @@
       </c>
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A168" s="21">
-        <v>2025</v>
-      </c>
-      <c r="B168" s="20">
+      <c r="A168">
+        <v>2025</v>
+      </c>
+      <c r="B168" s="1">
         <v>45902</v>
       </c>
       <c r="C168" s="16">
         <v>4.3900000000000002E-2</v>
       </c>
-      <c r="D168" s="19">
+      <c r="D168" s="6">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="E168" s="19">
+      <c r="E168" s="6">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="F168" s="19">
+      <c r="F168" s="6">
         <v>3.9899999999999998E-2</v>
       </c>
-      <c r="G168" s="19">
+      <c r="G168" s="6">
         <v>3.8199999999999998E-2</v>
       </c>
-      <c r="H168" s="19">
+      <c r="H168" s="6">
         <v>3.6600000000000001E-2</v>
       </c>
-      <c r="I168" s="19">
+      <c r="I168" s="6">
         <v>3.6299999999999999E-2</v>
       </c>
-      <c r="J168" s="19">
+      <c r="J168" s="6">
         <v>3.7400000000000003E-2</v>
       </c>
-      <c r="K168" s="19">
+      <c r="K168" s="6">
         <v>3.9800000000000002E-2</v>
       </c>
-      <c r="L168" s="19">
+      <c r="L168" s="6">
         <v>4.2799999999999998E-2</v>
       </c>
-      <c r="M168" s="19">
+      <c r="M168" s="6">
         <v>4.9200000000000001E-2</v>
       </c>
-      <c r="N168" s="19">
+      <c r="N168" s="6">
         <v>4.9700000000000001E-2</v>
       </c>
     </row>
     <row r="169" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A169" s="21">
-        <v>2025</v>
-      </c>
-      <c r="B169" s="20">
+      <c r="A169">
+        <v>2025</v>
+      </c>
+      <c r="B169" s="1">
         <v>45903</v>
       </c>
       <c r="C169" s="16">
         <v>4.3900000000000002E-2</v>
       </c>
-      <c r="D169" s="19">
+      <c r="D169" s="6">
         <v>4.3499999999999997E-2</v>
       </c>
-      <c r="E169" s="19">
+      <c r="E169" s="6">
         <v>4.1799999999999997E-2</v>
       </c>
-      <c r="F169" s="19">
+      <c r="F169" s="6">
         <v>3.9600000000000003E-2</v>
       </c>
-      <c r="G169" s="19">
+      <c r="G169" s="6">
         <v>3.7699999999999997E-2</v>
       </c>
-      <c r="H169" s="19">
+      <c r="H169" s="6">
         <v>3.61E-2</v>
       </c>
-      <c r="I169" s="19">
+      <c r="I169" s="6">
         <v>3.5799999999999998E-2</v>
       </c>
-      <c r="J169" s="19">
+      <c r="J169" s="6">
         <v>3.6900000000000002E-2</v>
       </c>
-      <c r="K169" s="19">
+      <c r="K169" s="6">
         <v>3.9199999999999999E-2</v>
       </c>
-      <c r="L169" s="19">
+      <c r="L169" s="6">
         <v>4.2200000000000001E-2</v>
       </c>
-      <c r="M169" s="19">
+      <c r="M169" s="6">
         <v>4.8500000000000001E-2</v>
       </c>
-      <c r="N169" s="19">
+      <c r="N169" s="6">
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
     <row r="170" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A170" s="21">
-        <v>2025</v>
-      </c>
-      <c r="B170" s="20">
+      <c r="A170">
+        <v>2025</v>
+      </c>
+      <c r="B170" s="1">
         <v>45904</v>
       </c>
       <c r="C170" s="16">
         <v>4.41E-2</v>
       </c>
-      <c r="D170" s="19">
+      <c r="D170" s="6">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="E170" s="19">
+      <c r="E170" s="6">
         <v>4.1599999999999998E-2</v>
       </c>
-      <c r="F170" s="19">
+      <c r="F170" s="6">
         <v>3.9399999999999998E-2</v>
       </c>
-      <c r="G170" s="19">
+      <c r="G170" s="6">
         <v>3.7600000000000001E-2</v>
       </c>
-      <c r="H170" s="19">
+      <c r="H170" s="6">
         <v>3.5900000000000001E-2</v>
       </c>
-      <c r="I170" s="19">
+      <c r="I170" s="6">
         <v>3.5499999999999997E-2</v>
       </c>
-      <c r="J170" s="19">
+      <c r="J170" s="6">
         <v>3.6499999999999998E-2</v>
       </c>
-      <c r="K170" s="19">
+      <c r="K170" s="6">
         <v>3.8699999999999998E-2</v>
       </c>
-      <c r="L170" s="19">
+      <c r="L170" s="6">
         <v>4.1700000000000001E-2</v>
       </c>
-      <c r="M170" s="19">
+      <c r="M170" s="6">
         <v>4.8099999999999997E-2</v>
       </c>
-      <c r="N170" s="19">
+      <c r="N170" s="6">
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A171" s="21">
-        <v>2025</v>
-      </c>
-      <c r="B171" s="20">
+      <c r="A171">
+        <v>2025</v>
+      </c>
+      <c r="B171" s="1">
         <v>45905</v>
       </c>
       <c r="C171" s="16">
         <v>4.4200000000000003E-2</v>
       </c>
-      <c r="D171" s="19">
+      <c r="D171" s="6">
         <v>4.2900000000000001E-2</v>
       </c>
-      <c r="E171" s="19">
+      <c r="E171" s="6">
         <v>4.07E-2</v>
       </c>
-      <c r="F171" s="19">
+      <c r="F171" s="6">
         <v>3.85E-2</v>
       </c>
-      <c r="G171" s="19">
+      <c r="G171" s="6">
         <v>3.6499999999999998E-2</v>
       </c>
-      <c r="H171" s="19">
+      <c r="H171" s="6">
         <v>3.5099999999999999E-2</v>
       </c>
-      <c r="I171" s="19">
+      <c r="I171" s="6">
         <v>3.4799999999999998E-2</v>
       </c>
-      <c r="J171" s="19">
+      <c r="J171" s="6">
         <v>3.5900000000000001E-2</v>
       </c>
-      <c r="K171" s="19">
+      <c r="K171" s="6">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="L171" s="19">
+      <c r="L171" s="6">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="M171" s="19">
+      <c r="M171" s="6">
         <v>4.7199999999999999E-2</v>
       </c>
-      <c r="N171" s="19">
+      <c r="N171" s="6">
         <v>4.7800000000000002E-2</v>
       </c>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A172" s="21">
-        <v>2025</v>
-      </c>
-      <c r="B172" s="20">
+      <c r="A172">
+        <v>2025</v>
+      </c>
+      <c r="B172" s="1">
         <v>45908</v>
       </c>
       <c r="C172" s="16">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="D172" s="19">
+      <c r="D172" s="6">
         <v>4.2599999999999999E-2</v>
       </c>
-      <c r="E172" s="19">
+      <c r="E172" s="6">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="F172" s="19">
+      <c r="F172" s="6">
         <v>3.8399999999999997E-2</v>
       </c>
-      <c r="G172" s="19">
+      <c r="G172" s="6">
         <v>3.6400000000000002E-2</v>
       </c>
-      <c r="H172" s="19">
+      <c r="H172" s="6">
         <v>3.49E-2</v>
       </c>
-      <c r="I172" s="19">
+      <c r="I172" s="6">
         <v>3.4700000000000002E-2</v>
       </c>
-      <c r="J172" s="19">
+      <c r="J172" s="6">
         <v>3.5700000000000003E-2</v>
       </c>
-      <c r="K172" s="19">
+      <c r="K172" s="6">
         <v>3.7699999999999997E-2</v>
       </c>
-      <c r="L172" s="19">
+      <c r="L172" s="6">
         <v>4.0500000000000001E-2</v>
       </c>
-      <c r="M172" s="19">
+      <c r="M172" s="6">
         <v>4.65E-2</v>
       </c>
-      <c r="N172" s="19">
+      <c r="N172" s="6">
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A173" s="21">
-        <v>2025</v>
-      </c>
-      <c r="B173" s="20">
+      <c r="A173">
+        <v>2025</v>
+      </c>
+      <c r="B173" s="1">
         <v>45909</v>
       </c>
       <c r="C173" s="16">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="D173" s="19">
+      <c r="D173" s="6">
         <v>4.2500000000000003E-2</v>
       </c>
-      <c r="E173" s="19">
+      <c r="E173" s="6">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="F173" s="19">
+      <c r="F173" s="6">
         <v>3.85E-2</v>
       </c>
-      <c r="G173" s="19">
+      <c r="G173" s="6">
         <v>3.6799999999999999E-2</v>
       </c>
-      <c r="H173" s="19">
+      <c r="H173" s="6">
         <v>3.5400000000000001E-2</v>
       </c>
-      <c r="I173" s="19">
+      <c r="I173" s="6">
         <v>3.4799999999999998E-2</v>
       </c>
-      <c r="J173" s="19">
+      <c r="J173" s="6">
         <v>3.61E-2</v>
       </c>
-      <c r="K173" s="19">
+      <c r="K173" s="6">
         <v>3.8100000000000002E-2</v>
       </c>
-      <c r="L173" s="19">
+      <c r="L173" s="6">
         <v>4.0800000000000003E-2</v>
       </c>
-      <c r="M173" s="19">
+      <c r="M173" s="6">
         <v>4.6800000000000001E-2</v>
       </c>
-      <c r="N173" s="19">
+      <c r="N173" s="6">
         <v>4.7199999999999999E-2</v>
       </c>
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A174" s="21">
-        <v>2025</v>
-      </c>
-      <c r="B174" s="20">
+      <c r="A174">
+        <v>2025</v>
+      </c>
+      <c r="B174" s="1">
         <v>45910</v>
       </c>
       <c r="C174" s="16">
         <v>4.3900000000000002E-2</v>
       </c>
-      <c r="D174" s="19">
+      <c r="D174" s="6">
         <v>4.2299999999999997E-2</v>
       </c>
-      <c r="E174" s="19">
+      <c r="E174" s="6">
         <v>4.0899999999999999E-2</v>
       </c>
-      <c r="F174" s="19">
+      <c r="F174" s="6">
         <v>3.8300000000000001E-2</v>
       </c>
-      <c r="G174" s="19">
+      <c r="G174" s="6">
         <v>3.6600000000000001E-2</v>
       </c>
-      <c r="H174" s="19">
+      <c r="H174" s="6">
         <v>3.5400000000000001E-2</v>
       </c>
-      <c r="I174" s="19">
+      <c r="I174" s="6">
         <v>3.4700000000000002E-2</v>
       </c>
-      <c r="J174" s="19">
+      <c r="J174" s="6">
         <v>3.5900000000000001E-2</v>
       </c>
-      <c r="K174" s="19">
+      <c r="K174" s="6">
         <v>3.78E-2</v>
       </c>
-      <c r="L174" s="19">
+      <c r="L174" s="6">
         <v>4.0399999999999998E-2</v>
       </c>
-      <c r="M174" s="19">
+      <c r="M174" s="6">
         <v>4.65E-2</v>
       </c>
-      <c r="N174" s="19">
+      <c r="N174" s="6">
         <v>4.6899999999999997E-2</v>
       </c>
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A175" s="21">
-        <v>2025</v>
-      </c>
-      <c r="B175" s="20">
+      <c r="A175">
+        <v>2025</v>
+      </c>
+      <c r="B175" s="1">
         <v>45911</v>
       </c>
       <c r="C175" s="16">
         <v>4.41E-2</v>
       </c>
-      <c r="D175" s="19">
+      <c r="D175" s="6">
         <v>4.2200000000000001E-2</v>
       </c>
-      <c r="E175" s="19">
+      <c r="E175" s="6">
         <v>4.0800000000000003E-2</v>
       </c>
-      <c r="F175" s="19">
+      <c r="F175" s="6">
         <v>3.8199999999999998E-2</v>
       </c>
-      <c r="G175" s="19">
+      <c r="G175" s="6">
         <v>3.6299999999999999E-2</v>
       </c>
-      <c r="H175" s="19">
+      <c r="H175" s="6">
         <v>3.5200000000000002E-2</v>
       </c>
-      <c r="I175" s="19">
+      <c r="I175" s="6">
         <v>3.4700000000000002E-2</v>
       </c>
-      <c r="J175" s="19">
+      <c r="J175" s="6">
         <v>3.5900000000000001E-2</v>
       </c>
-      <c r="K175" s="19">
+      <c r="K175" s="6">
         <v>3.7600000000000001E-2</v>
       </c>
-      <c r="L175" s="19">
+      <c r="L175" s="6">
         <v>4.0099999999999997E-2</v>
       </c>
-      <c r="M175" s="19">
+      <c r="M175" s="6">
         <v>4.6100000000000002E-2</v>
       </c>
-      <c r="N175" s="19">
+      <c r="N175" s="6">
         <v>4.65E-2</v>
       </c>
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A176" s="21">
-        <v>2025</v>
-      </c>
-      <c r="B176" s="20">
+      <c r="A176">
+        <v>2025</v>
+      </c>
+      <c r="B176" s="1">
         <v>45912</v>
       </c>
       <c r="C176" s="16">
         <v>4.4200000000000003E-2</v>
       </c>
-      <c r="D176" s="19">
+      <c r="D176" s="6">
         <v>4.24E-2</v>
       </c>
-      <c r="E176" s="19">
+      <c r="E176" s="6">
         <v>4.0800000000000003E-2</v>
       </c>
-      <c r="F176" s="19">
+      <c r="F176" s="6">
         <v>3.8300000000000001E-2</v>
       </c>
-      <c r="G176" s="19">
+      <c r="G176" s="6">
         <v>3.6600000000000001E-2</v>
       </c>
-      <c r="H176" s="19">
+      <c r="H176" s="6">
         <v>3.56E-2</v>
       </c>
-      <c r="I176" s="19">
+      <c r="I176" s="6">
         <v>3.5200000000000002E-2</v>
       </c>
-      <c r="J176" s="19">
+      <c r="J176" s="6">
         <v>3.6299999999999999E-2</v>
       </c>
-      <c r="K176" s="19">
+      <c r="K176" s="6">
         <v>3.8100000000000002E-2</v>
       </c>
-      <c r="L176" s="19">
+      <c r="L176" s="6">
         <v>4.0599999999999997E-2</v>
       </c>
-      <c r="M176" s="19">
+      <c r="M176" s="6">
         <v>4.65E-2</v>
       </c>
-      <c r="N176" s="19">
+      <c r="N176" s="6">
         <v>4.6800000000000001E-2</v>
       </c>
     </row>
     <row r="177" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A177" s="21">
-        <v>2025</v>
-      </c>
-      <c r="B177" s="20">
+      <c r="A177">
+        <v>2025</v>
+      </c>
+      <c r="B177" s="1">
         <v>45915</v>
       </c>
       <c r="C177" s="16">
         <v>4.5100000000000001E-2</v>
       </c>
-      <c r="D177" s="19">
+      <c r="D177" s="6">
         <v>4.2200000000000001E-2</v>
       </c>
-      <c r="E177" s="19">
+      <c r="E177" s="6">
         <v>4.0599999999999997E-2</v>
       </c>
-      <c r="F177" s="19">
+      <c r="F177" s="6">
         <v>3.8100000000000002E-2</v>
       </c>
-      <c r="G177" s="19">
+      <c r="G177" s="6">
         <v>3.6400000000000002E-2</v>
       </c>
-      <c r="H177" s="19">
+      <c r="H177" s="6">
         <v>3.5400000000000001E-2</v>
       </c>
-      <c r="I177" s="19">
+      <c r="I177" s="6">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="J177" s="19">
+      <c r="J177" s="6">
         <v>3.61E-2</v>
       </c>
-      <c r="K177" s="19">
+      <c r="K177" s="6">
         <v>3.7900000000000003E-2</v>
       </c>
-      <c r="L177" s="19">
+      <c r="L177" s="6">
         <v>4.0500000000000001E-2</v>
       </c>
-      <c r="M177" s="19">
+      <c r="M177" s="6">
         <v>4.6300000000000001E-2</v>
       </c>
-      <c r="N177" s="19">
+      <c r="N177" s="6">
         <v>4.6600000000000003E-2</v>
       </c>
     </row>
     <row r="178" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A178" s="21">
-        <v>2025</v>
-      </c>
-      <c r="B178" s="20">
+      <c r="A178">
+        <v>2025</v>
+      </c>
+      <c r="B178" s="1">
         <v>45916</v>
       </c>
       <c r="C178" s="16">
         <v>4.3900000000000002E-2</v>
       </c>
-      <c r="D178" s="19">
+      <c r="D178" s="6">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="E178" s="19">
+      <c r="E178" s="6">
         <v>4.0399999999999998E-2</v>
       </c>
-      <c r="F178" s="19">
+      <c r="F178" s="6">
         <v>3.8100000000000002E-2</v>
       </c>
-      <c r="G178" s="19">
+      <c r="G178" s="6">
         <v>3.6200000000000003E-2</v>
       </c>
-      <c r="H178" s="19">
+      <c r="H178" s="6">
         <v>3.5099999999999999E-2</v>
       </c>
-      <c r="I178" s="19">
+      <c r="I178" s="6">
         <v>3.4700000000000002E-2</v>
       </c>
-      <c r="J178" s="19">
+      <c r="J178" s="6">
         <v>3.5900000000000001E-2</v>
       </c>
-      <c r="K178" s="19">
+      <c r="K178" s="6">
         <v>3.78E-2</v>
       </c>
-      <c r="L178" s="19">
+      <c r="L178" s="6">
         <v>4.0399999999999998E-2</v>
       </c>
-      <c r="M178" s="19">
+      <c r="M178" s="6">
         <v>4.6100000000000002E-2</v>
       </c>
-      <c r="N178" s="19">
+      <c r="N178" s="6">
         <v>4.65E-2</v>
       </c>
     </row>
     <row r="179" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A179" s="21">
-        <v>2025</v>
-      </c>
-      <c r="B179" s="20">
+      <c r="A179">
+        <v>2025</v>
+      </c>
+      <c r="B179" s="1">
         <v>45917</v>
       </c>
       <c r="C179" s="16">
         <v>4.3799999999999999E-2</v>
       </c>
-      <c r="D179" s="19">
+      <c r="D179" s="6">
         <v>4.1700000000000001E-2</v>
       </c>
-      <c r="E179" s="19">
+      <c r="E179" s="6">
         <v>4.02E-2</v>
       </c>
-      <c r="F179" s="19">
+      <c r="F179" s="6">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="G179" s="19">
+      <c r="G179" s="6">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="H179" s="19">
+      <c r="H179" s="6">
         <v>3.5200000000000002E-2</v>
       </c>
-      <c r="I179" s="19">
+      <c r="I179" s="6">
         <v>3.5099999999999999E-2</v>
       </c>
-      <c r="J179" s="19">
+      <c r="J179" s="6">
         <v>3.6200000000000003E-2</v>
       </c>
-      <c r="K179" s="19">
+      <c r="K179" s="6">
         <v>3.8100000000000002E-2</v>
       </c>
-      <c r="L179" s="19">
+      <c r="L179" s="6">
         <v>4.0599999999999997E-2</v>
       </c>
-      <c r="M179" s="19">
+      <c r="M179" s="6">
         <v>4.6199999999999998E-2</v>
       </c>
-      <c r="N179" s="19">
+      <c r="N179" s="6">
         <v>4.6600000000000003E-2</v>
       </c>
     </row>
     <row r="180" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A180" s="21">
-        <v>2025</v>
-      </c>
-      <c r="B180" s="20">
+      <c r="A180">
+        <v>2025</v>
+      </c>
+      <c r="B180" s="1">
         <v>45918</v>
       </c>
-      <c r="C180" s="18">
+      <c r="C180" s="17">
         <v>4.1399999999999999E-2</v>
       </c>
-      <c r="D180" s="17">
+      <c r="D180" s="6">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="E180" s="17">
+      <c r="E180" s="6">
         <v>4.0300000000000002E-2</v>
       </c>
-      <c r="F180" s="17">
+      <c r="F180" s="6">
         <v>3.8100000000000002E-2</v>
       </c>
-      <c r="G180" s="17">
+      <c r="G180" s="6">
         <v>3.61E-2</v>
       </c>
-      <c r="H180" s="17">
+      <c r="H180" s="6">
         <v>3.5700000000000003E-2</v>
       </c>
-      <c r="I180" s="17">
+      <c r="I180" s="6">
         <v>3.5499999999999997E-2</v>
       </c>
-      <c r="J180" s="17">
+      <c r="J180" s="6">
         <v>3.6700000000000003E-2</v>
       </c>
-      <c r="K180" s="17">
+      <c r="K180" s="6">
         <v>3.8600000000000002E-2</v>
       </c>
-      <c r="L180" s="17">
+      <c r="L180" s="6">
         <v>4.1099999999999998E-2</v>
       </c>
-      <c r="M180" s="17">
+      <c r="M180" s="6">
         <v>4.6800000000000001E-2</v>
       </c>
-      <c r="N180" s="17">
+      <c r="N180" s="6">
         <v>4.7199999999999999E-2</v>
       </c>
     </row>
@@ -14662,19 +14652,19 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="22">
-        <v>2025</v>
-      </c>
-      <c r="B23" s="23">
+      <c r="A23">
+        <v>2025</v>
+      </c>
+      <c r="B23" s="1">
         <v>45902</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23">
         <v>45295.80859375</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23">
         <v>6415.5400390625</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23">
         <v>21279.630859375</v>
       </c>
       <c r="F23" s="7">
@@ -14691,19 +14681,19 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="22">
-        <v>2025</v>
-      </c>
-      <c r="B24" s="23">
+      <c r="A24">
+        <v>2025</v>
+      </c>
+      <c r="B24" s="1">
         <v>45903</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24">
         <v>45271.23046875</v>
       </c>
-      <c r="D24" s="22">
+      <c r="D24">
         <v>6448.259765625</v>
       </c>
-      <c r="E24" s="22">
+      <c r="E24">
         <v>21497.73046875</v>
       </c>
       <c r="F24" s="7">
@@ -14720,19 +14710,19 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="22">
-        <v>2025</v>
-      </c>
-      <c r="B25" s="23">
+      <c r="A25">
+        <v>2025</v>
+      </c>
+      <c r="B25" s="1">
         <v>45904</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25">
         <v>45621.2890625</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25">
         <v>6502.080078125</v>
       </c>
-      <c r="E25" s="22">
+      <c r="E25">
         <v>21707.689453125</v>
       </c>
       <c r="F25" s="7">
@@ -14749,19 +14739,19 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="22">
-        <v>2025</v>
-      </c>
-      <c r="B26" s="23">
+      <c r="A26">
+        <v>2025</v>
+      </c>
+      <c r="B26" s="1">
         <v>45905</v>
       </c>
-      <c r="C26" s="22">
+      <c r="C26">
         <v>45400.859375</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26">
         <v>6481.5</v>
       </c>
-      <c r="E26" s="22">
+      <c r="E26">
         <v>21700.390625</v>
       </c>
       <c r="F26" s="7">
@@ -14778,19 +14768,19 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="22">
-        <v>2025</v>
-      </c>
-      <c r="B27" s="23">
+      <c r="A27">
+        <v>2025</v>
+      </c>
+      <c r="B27" s="1">
         <v>45908</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C27">
         <v>45514.94921875</v>
       </c>
-      <c r="D27" s="22">
+      <c r="D27">
         <v>6495.14990234375</v>
       </c>
-      <c r="E27" s="22">
+      <c r="E27">
         <v>21798.69921875</v>
       </c>
       <c r="F27" s="7">
@@ -14807,19 +14797,19 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="22">
-        <v>2025</v>
-      </c>
-      <c r="B28" s="23">
+      <c r="A28">
+        <v>2025</v>
+      </c>
+      <c r="B28" s="1">
         <v>45909</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28">
         <v>45711.33984375</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D28">
         <v>6512.60986328125</v>
       </c>
-      <c r="E28" s="22">
+      <c r="E28">
         <v>21879.490234375</v>
       </c>
       <c r="F28" s="7">
@@ -14836,19 +14826,19 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="22">
-        <v>2025</v>
-      </c>
-      <c r="B29" s="23">
+      <c r="A29">
+        <v>2025</v>
+      </c>
+      <c r="B29" s="1">
         <v>45910</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C29">
         <v>45490.921875</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29">
         <v>6532.0400390625</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E29">
         <v>21886.060546875</v>
       </c>
       <c r="F29" s="7">
@@ -14865,19 +14855,19 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="22">
-        <v>2025</v>
-      </c>
-      <c r="B30" s="23">
+      <c r="A30">
+        <v>2025</v>
+      </c>
+      <c r="B30" s="1">
         <v>45911</v>
       </c>
-      <c r="C30" s="22">
+      <c r="C30">
         <v>46108</v>
       </c>
-      <c r="D30" s="22">
+      <c r="D30">
         <v>6587.47021484375</v>
       </c>
-      <c r="E30" s="22">
+      <c r="E30">
         <v>22043.0703125</v>
       </c>
       <c r="F30" s="7">
@@ -14894,19 +14884,19 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="22">
-        <v>2025</v>
-      </c>
-      <c r="B31" s="23">
+      <c r="A31">
+        <v>2025</v>
+      </c>
+      <c r="B31" s="1">
         <v>45912</v>
       </c>
-      <c r="C31" s="22">
+      <c r="C31">
         <v>45834.21875</v>
       </c>
-      <c r="D31" s="22">
+      <c r="D31">
         <v>6584.2900390625</v>
       </c>
-      <c r="E31" s="22">
+      <c r="E31">
         <v>22141.099609375</v>
       </c>
       <c r="F31" s="7">
@@ -14923,19 +14913,19 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="22">
-        <v>2025</v>
-      </c>
-      <c r="B32" s="23">
+      <c r="A32">
+        <v>2025</v>
+      </c>
+      <c r="B32" s="1">
         <v>45915</v>
       </c>
-      <c r="C32" s="22">
+      <c r="C32">
         <v>45883.44921875</v>
       </c>
-      <c r="D32" s="22">
+      <c r="D32">
         <v>6615.27978515625</v>
       </c>
-      <c r="E32" s="22">
+      <c r="E32">
         <v>22348.75</v>
       </c>
       <c r="F32" s="7">
@@ -14952,19 +14942,19 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="22">
-        <v>2025</v>
-      </c>
-      <c r="B33" s="23">
+      <c r="A33">
+        <v>2025</v>
+      </c>
+      <c r="B33" s="1">
         <v>45916</v>
       </c>
-      <c r="C33" s="22">
+      <c r="C33">
         <v>45757.8984375</v>
       </c>
-      <c r="D33" s="22">
+      <c r="D33">
         <v>6606.759765625</v>
       </c>
-      <c r="E33" s="22">
+      <c r="E33">
         <v>22333.9609375</v>
       </c>
       <c r="F33" s="7">
@@ -14981,19 +14971,19 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="22">
-        <v>2025</v>
-      </c>
-      <c r="B34" s="23">
+      <c r="A34">
+        <v>2025</v>
+      </c>
+      <c r="B34" s="1">
         <v>45917</v>
       </c>
-      <c r="C34" s="22">
+      <c r="C34">
         <v>46018.3203125</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34">
         <v>6600.35009765625</v>
       </c>
-      <c r="E34" s="22">
+      <c r="E34">
         <v>22261.330078125</v>
       </c>
       <c r="F34" s="7">
@@ -15010,19 +15000,19 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="22">
-        <v>2025</v>
-      </c>
-      <c r="B35" s="23">
+      <c r="A35">
+        <v>2025</v>
+      </c>
+      <c r="B35" s="1">
         <v>45918</v>
       </c>
-      <c r="C35" s="22">
+      <c r="C35">
         <v>46142.421875</v>
       </c>
-      <c r="D35" s="22">
+      <c r="D35">
         <v>6631.9599609375</v>
       </c>
-      <c r="E35" s="22">
+      <c r="E35">
         <v>22470.720703125</v>
       </c>
       <c r="F35" s="7">
@@ -15039,19 +15029,19 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="22">
-        <v>2025</v>
-      </c>
-      <c r="B36" s="23">
+      <c r="A36">
+        <v>2025</v>
+      </c>
+      <c r="B36" s="1">
         <v>45919</v>
       </c>
-      <c r="C36" s="22">
+      <c r="C36">
         <v>46315.26953125</v>
       </c>
-      <c r="D36" s="22">
+      <c r="D36">
         <v>6664.35986328125</v>
       </c>
-      <c r="E36" s="22">
+      <c r="E36">
         <v>22631.48046875</v>
       </c>
       <c r="F36" s="7">
@@ -15223,744 +15213,900 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE3EAA2-8F6D-45D1-94CD-1021786505AF}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2025</v>
+      </c>
+      <c r="B2" s="1">
         <v>45870</v>
       </c>
-      <c r="B2" s="7">
+      <c r="C2" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C2" s="7">
+      <c r="D2" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D2" s="7">
+      <c r="E2" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3" s="1">
         <v>45871</v>
       </c>
-      <c r="B3" s="7">
+      <c r="C3" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C3" s="7">
+      <c r="D3" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D3" s="7">
+      <c r="E3" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2025</v>
+      </c>
+      <c r="B4" s="1">
         <v>45872</v>
       </c>
-      <c r="B4" s="7">
+      <c r="C4" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C4" s="7">
+      <c r="D4" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D4" s="7">
+      <c r="E4" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2025</v>
+      </c>
+      <c r="B5" s="1">
         <v>45873</v>
       </c>
-      <c r="B5" s="7">
+      <c r="C5" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C5" s="7">
+      <c r="D5" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D5" s="7">
+      <c r="E5" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2025</v>
+      </c>
+      <c r="B6" s="1">
         <v>45874</v>
       </c>
-      <c r="B6" s="7">
+      <c r="C6" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C6" s="7">
+      <c r="D6" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D6" s="7">
+      <c r="E6" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2025</v>
+      </c>
+      <c r="B7" s="1">
         <v>45875</v>
       </c>
-      <c r="B7" s="7">
+      <c r="C7" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C7" s="7">
+      <c r="D7" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D7" s="7">
+      <c r="E7" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2025</v>
+      </c>
+      <c r="B8" s="1">
         <v>45876</v>
       </c>
-      <c r="B8" s="7">
+      <c r="C8" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C8" s="7">
+      <c r="D8" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D8" s="7">
+      <c r="E8" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2025</v>
+      </c>
+      <c r="B9" s="1">
         <v>45877</v>
       </c>
-      <c r="B9" s="7">
+      <c r="C9" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C9" s="7">
+      <c r="D9" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D9" s="7">
+      <c r="E9" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2025</v>
+      </c>
+      <c r="B10" s="1">
         <v>45878</v>
       </c>
-      <c r="B10" s="7">
+      <c r="C10" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C10" s="7">
+      <c r="D10" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D10" s="7">
+      <c r="E10" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2025</v>
+      </c>
+      <c r="B11" s="1">
         <v>45879</v>
       </c>
-      <c r="B11" s="7">
+      <c r="C11" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C11" s="7">
+      <c r="D11" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D11" s="7">
+      <c r="E11" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2025</v>
+      </c>
+      <c r="B12" s="1">
         <v>45880</v>
       </c>
-      <c r="B12" s="7">
+      <c r="C12" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C12" s="7">
+      <c r="D12" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D12" s="7">
+      <c r="E12" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2025</v>
+      </c>
+      <c r="B13" s="1">
         <v>45881</v>
       </c>
-      <c r="B13" s="7">
+      <c r="C13" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C13" s="7">
+      <c r="D13" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D13" s="7">
+      <c r="E13" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2025</v>
+      </c>
+      <c r="B14" s="1">
         <v>45882</v>
       </c>
-      <c r="B14" s="7">
+      <c r="C14" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C14" s="7">
+      <c r="D14" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D14" s="7">
+      <c r="E14" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2025</v>
+      </c>
+      <c r="B15" s="1">
         <v>45883</v>
       </c>
-      <c r="B15" s="7">
+      <c r="C15" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C15" s="7">
+      <c r="D15" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D15" s="7">
+      <c r="E15" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2025</v>
+      </c>
+      <c r="B16" s="1">
         <v>45884</v>
       </c>
-      <c r="B16" s="7">
+      <c r="C16" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C16" s="7">
+      <c r="D16" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D16" s="7">
+      <c r="E16" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2025</v>
+      </c>
+      <c r="B17" s="1">
         <v>45885</v>
       </c>
-      <c r="B17" s="7">
+      <c r="C17" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C17" s="7">
+      <c r="D17" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D17" s="7">
+      <c r="E17" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2025</v>
+      </c>
+      <c r="B18" s="1">
         <v>45886</v>
       </c>
-      <c r="B18" s="7">
+      <c r="C18" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C18" s="7">
+      <c r="D18" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D18" s="7">
+      <c r="E18" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2025</v>
+      </c>
+      <c r="B19" s="1">
         <v>45887</v>
       </c>
-      <c r="B19" s="7">
+      <c r="C19" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C19" s="7">
+      <c r="D19" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D19" s="7">
+      <c r="E19" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2025</v>
+      </c>
+      <c r="B20" s="1">
         <v>45888</v>
       </c>
-      <c r="B20" s="7">
+      <c r="C20" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C20" s="7">
+      <c r="D20" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D20" s="7">
+      <c r="E20" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2025</v>
+      </c>
+      <c r="B21" s="1">
         <v>45889</v>
       </c>
-      <c r="B21" s="7">
+      <c r="C21" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C21" s="7">
+      <c r="D21" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D21" s="7">
+      <c r="E21" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2025</v>
+      </c>
+      <c r="B22" s="1">
         <v>45890</v>
       </c>
-      <c r="B22" s="7">
+      <c r="C22" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C22" s="7">
+      <c r="D22" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D22" s="7">
+      <c r="E22" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2025</v>
+      </c>
+      <c r="B23" s="1">
         <v>45891</v>
       </c>
-      <c r="B23" s="7">
+      <c r="C23" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C23" s="7">
+      <c r="D23" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D23" s="7">
+      <c r="E23" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2025</v>
+      </c>
+      <c r="B24" s="1">
         <v>45892</v>
       </c>
-      <c r="B24" s="7">
+      <c r="C24" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C24" s="7">
+      <c r="D24" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D24" s="7">
+      <c r="E24" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2025</v>
+      </c>
+      <c r="B25" s="1">
         <v>45893</v>
       </c>
-      <c r="B25" s="7">
+      <c r="C25" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C25" s="7">
+      <c r="D25" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D25" s="7">
+      <c r="E25" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2025</v>
+      </c>
+      <c r="B26" s="1">
         <v>45894</v>
       </c>
-      <c r="B26" s="7">
+      <c r="C26" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C26" s="7">
+      <c r="D26" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D26" s="7">
+      <c r="E26" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2025</v>
+      </c>
+      <c r="B27" s="1">
         <v>45895</v>
       </c>
-      <c r="B27" s="7">
+      <c r="C27" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C27" s="7">
+      <c r="D27" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D27" s="7">
+      <c r="E27" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2025</v>
+      </c>
+      <c r="B28" s="1">
         <v>45896</v>
       </c>
-      <c r="B28" s="7">
+      <c r="C28" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C28" s="7">
+      <c r="D28" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D28" s="7">
+      <c r="E28" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2025</v>
+      </c>
+      <c r="B29" s="1">
         <v>45897</v>
       </c>
-      <c r="B29" s="7">
+      <c r="C29" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C29" s="7">
+      <c r="D29" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D29" s="7">
+      <c r="E29" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2025</v>
+      </c>
+      <c r="B30" s="1">
         <v>45898</v>
       </c>
-      <c r="B30" s="7">
+      <c r="C30" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C30" s="7">
+      <c r="D30" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D30" s="7">
+      <c r="E30" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2025</v>
+      </c>
+      <c r="B31" s="1">
         <v>45899</v>
       </c>
-      <c r="B31" s="7">
+      <c r="C31" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C31" s="7">
+      <c r="D31" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D31" s="7">
+      <c r="E31" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2025</v>
+      </c>
+      <c r="B32" s="1">
         <v>45900</v>
       </c>
-      <c r="B32" s="7">
+      <c r="C32" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C32" s="7">
+      <c r="D32" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D32" s="7">
+      <c r="E32" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2025</v>
+      </c>
+      <c r="B33" s="1">
         <v>45901</v>
       </c>
-      <c r="B33" s="7">
+      <c r="C33" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C33" s="7">
+      <c r="D33" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D33" s="7">
+      <c r="E33" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>2025</v>
+      </c>
+      <c r="B34" s="1">
         <v>45902</v>
       </c>
-      <c r="B34" s="7">
+      <c r="C34" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C34" s="7">
+      <c r="D34" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D34" s="7">
+      <c r="E34" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>2025</v>
+      </c>
+      <c r="B35" s="1">
         <v>45903</v>
       </c>
-      <c r="B35" s="7">
+      <c r="C35" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C35" s="7">
+      <c r="D35" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D35" s="7">
+      <c r="E35" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>2025</v>
+      </c>
+      <c r="B36" s="1">
         <v>45904</v>
       </c>
-      <c r="B36" s="7">
+      <c r="C36" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C36" s="7">
+      <c r="D36" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D36" s="7">
+      <c r="E36" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>2025</v>
+      </c>
+      <c r="B37" s="1">
         <v>45905</v>
       </c>
-      <c r="B37" s="7">
+      <c r="C37" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C37" s="7">
+      <c r="D37" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D37" s="7">
+      <c r="E37" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2025</v>
+      </c>
+      <c r="B38" s="1">
         <v>45906</v>
       </c>
-      <c r="B38" s="7">
+      <c r="C38" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C38" s="7">
+      <c r="D38" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D38" s="7">
+      <c r="E38" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>2025</v>
+      </c>
+      <c r="B39" s="1">
         <v>45907</v>
       </c>
-      <c r="B39" s="7">
+      <c r="C39" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C39" s="7">
+      <c r="D39" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D39" s="7">
+      <c r="E39" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>2025</v>
+      </c>
+      <c r="B40" s="1">
         <v>45908</v>
       </c>
-      <c r="B40" s="7">
+      <c r="C40" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C40" s="7">
+      <c r="D40" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D40" s="7">
+      <c r="E40" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>2025</v>
+      </c>
+      <c r="B41" s="1">
         <v>45909</v>
       </c>
-      <c r="B41" s="7">
+      <c r="C41" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C41" s="7">
+      <c r="D41" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D41" s="7">
+      <c r="E41" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>2025</v>
+      </c>
+      <c r="B42" s="1">
         <v>45910</v>
       </c>
-      <c r="B42" s="7">
+      <c r="C42" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C42" s="7">
+      <c r="D42" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D42" s="7">
+      <c r="E42" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>2025</v>
+      </c>
+      <c r="B43" s="1">
         <v>45911</v>
       </c>
-      <c r="B43" s="7">
+      <c r="C43" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C43" s="7">
+      <c r="D43" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D43" s="7">
+      <c r="E43" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>2025</v>
+      </c>
+      <c r="B44" s="1">
         <v>45912</v>
       </c>
-      <c r="B44" s="7">
+      <c r="C44" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C44" s="7">
+      <c r="D44" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D44" s="7">
+      <c r="E44" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="1">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>2025</v>
+      </c>
+      <c r="B45" s="1">
         <v>45913</v>
       </c>
-      <c r="B45" s="7">
+      <c r="C45" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C45" s="7">
+      <c r="D45" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D45" s="7">
+      <c r="E45" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>2025</v>
+      </c>
+      <c r="B46" s="1">
         <v>45914</v>
       </c>
-      <c r="B46" s="7">
+      <c r="C46" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C46" s="7">
+      <c r="D46" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D46" s="7">
+      <c r="E46" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>2025</v>
+      </c>
+      <c r="B47" s="1">
         <v>45915</v>
       </c>
-      <c r="B47" s="7">
+      <c r="C47" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C47" s="7">
+      <c r="D47" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D47" s="7">
+      <c r="E47" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>2025</v>
+      </c>
+      <c r="B48" s="1">
         <v>45916</v>
       </c>
-      <c r="B48" s="7">
+      <c r="C48" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C48" s="7">
+      <c r="D48" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D48" s="7">
+      <c r="E48" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>2025</v>
+      </c>
+      <c r="B49" s="1">
         <v>45917</v>
       </c>
-      <c r="B49" s="7">
+      <c r="C49" s="7">
         <v>4.3299999999999998E-2</v>
       </c>
-      <c r="C49" s="7">
+      <c r="D49" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D49" s="7">
+      <c r="E49" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="1">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>2025</v>
+      </c>
+      <c r="B50" s="1">
         <v>45918</v>
       </c>
-      <c r="B50" s="7">
+      <c r="C50" s="7">
         <v>4.0800000000000003E-2</v>
       </c>
-      <c r="C50" s="7">
+      <c r="D50" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
-      <c r="D50" s="7">
+      <c r="E50" s="7">
         <v>0.04</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>2025</v>
+      </c>
+      <c r="B51" s="1">
         <v>45919</v>
       </c>
-      <c r="B51" s="7">
+      <c r="C51" s="7">
         <v>4.0800000000000003E-2</v>
       </c>
-      <c r="C51" s="7">
+      <c r="D51" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
-      <c r="D51" s="7">
+      <c r="E51" s="7">
         <v>0.04</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="1">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>2025</v>
+      </c>
+      <c r="B52" s="1">
         <v>45920</v>
       </c>
-      <c r="B52" s="7">
+      <c r="C52" s="7">
         <v>4.0800000000000003E-2</v>
       </c>
-      <c r="C52" s="7">
+      <c r="D52" s="7">
         <v>4.2500000000000003E-2</v>
       </c>
-      <c r="D52" s="7">
+      <c r="E52" s="7">
         <v>0.04</v>
       </c>
     </row>

</xml_diff>

<commit_message>
agregar tasas de interés US_v8
</commit_message>
<xml_diff>
--- a/tipo de cambio y tasas de interés.xlsx
+++ b/tipo de cambio y tasas de interés.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA52D60-F3A9-4587-9EFF-B7C827993408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FB27AC-70BC-4F45-8061-DD0BCC0E3522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="7" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo de Cambio" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>Año</t>
-  </si>
-  <si>
-    <t>Tasa de Interés Objetivo</t>
   </si>
   <si>
     <t>TIIE 28 días</t>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>Tasa efectiva FED</t>
+  </si>
+  <si>
+    <t>Tasa de Interés Objetivo Banxico</t>
   </si>
 </sst>
 </file>
@@ -945,7 +945,7 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B700B119-8C38-4F55-BC79-C4D6BC8E0C88}" name="Año"/>
     <tableColumn id="2" xr3:uid="{47E09E7D-A904-4405-9048-49D33EE0E8EB}" name="Fecha" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{0E168449-32EF-450B-812C-11DC4F0F3A30}" name="Tasa de Interés Objetivo"/>
+    <tableColumn id="3" xr3:uid="{0E168449-32EF-450B-812C-11DC4F0F3A30}" name="Tasa de Interés Objetivo Banxico"/>
     <tableColumn id="4" xr3:uid="{EE5A2D13-088C-4226-A754-1A001EC14095}" name="TIIE 28 días"/>
     <tableColumn id="5" xr3:uid="{91C093C9-2029-4DE0-AF73-BB6DB79C251D}" name="TIIE 91 días"/>
     <tableColumn id="6" xr3:uid="{B133AA74-E94C-4608-8061-B6BA564978B5}" name="TIIE 182 días"/>
@@ -1321,10 +1321,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2648,8 +2648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394FE10B-CC5B-4887-BA9F-8638E71CB003}">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2667,16 +2667,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -4231,40 +4231,40 @@
         <v>0</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>19</v>
-      </c>
-      <c r="N1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -12169,7 +12169,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -14024,22 +14024,22 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>25</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -15087,10 +15087,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -15158,10 +15158,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -15215,8 +15215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE3EAA2-8F6D-45D1-94CD-1021786505AF}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15234,13 +15234,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
         <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajuste del código para que aguante los nuevos títulos de inflación
</commit_message>
<xml_diff>
--- a/tipo de cambio y tasas de interés.xlsx
+++ b/tipo de cambio y tasas de interés.xlsx
@@ -8,29 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FB27AC-70BC-4F45-8061-DD0BCC0E3522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83571F13-E270-4D28-8E79-DEAC2E96336F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo de Cambio" sheetId="1" r:id="rId1"/>
-    <sheet name="Tasas de interés" sheetId="2" r:id="rId2"/>
-    <sheet name="Treasuries_SOFR" sheetId="3" r:id="rId3"/>
-    <sheet name="SOFR" sheetId="7" r:id="rId4"/>
-    <sheet name="Wallstreet" sheetId="6" r:id="rId5"/>
-    <sheet name="InflaciónUS" sheetId="4" r:id="rId6"/>
-    <sheet name="InflaciónMEX" sheetId="10" r:id="rId7"/>
-    <sheet name="Tasas de interés US" sheetId="13" r:id="rId8"/>
+    <sheet name="Tasas de interés2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tasas de interés" sheetId="14" r:id="rId3"/>
+    <sheet name="Treasuries_SOFR" sheetId="3" r:id="rId4"/>
+    <sheet name="SOFR" sheetId="7" r:id="rId5"/>
+    <sheet name="Wallstreet" sheetId="6" r:id="rId6"/>
+    <sheet name="InflaciónUS" sheetId="4" r:id="rId7"/>
+    <sheet name="InflaciónMEX" sheetId="10" r:id="rId8"/>
+    <sheet name="Tasas de interés US" sheetId="13" r:id="rId9"/>
+    <sheet name="Tasas de interés US2" sheetId="15" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Tasas de interés'!$D$1:$F$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Tasas de interés2'!$D$1:$F$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>Fecha</t>
   </si>
@@ -126,6 +128,12 @@
   </si>
   <si>
     <t>Tasa de Interés Objetivo Banxico</t>
+  </si>
+  <si>
+    <t>Tasa de Interés Objetivo</t>
+  </si>
+  <si>
+    <t>Tasa efectiva de fondos federales</t>
   </si>
 </sst>
 </file>
@@ -770,7 +778,10 @@
     <cellStyle name="Título 3" xfId="6" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="19" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="24">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -926,14 +937,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}" name="Tabla1" displayName="Tabla1" ref="A1:E78" totalsRowShown="0" dataDxfId="22" dataCellStyle="Moneda">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}" name="Tabla1" displayName="Tabla1" ref="A1:E78" totalsRowShown="0" dataDxfId="23" dataCellStyle="Moneda">
   <autoFilter ref="A1:E78" xr:uid="{89FEBF79-34BE-422C-9B3B-1ABEB5D5A6E9}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8E09B427-5E44-4BBB-89FC-35463079BE46}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{3D7466AA-D045-44D9-96B5-BDFB7062F58C}" name="Fecha" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{157C7180-B5CE-4C51-9BD0-3AEECF3B91F1}" name="Tipo de Cambio FIX" dataDxfId="20" dataCellStyle="Moneda"/>
-    <tableColumn id="4" xr3:uid="{74B4BBBC-E72A-423F-B8FA-CE596B4E990E}" name="Nivel máximo" dataDxfId="19" dataCellStyle="Moneda"/>
-    <tableColumn id="5" xr3:uid="{74EB6E0A-1398-4291-8596-80BA6140571D}" name="Nivel mínimo" dataDxfId="18" dataCellStyle="Moneda"/>
+    <tableColumn id="2" xr3:uid="{3D7466AA-D045-44D9-96B5-BDFB7062F58C}" name="Fecha" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{157C7180-B5CE-4C51-9BD0-3AEECF3B91F1}" name="Tipo de Cambio FIX" dataDxfId="21" dataCellStyle="Moneda"/>
+    <tableColumn id="4" xr3:uid="{74B4BBBC-E72A-423F-B8FA-CE596B4E990E}" name="Nivel máximo" dataDxfId="20" dataCellStyle="Moneda"/>
+    <tableColumn id="5" xr3:uid="{74EB6E0A-1398-4291-8596-80BA6140571D}" name="Nivel mínimo" dataDxfId="19" dataCellStyle="Moneda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -944,8 +955,8 @@
   <autoFilter ref="A1:F77" xr:uid="{F4FA084B-10DE-49EA-A77A-CF0EB874CD28}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B700B119-8C38-4F55-BC79-C4D6BC8E0C88}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{47E09E7D-A904-4405-9048-49D33EE0E8EB}" name="Fecha" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{0E168449-32EF-450B-812C-11DC4F0F3A30}" name="Tasa de Interés Objetivo Banxico"/>
+    <tableColumn id="2" xr3:uid="{47E09E7D-A904-4405-9048-49D33EE0E8EB}" name="Fecha" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{0E168449-32EF-450B-812C-11DC4F0F3A30}" name="Tasa de Interés Objetivo"/>
     <tableColumn id="4" xr3:uid="{EE5A2D13-088C-4226-A754-1A001EC14095}" name="TIIE 28 días"/>
     <tableColumn id="5" xr3:uid="{91C093C9-2029-4DE0-AF73-BB6DB79C251D}" name="TIIE 91 días"/>
     <tableColumn id="6" xr3:uid="{B133AA74-E94C-4608-8061-B6BA564978B5}" name="TIIE 182 días"/>
@@ -955,44 +966,59 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{41D25D3A-81CA-4450-B7DF-F71343E59E89}" name="Tabla7" displayName="Tabla7" ref="A1:N180" totalsRowShown="0">
-  <autoFilter ref="A1:N180" xr:uid="{41D25D3A-81CA-4450-B7DF-F71343E59E89}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{4B709A46-FEF4-4082-A1C7-4443452E16C3}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{288E25E9-721A-4984-9062-39446AEF10A2}" name="Fecha" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{B14E5478-3494-4D1C-8F7A-C3666CA59C27}" name="SOFR" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{BA101BB9-5BDD-49C2-A01D-82F8C1F40DE3}" name="1M Treasury" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{7FE75A9A-7044-4B06-B3A6-F01D3A56E2C5}" name="3M Treasury" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{602D7FBF-E731-4F49-9A0B-6365C780F089}" name="6M Treasury" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{7887EB81-463F-4BB8-9E84-4229D2CAC9A1}" name="1Y Treasury" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{8C5475BF-3FF2-497D-B569-0B378CC77D79}" name="2Y Treasury" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{3B424ABE-EF8F-498A-8F4F-7FDBD990A429}" name="3Y Treasury" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{383F89E5-27BF-4792-BA7B-6E4263B946C9}" name="5Y Treasury" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{A94CC5AD-A6E2-4E44-AAAF-147E46B23BA1}" name="7Y Treasury" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{BA073A53-DD09-4842-A47E-B2F4D2CD2F0B}" name="10Y Treasury" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{0AB1292E-1821-4704-ACB3-22F12D9A1EBD}" name="20Y Treasury" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{FCEEF9DA-C290-458F-AEF1-C46CBE6DCD16}" name="30Y Treasury" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4E717856-AEC4-4D15-83FE-EF067029218F}" name="Tabla24" displayName="Tabla24" ref="A1:F77" totalsRowShown="0">
+  <autoFilter ref="A1:F77" xr:uid="{4E717856-AEC4-4D15-83FE-EF067029218F}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{2E0B3A81-10BF-4919-93D3-DFCB7943009F}" name="Año"/>
+    <tableColumn id="2" xr3:uid="{4DDFFDA1-F291-46D8-8D65-F7040EF322C5}" name="Fecha" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{772F16E4-347C-44C5-ACC4-C16C0185C7B0}" name="Tasa de Interés Objetivo Banxico"/>
+    <tableColumn id="4" xr3:uid="{5355F4FC-28EC-4FFA-B3F8-C7F7D2ED6257}" name="TIIE 28 días"/>
+    <tableColumn id="5" xr3:uid="{8F2A0142-D5F1-4DBA-99E4-CD6E3D7E7363}" name="TIIE 91 días"/>
+    <tableColumn id="6" xr3:uid="{2B99450C-C287-476E-A955-BBFEB6F07E36}" name="TIIE 182 días"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{41D25D3A-81CA-4450-B7DF-F71343E59E89}" name="Tabla7" displayName="Tabla7" ref="A1:N180" totalsRowShown="0">
+  <autoFilter ref="A1:N180" xr:uid="{41D25D3A-81CA-4450-B7DF-F71343E59E89}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{4B709A46-FEF4-4082-A1C7-4443452E16C3}" name="Año"/>
+    <tableColumn id="2" xr3:uid="{288E25E9-721A-4984-9062-39446AEF10A2}" name="Fecha" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{B14E5478-3494-4D1C-8F7A-C3666CA59C27}" name="SOFR" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{BA101BB9-5BDD-49C2-A01D-82F8C1F40DE3}" name="1M Treasury" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{7FE75A9A-7044-4B06-B3A6-F01D3A56E2C5}" name="3M Treasury" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{602D7FBF-E731-4F49-9A0B-6365C780F089}" name="6M Treasury" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{7887EB81-463F-4BB8-9E84-4229D2CAC9A1}" name="1Y Treasury" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{8C5475BF-3FF2-497D-B569-0B378CC77D79}" name="2Y Treasury" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{3B424ABE-EF8F-498A-8F4F-7FDBD990A429}" name="3Y Treasury" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{383F89E5-27BF-4792-BA7B-6E4263B946C9}" name="5Y Treasury" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{A94CC5AD-A6E2-4E44-AAAF-147E46B23BA1}" name="7Y Treasury" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{BA073A53-DD09-4842-A47E-B2F4D2CD2F0B}" name="10Y Treasury" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{0AB1292E-1821-4704-ACB3-22F12D9A1EBD}" name="20Y Treasury" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{FCEEF9DA-C290-458F-AEF1-C46CBE6DCD16}" name="30Y Treasury" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}" name="Tabla8" displayName="Tabla8" ref="A1:H36" totalsRowShown="0">
   <autoFilter ref="A1:H36" xr:uid="{E8483F90-A69D-4E36-9F78-F36E94A075B5}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{7676C863-947F-4296-8B2C-4C1C2493E9D9}" name="Año"/>
-    <tableColumn id="2" xr3:uid="{55C318C8-9926-4D62-8294-177D6BC0FE75}" name="Fecha" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{55C318C8-9926-4D62-8294-177D6BC0FE75}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{1D145B8D-1465-4EF3-BECF-49ACE623BEC5}" name="Dow Jones"/>
     <tableColumn id="4" xr3:uid="{F2357A84-5C07-4E65-841A-42DAECACF403}" name="S&amp;P 500"/>
     <tableColumn id="5" xr3:uid="{388751CA-0A21-4A09-8009-2BB8B01233CE}" name="Nasdaq"/>
-    <tableColumn id="6" xr3:uid="{DEF693B5-3B7C-424D-8BCC-52947BCEC3CF}" name="% Dow Jones" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{DEF693B5-3B7C-424D-8BCC-52947BCEC3CF}" name="% Dow Jones" dataDxfId="3">
       <calculatedColumnFormula>IFERROR((Tabla8[[#This Row],[Dow Jones]]-C1)/C1,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{A64DA0F4-44F9-4388-B98F-ED267001BCC9}" name="% S&amp;P500" dataDxfId="1">
+    <tableColumn id="7" xr3:uid="{A64DA0F4-44F9-4388-B98F-ED267001BCC9}" name="% S&amp;P500" dataDxfId="2">
       <calculatedColumnFormula>IFERROR((Tabla8[[#This Row],[S&amp;P 500]]-D1)/D1,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{9B8FC688-A5F6-4240-9AD9-64ED7FF46AD3}" name="% Nasdaq" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{9B8FC688-A5F6-4240-9AD9-64ED7FF46AD3}" name="% Nasdaq" dataDxfId="1">
       <calculatedColumnFormula>IFERROR((Tabla8[[#This Row],[Nasdaq]]-E1)/E1,"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2644,12 +2670,911 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB728CC-3545-439B-8305-CE331A9F0964}">
+  <dimension ref="A1:E52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2025</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45870</v>
+      </c>
+      <c r="C2" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D2" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E2" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45871</v>
+      </c>
+      <c r="C3" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D3" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E3" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2025</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45872</v>
+      </c>
+      <c r="C4" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D4" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E4" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2025</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45873</v>
+      </c>
+      <c r="C5" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D5" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E5" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2025</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45874</v>
+      </c>
+      <c r="C6" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D6" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E6" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2025</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45875</v>
+      </c>
+      <c r="C7" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D7" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E7" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2025</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45876</v>
+      </c>
+      <c r="C8" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D8" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E8" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2025</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45877</v>
+      </c>
+      <c r="C9" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D9" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E9" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2025</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45878</v>
+      </c>
+      <c r="C10" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D10" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E10" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2025</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45879</v>
+      </c>
+      <c r="C11" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D11" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E11" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2025</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45880</v>
+      </c>
+      <c r="C12" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D12" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E12" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2025</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45881</v>
+      </c>
+      <c r="C13" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D13" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E13" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2025</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45882</v>
+      </c>
+      <c r="C14" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D14" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E14" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2025</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45883</v>
+      </c>
+      <c r="C15" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D15" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E15" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2025</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45884</v>
+      </c>
+      <c r="C16" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D16" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E16" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2025</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45885</v>
+      </c>
+      <c r="C17" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D17" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E17" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2025</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45886</v>
+      </c>
+      <c r="C18" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D18" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E18" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2025</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45887</v>
+      </c>
+      <c r="C19" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D19" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E19" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2025</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45888</v>
+      </c>
+      <c r="C20" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D20" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E20" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2025</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45889</v>
+      </c>
+      <c r="C21" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D21" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E21" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2025</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45890</v>
+      </c>
+      <c r="C22" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D22" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E22" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2025</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45891</v>
+      </c>
+      <c r="C23" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D23" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E23" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2025</v>
+      </c>
+      <c r="B24" s="1">
+        <v>45892</v>
+      </c>
+      <c r="C24" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D24" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E24" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2025</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45893</v>
+      </c>
+      <c r="C25" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D25" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E25" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2025</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45894</v>
+      </c>
+      <c r="C26" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D26" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E26" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2025</v>
+      </c>
+      <c r="B27" s="1">
+        <v>45895</v>
+      </c>
+      <c r="C27" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D27" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E27" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2025</v>
+      </c>
+      <c r="B28" s="1">
+        <v>45896</v>
+      </c>
+      <c r="C28" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D28" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E28" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2025</v>
+      </c>
+      <c r="B29" s="1">
+        <v>45897</v>
+      </c>
+      <c r="C29" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D29" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E29" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2025</v>
+      </c>
+      <c r="B30" s="1">
+        <v>45898</v>
+      </c>
+      <c r="C30" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D30" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E30" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2025</v>
+      </c>
+      <c r="B31" s="1">
+        <v>45899</v>
+      </c>
+      <c r="C31" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D31" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E31" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2025</v>
+      </c>
+      <c r="B32" s="1">
+        <v>45900</v>
+      </c>
+      <c r="C32" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D32" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E32" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2025</v>
+      </c>
+      <c r="B33" s="1">
+        <v>45901</v>
+      </c>
+      <c r="C33" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D33" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E33" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>2025</v>
+      </c>
+      <c r="B34" s="1">
+        <v>45902</v>
+      </c>
+      <c r="C34" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D34" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E34" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>2025</v>
+      </c>
+      <c r="B35" s="1">
+        <v>45903</v>
+      </c>
+      <c r="C35" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D35" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E35" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>2025</v>
+      </c>
+      <c r="B36" s="1">
+        <v>45904</v>
+      </c>
+      <c r="C36" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D36" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E36" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>2025</v>
+      </c>
+      <c r="B37" s="1">
+        <v>45905</v>
+      </c>
+      <c r="C37" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D37" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E37" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2025</v>
+      </c>
+      <c r="B38" s="1">
+        <v>45906</v>
+      </c>
+      <c r="C38" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D38" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E38" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>2025</v>
+      </c>
+      <c r="B39" s="1">
+        <v>45907</v>
+      </c>
+      <c r="C39" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D39" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E39" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>2025</v>
+      </c>
+      <c r="B40" s="1">
+        <v>45908</v>
+      </c>
+      <c r="C40" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D40" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E40" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>2025</v>
+      </c>
+      <c r="B41" s="1">
+        <v>45909</v>
+      </c>
+      <c r="C41" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D41" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E41" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>2025</v>
+      </c>
+      <c r="B42" s="1">
+        <v>45910</v>
+      </c>
+      <c r="C42" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D42" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E42" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>2025</v>
+      </c>
+      <c r="B43" s="1">
+        <v>45911</v>
+      </c>
+      <c r="C43" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D43" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E43" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>2025</v>
+      </c>
+      <c r="B44" s="1">
+        <v>45912</v>
+      </c>
+      <c r="C44" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D44" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E44" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>2025</v>
+      </c>
+      <c r="B45" s="1">
+        <v>45913</v>
+      </c>
+      <c r="C45" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D45" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E45" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>2025</v>
+      </c>
+      <c r="B46" s="1">
+        <v>45914</v>
+      </c>
+      <c r="C46" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D46" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E46" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>2025</v>
+      </c>
+      <c r="B47" s="1">
+        <v>45915</v>
+      </c>
+      <c r="C47" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D47" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E47" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>2025</v>
+      </c>
+      <c r="B48" s="1">
+        <v>45916</v>
+      </c>
+      <c r="C48" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D48" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E48" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>2025</v>
+      </c>
+      <c r="B49" s="1">
+        <v>45917</v>
+      </c>
+      <c r="C49" s="7">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="D49" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E49" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>2025</v>
+      </c>
+      <c r="B50" s="1">
+        <v>45918</v>
+      </c>
+      <c r="C50" s="7">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="D50" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="E50" s="7">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>2025</v>
+      </c>
+      <c r="B51" s="1">
+        <v>45919</v>
+      </c>
+      <c r="C51" s="7">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="D51" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="E51" s="7">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>2025</v>
+      </c>
+      <c r="B52" s="1">
+        <v>45920</v>
+      </c>
+      <c r="C52" s="7">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="D52" s="7">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="E52" s="7">
+        <v>0.04</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394FE10B-CC5B-4887-BA9F-8638E71CB003}">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2667,7 +3592,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -4208,6 +5133,1569 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4FBFFC-676F-4493-85F5-BF4178BC747B}">
+  <dimension ref="A1:F77"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2025</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45812</v>
+      </c>
+      <c r="C2" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>8.7772000000000003E-2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>8.8412000000000004E-2</v>
+      </c>
+      <c r="F2" s="3">
+        <v>8.9346999999999996E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45813</v>
+      </c>
+      <c r="C3" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D3" s="3">
+        <v>8.7570999999999996E-2</v>
+      </c>
+      <c r="E3" s="3">
+        <v>8.8207000000000008E-2</v>
+      </c>
+      <c r="F3" s="3">
+        <v>8.9137999999999995E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2025</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45814</v>
+      </c>
+      <c r="C4" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>8.7469999999999992E-2</v>
+      </c>
+      <c r="E4" s="3">
+        <v>8.8104999999999989E-2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>8.9034000000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2025</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45817</v>
+      </c>
+      <c r="C5" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>8.7370000000000003E-2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>8.8002999999999998E-2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>8.8928999999999994E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2025</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45818</v>
+      </c>
+      <c r="C6" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>8.7167999999999995E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>8.7799000000000002E-2</v>
+      </c>
+      <c r="F6" s="3">
+        <v>8.8720999999999994E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2025</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45819</v>
+      </c>
+      <c r="C7" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>8.7370000000000003E-2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>8.8002999999999998E-2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>8.8928999999999994E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2025</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45820</v>
+      </c>
+      <c r="C8" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>8.7370000000000003E-2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>8.8002999999999998E-2</v>
+      </c>
+      <c r="F8" s="3">
+        <v>8.8928999999999994E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2025</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45821</v>
+      </c>
+      <c r="C9" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>8.7370000000000003E-2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>8.8002999999999998E-2</v>
+      </c>
+      <c r="F9" s="3">
+        <v>8.8928999999999994E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2025</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45824</v>
+      </c>
+      <c r="C10" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>8.7370000000000003E-2</v>
+      </c>
+      <c r="E10" s="3">
+        <v>8.8002999999999998E-2</v>
+      </c>
+      <c r="F10" s="3">
+        <v>8.8928999999999994E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2025</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45825</v>
+      </c>
+      <c r="C11" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>8.7469999999999992E-2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>8.8104999999999989E-2</v>
+      </c>
+      <c r="F11" s="3">
+        <v>8.9034000000000002E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2025</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45826</v>
+      </c>
+      <c r="C12" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>8.7570999999999996E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>8.8207000000000008E-2</v>
+      </c>
+      <c r="F12" s="3">
+        <v>8.9137999999999995E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2025</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45827</v>
+      </c>
+      <c r="C13" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>8.7670999999999999E-2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>8.8308999999999999E-2</v>
+      </c>
+      <c r="F13" s="3">
+        <v>8.9242000000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2025</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45828</v>
+      </c>
+      <c r="C14" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>8.7570999999999996E-2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>8.8207000000000008E-2</v>
+      </c>
+      <c r="F14" s="3">
+        <v>8.9137999999999995E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2025</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45831</v>
+      </c>
+      <c r="C15" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D15" s="3">
+        <v>8.7670999999999999E-2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>8.8308999999999999E-2</v>
+      </c>
+      <c r="F15" s="3">
+        <v>8.9242000000000002E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2025</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45832</v>
+      </c>
+      <c r="C16" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D16" s="3">
+        <v>8.7670999999999999E-2</v>
+      </c>
+      <c r="E16" s="3">
+        <v>8.8308999999999999E-2</v>
+      </c>
+      <c r="F16" s="3">
+        <v>8.9242000000000002E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2025</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45833</v>
+      </c>
+      <c r="C17" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D17" s="3">
+        <v>8.7873000000000007E-2</v>
+      </c>
+      <c r="E17" s="3">
+        <v>8.8513999999999995E-2</v>
+      </c>
+      <c r="F17" s="3">
+        <v>8.9451000000000003E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2025</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45834</v>
+      </c>
+      <c r="C18" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D18" s="3">
+        <v>8.7670999999999999E-2</v>
+      </c>
+      <c r="E18" s="3">
+        <v>8.8308999999999999E-2</v>
+      </c>
+      <c r="F18" s="3">
+        <v>8.9242000000000002E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2025</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45835</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="D19" s="3">
+        <v>8.7772000000000003E-2</v>
+      </c>
+      <c r="E19" s="3">
+        <v>8.8412000000000004E-2</v>
+      </c>
+      <c r="F19" s="3">
+        <v>8.9346999999999996E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2025</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45838</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="D20" s="3">
+        <v>8.2841999999999999E-2</v>
+      </c>
+      <c r="E20" s="3">
+        <v>8.3408999999999997E-2</v>
+      </c>
+      <c r="F20" s="3">
+        <v>8.4238999999999994E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2025</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45839</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="D21" s="3">
+        <v>8.3042999999999992E-2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>8.3612999999999993E-2</v>
+      </c>
+      <c r="F21" s="3">
+        <v>8.4446999999999994E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2025</v>
+      </c>
+      <c r="B22" s="1">
+        <v>45840</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="D22" s="3">
+        <v>8.4048999999999999E-2</v>
+      </c>
+      <c r="E22" s="3">
+        <v>8.4634000000000001E-2</v>
+      </c>
+      <c r="F22" s="3">
+        <v>8.5488999999999996E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2025</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45841</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="D23" s="3">
+        <v>8.2942000000000002E-2</v>
+      </c>
+      <c r="E23" s="3">
+        <v>8.3511000000000002E-2</v>
+      </c>
+      <c r="F23" s="3">
+        <v>8.4343000000000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2025</v>
+      </c>
+      <c r="B24" s="1">
+        <v>45842</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="D24" s="3">
+        <v>8.2639999999999991E-2</v>
+      </c>
+      <c r="E24" s="3">
+        <v>8.3204999999999987E-2</v>
+      </c>
+      <c r="F24" s="3">
+        <v>8.4031000000000008E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2025</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45845</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="D25" s="3">
+        <v>8.2238000000000006E-2</v>
+      </c>
+      <c r="E25" s="3">
+        <v>8.2796999999999996E-2</v>
+      </c>
+      <c r="F25" s="3">
+        <v>8.3613999999999994E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2025</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45846</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="D26" s="3">
+        <v>8.2438999999999998E-2</v>
+      </c>
+      <c r="E26" s="3">
+        <v>8.3001000000000005E-2</v>
+      </c>
+      <c r="F26" s="3">
+        <v>8.3821999999999994E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2025</v>
+      </c>
+      <c r="B27" s="1">
+        <v>45847</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="D27" s="3">
+        <v>8.2438999999999998E-2</v>
+      </c>
+      <c r="E27" s="3">
+        <v>8.3001000000000005E-2</v>
+      </c>
+      <c r="F27" s="3">
+        <v>8.3821999999999994E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2025</v>
+      </c>
+      <c r="B28" s="1">
+        <v>45848</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="D28" s="3">
+        <v>8.2438999999999998E-2</v>
+      </c>
+      <c r="E28" s="3">
+        <v>8.3001000000000005E-2</v>
+      </c>
+      <c r="F28" s="3">
+        <v>8.3821999999999994E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2025</v>
+      </c>
+      <c r="B29" s="1">
+        <v>45849</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="D29" s="3">
+        <v>8.2438999999999998E-2</v>
+      </c>
+      <c r="E29" s="3">
+        <v>8.3001000000000005E-2</v>
+      </c>
+      <c r="F29" s="3">
+        <v>8.3821999999999994E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2025</v>
+      </c>
+      <c r="B30" s="1">
+        <v>45852</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="D30" s="3">
+        <v>8.2438999999999998E-2</v>
+      </c>
+      <c r="E30" s="3">
+        <v>8.3001000000000005E-2</v>
+      </c>
+      <c r="F30" s="3">
+        <v>8.3821999999999994E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2025</v>
+      </c>
+      <c r="B31" s="1">
+        <v>45853</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="D31" s="3">
+        <v>8.2338999999999996E-2</v>
+      </c>
+      <c r="E31" s="3">
+        <v>8.2899E-2</v>
+      </c>
+      <c r="F31" s="3">
+        <v>8.3718000000000001E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2025</v>
+      </c>
+      <c r="B32" s="1">
+        <v>45854</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D32" s="4">
+        <v>8.2400000000000001E-2</v>
+      </c>
+      <c r="E32" s="4">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F32" s="4">
+        <v>8.3799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2025</v>
+      </c>
+      <c r="B33" s="1">
+        <v>45855</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D33" s="4">
+        <v>8.2400000000000001E-2</v>
+      </c>
+      <c r="E33" s="4">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F33" s="4">
+        <v>8.3799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>2025</v>
+      </c>
+      <c r="B34" s="1">
+        <v>45856</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D34" s="4">
+        <v>8.2299999999999998E-2</v>
+      </c>
+      <c r="E34" s="4">
+        <v>8.2900000000000001E-2</v>
+      </c>
+      <c r="F34" s="4">
+        <v>8.3699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>2025</v>
+      </c>
+      <c r="B35" s="1">
+        <v>45859</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D35" s="4">
+        <v>8.2299999999999998E-2</v>
+      </c>
+      <c r="E35" s="4">
+        <v>8.2900000000000001E-2</v>
+      </c>
+      <c r="F35" s="4">
+        <v>8.3699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>2025</v>
+      </c>
+      <c r="B36" s="1">
+        <v>45860</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D36" s="4">
+        <v>8.2299999999999998E-2</v>
+      </c>
+      <c r="E36" s="4">
+        <v>8.2900000000000001E-2</v>
+      </c>
+      <c r="F36" s="4">
+        <v>8.3699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>2025</v>
+      </c>
+      <c r="B37" s="1">
+        <v>45861</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D37" s="4">
+        <v>8.2500000000000004E-2</v>
+      </c>
+      <c r="E37" s="4">
+        <v>8.3099999999999993E-2</v>
+      </c>
+      <c r="F37" s="4">
+        <v>8.3900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2025</v>
+      </c>
+      <c r="B38" s="1">
+        <v>45862</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D38" s="4">
+        <v>8.2699999999999996E-2</v>
+      </c>
+      <c r="E38" s="4">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="F38" s="4">
+        <v>8.4099999999999994E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>2025</v>
+      </c>
+      <c r="B39" s="1">
+        <v>45866</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D39" s="4">
+        <v>8.2600000000000007E-2</v>
+      </c>
+      <c r="E39" s="4">
+        <v>8.3199999999999996E-2</v>
+      </c>
+      <c r="F39" s="4">
+        <v>8.4000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>2025</v>
+      </c>
+      <c r="B40" s="1">
+        <v>45867</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D40" s="4">
+        <v>8.2299999999999998E-2</v>
+      </c>
+      <c r="E40" s="4">
+        <v>8.2900000000000001E-2</v>
+      </c>
+      <c r="F40" s="4">
+        <v>8.3699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>2025</v>
+      </c>
+      <c r="B41" s="1">
+        <v>45868</v>
+      </c>
+      <c r="C41" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D41" s="4">
+        <v>8.2299999999999998E-2</v>
+      </c>
+      <c r="E41" s="4">
+        <v>8.2900000000000001E-2</v>
+      </c>
+      <c r="F41" s="4">
+        <v>8.3699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>2025</v>
+      </c>
+      <c r="B42" s="1">
+        <v>45869</v>
+      </c>
+      <c r="C42" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D42" s="4">
+        <v>8.2299999999999998E-2</v>
+      </c>
+      <c r="E42" s="4">
+        <v>8.2900000000000001E-2</v>
+      </c>
+      <c r="F42" s="4">
+        <v>8.3699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>2025</v>
+      </c>
+      <c r="B43" s="1">
+        <v>45870</v>
+      </c>
+      <c r="C43" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D43" s="4">
+        <v>8.2400000000000001E-2</v>
+      </c>
+      <c r="E43" s="4">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F43" s="4">
+        <v>8.3799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>2025</v>
+      </c>
+      <c r="B44" s="1">
+        <v>45873</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D44" s="4">
+        <v>8.3099999999999993E-2</v>
+      </c>
+      <c r="E44" s="4">
+        <v>8.3699999999999997E-2</v>
+      </c>
+      <c r="F44" s="4">
+        <v>8.4599999999999995E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>2025</v>
+      </c>
+      <c r="B45" s="1">
+        <v>45874</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D45" s="4">
+        <v>8.2400000000000001E-2</v>
+      </c>
+      <c r="E45" s="4">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F45" s="4">
+        <v>8.3799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>2025</v>
+      </c>
+      <c r="B46" s="1">
+        <v>45875</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D46" s="4">
+        <v>8.2400000000000001E-2</v>
+      </c>
+      <c r="E46" s="4">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F46" s="4">
+        <v>8.3799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>2025</v>
+      </c>
+      <c r="B47" s="1">
+        <v>45876</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="D47" s="4">
+        <v>8.2400000000000001E-2</v>
+      </c>
+      <c r="E47" s="4">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F47" s="4">
+        <v>8.3799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>2025</v>
+      </c>
+      <c r="B48" s="1">
+        <v>45877</v>
+      </c>
+      <c r="C48" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D48" s="4">
+        <v>8.2400000000000001E-2</v>
+      </c>
+      <c r="E48" s="4">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F48" s="4">
+        <v>8.3799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>2025</v>
+      </c>
+      <c r="B49" s="1">
+        <v>45880</v>
+      </c>
+      <c r="C49" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="E49" s="4">
+        <v>8.0600000000000005E-2</v>
+      </c>
+      <c r="F49" s="4">
+        <v>8.1299999999999997E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>2025</v>
+      </c>
+      <c r="B50" s="1">
+        <v>45881</v>
+      </c>
+      <c r="C50" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D50" s="4">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E50" s="4">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F50" s="4">
+        <v>8.14E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>2025</v>
+      </c>
+      <c r="B51" s="1">
+        <v>45882</v>
+      </c>
+      <c r="C51" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D51" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="E51" s="4">
+        <v>8.0600000000000005E-2</v>
+      </c>
+      <c r="F51" s="4">
+        <v>8.1299999999999997E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>2025</v>
+      </c>
+      <c r="B52" s="1">
+        <v>45883</v>
+      </c>
+      <c r="C52" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D52" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="E52" s="4">
+        <v>8.0600000000000005E-2</v>
+      </c>
+      <c r="F52" s="4">
+        <v>8.1299999999999997E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>2025</v>
+      </c>
+      <c r="B53" s="1">
+        <v>45884</v>
+      </c>
+      <c r="C53" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D53" s="4">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E53" s="4">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F53" s="4">
+        <v>8.14E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>2025</v>
+      </c>
+      <c r="B54" s="1">
+        <v>45887</v>
+      </c>
+      <c r="C54" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D54" s="5">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E54" s="5">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F54" s="5">
+        <v>8.14E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>2025</v>
+      </c>
+      <c r="B55" s="1">
+        <v>45888</v>
+      </c>
+      <c r="C55" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D55" s="4">
+        <v>8.0299999999999996E-2</v>
+      </c>
+      <c r="E55" s="4">
+        <v>8.09E-2</v>
+      </c>
+      <c r="F55" s="4">
+        <v>8.1600000000000006E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>2025</v>
+      </c>
+      <c r="B56" s="1">
+        <v>45889</v>
+      </c>
+      <c r="C56" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D56" s="4">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E56" s="4">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F56" s="4">
+        <v>8.14E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>2025</v>
+      </c>
+      <c r="B57" s="1">
+        <v>45890</v>
+      </c>
+      <c r="C57" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D57" s="4">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="E57" s="4">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="F57" s="4">
+        <v>8.1500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>2025</v>
+      </c>
+      <c r="B58" s="1">
+        <v>45891</v>
+      </c>
+      <c r="C58" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D58" s="4">
+        <v>8.0299999999999996E-2</v>
+      </c>
+      <c r="E58" s="4">
+        <v>8.09E-2</v>
+      </c>
+      <c r="F58" s="4">
+        <v>8.1600000000000006E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>2025</v>
+      </c>
+      <c r="B59" s="8">
+        <v>45894</v>
+      </c>
+      <c r="C59" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D59" s="4">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="E59" s="4">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="F59" s="4">
+        <v>8.1500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>2025</v>
+      </c>
+      <c r="B60" s="8">
+        <v>45895</v>
+      </c>
+      <c r="C60" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D60" s="4">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E60" s="4">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F60" s="4">
+        <v>8.14E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>2025</v>
+      </c>
+      <c r="B61" s="8">
+        <v>45896</v>
+      </c>
+      <c r="C61" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D61" s="4">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="E61" s="4">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="F61" s="4">
+        <v>8.1500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>2025</v>
+      </c>
+      <c r="B62" s="8">
+        <v>45897</v>
+      </c>
+      <c r="C62" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D62" s="4">
+        <v>8.0299999999999996E-2</v>
+      </c>
+      <c r="E62" s="4">
+        <v>8.09E-2</v>
+      </c>
+      <c r="F62" s="4">
+        <v>8.1600000000000006E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>2025</v>
+      </c>
+      <c r="B63" s="8">
+        <v>45898</v>
+      </c>
+      <c r="C63" s="4">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D63" s="4">
+        <v>8.0299999999999996E-2</v>
+      </c>
+      <c r="E63" s="4">
+        <v>8.09E-2</v>
+      </c>
+      <c r="F63" s="4">
+        <v>8.1600000000000006E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>2025</v>
+      </c>
+      <c r="B64" s="1">
+        <v>45901</v>
+      </c>
+      <c r="C64" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D64" s="5">
+        <v>8.0399999999999999E-2</v>
+      </c>
+      <c r="E64" s="5">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="F64" s="5">
+        <v>8.1699999999999995E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>2025</v>
+      </c>
+      <c r="B65" s="1">
+        <v>45902</v>
+      </c>
+      <c r="C65" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D65" s="5">
+        <v>8.1100000000000005E-2</v>
+      </c>
+      <c r="E65" s="5">
+        <v>8.1699999999999995E-2</v>
+      </c>
+      <c r="F65" s="5">
+        <v>8.2500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>2025</v>
+      </c>
+      <c r="B66" s="1">
+        <v>45903</v>
+      </c>
+      <c r="C66" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D66" s="5">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="E66" s="5">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="F66" s="5">
+        <v>8.1500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>2025</v>
+      </c>
+      <c r="B67" s="1">
+        <v>45904</v>
+      </c>
+      <c r="C67" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D67" s="5">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="E67" s="5">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="F67" s="5">
+        <v>8.1500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>2025</v>
+      </c>
+      <c r="B68" s="1">
+        <v>45905</v>
+      </c>
+      <c r="C68" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D68" s="5">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="E68" s="5">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="F68" s="5">
+        <v>8.1500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>2025</v>
+      </c>
+      <c r="B69" s="1">
+        <v>45908</v>
+      </c>
+      <c r="C69" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D69" s="5">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="E69" s="5">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="F69" s="5">
+        <v>8.1500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>2025</v>
+      </c>
+      <c r="B70" s="1">
+        <v>45909</v>
+      </c>
+      <c r="C70" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D70" s="5">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E70" s="5">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F70" s="5">
+        <v>8.14E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>2025</v>
+      </c>
+      <c r="B71" s="1">
+        <v>45910</v>
+      </c>
+      <c r="C71" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D71" s="5">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E71" s="5">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F71" s="5">
+        <v>8.14E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>2025</v>
+      </c>
+      <c r="B72" s="1">
+        <v>45911</v>
+      </c>
+      <c r="C72" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D72" s="5">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E72" s="5">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F72" s="5">
+        <v>8.14E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>2025</v>
+      </c>
+      <c r="B73" s="1">
+        <v>45912</v>
+      </c>
+      <c r="C73" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D73" s="5">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E73" s="5">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F73" s="5">
+        <v>8.14E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>2025</v>
+      </c>
+      <c r="B74" s="1">
+        <v>45915</v>
+      </c>
+      <c r="C74" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D74" s="5">
+        <v>8.0100000000000005E-2</v>
+      </c>
+      <c r="E74" s="5">
+        <v>8.0699999999999994E-2</v>
+      </c>
+      <c r="F74" s="5">
+        <v>8.14E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>2025</v>
+      </c>
+      <c r="B75" s="1">
+        <v>45917</v>
+      </c>
+      <c r="C75" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D75" s="5">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="E75" s="5">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="F75" s="5">
+        <v>8.1500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>2025</v>
+      </c>
+      <c r="B76" s="1">
+        <v>45918</v>
+      </c>
+      <c r="C76" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D76" s="5">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="E76" s="5">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="F76" s="5">
+        <v>8.1500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>2025</v>
+      </c>
+      <c r="B77" s="1">
+        <v>45919</v>
+      </c>
+      <c r="C77" s="5">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="D77" s="5">
+        <v>8.0299999999999996E-2</v>
+      </c>
+      <c r="E77" s="5">
+        <v>8.09E-2</v>
+      </c>
+      <c r="F77" s="5">
+        <v>8.1600000000000006E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B7A3E5-7422-42F6-B226-5BFEA691299B}">
   <dimension ref="A1:N180"/>
   <sheetViews>
@@ -12151,7 +14639,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A0379E-1221-4F1B-BC4B-DB7651DB87BC}">
   <dimension ref="A1:C167"/>
   <sheetViews>
@@ -14003,7 +16491,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6F7ED1-F67A-4D3F-B065-CA644B535717}">
   <dimension ref="A1:H36"/>
   <sheetViews>
@@ -15066,7 +17554,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D941C0-37A8-48F7-8F55-1334D82BCF20}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -15140,7 +17628,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9B52AB-9F4D-4048-B6BB-4409FE75ED91}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -15211,12 +17699,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE3EAA2-8F6D-45D1-94CD-1021786505AF}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15234,7 +17722,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
actualización del archivo de noticias hasta el 24 de septiembre
</commit_message>
<xml_diff>
--- a/tipo de cambio y tasas de interés.xlsx
+++ b/tipo de cambio y tasas de interés.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83571F13-E270-4D28-8E79-DEAC2E96336F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EAB104-AB33-4D08-8D75-4CC9DECC938C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="8" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo de Cambio" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,7 @@
     <sheet name="Wallstreet" sheetId="6" r:id="rId6"/>
     <sheet name="InflaciónUS" sheetId="4" r:id="rId7"/>
     <sheet name="InflaciónMEX" sheetId="10" r:id="rId8"/>
-    <sheet name="Tasas de interés US" sheetId="13" r:id="rId9"/>
-    <sheet name="Tasas de interés US2" sheetId="15" r:id="rId10"/>
+    <sheet name="Tasas de interés US2" sheetId="15" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Tasas de interés2'!$D$1:$F$30</definedName>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>Fecha</t>
   </si>
@@ -131,9 +130,6 @@
   </si>
   <si>
     <t>Tasa de Interés Objetivo</t>
-  </si>
-  <si>
-    <t>Tasa efectiva de fondos federales</t>
   </si>
 </sst>
 </file>
@@ -1325,7 +1321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892B4731-B44C-4F20-9A44-95C4BD8A73FF}">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
@@ -2667,905 +2663,6 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB728CC-3545-439B-8305-CE331A9F0964}">
-  <dimension ref="A1:E52"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2025</v>
-      </c>
-      <c r="B2" s="1">
-        <v>45870</v>
-      </c>
-      <c r="C2" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D2" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E2" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2025</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45871</v>
-      </c>
-      <c r="C3" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D3" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E3" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2025</v>
-      </c>
-      <c r="B4" s="1">
-        <v>45872</v>
-      </c>
-      <c r="C4" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D4" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E4" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2025</v>
-      </c>
-      <c r="B5" s="1">
-        <v>45873</v>
-      </c>
-      <c r="C5" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D5" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E5" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2025</v>
-      </c>
-      <c r="B6" s="1">
-        <v>45874</v>
-      </c>
-      <c r="C6" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D6" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E6" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2025</v>
-      </c>
-      <c r="B7" s="1">
-        <v>45875</v>
-      </c>
-      <c r="C7" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D7" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E7" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2025</v>
-      </c>
-      <c r="B8" s="1">
-        <v>45876</v>
-      </c>
-      <c r="C8" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D8" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E8" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2025</v>
-      </c>
-      <c r="B9" s="1">
-        <v>45877</v>
-      </c>
-      <c r="C9" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D9" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E9" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>2025</v>
-      </c>
-      <c r="B10" s="1">
-        <v>45878</v>
-      </c>
-      <c r="C10" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D10" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E10" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>2025</v>
-      </c>
-      <c r="B11" s="1">
-        <v>45879</v>
-      </c>
-      <c r="C11" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D11" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E11" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>2025</v>
-      </c>
-      <c r="B12" s="1">
-        <v>45880</v>
-      </c>
-      <c r="C12" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D12" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E12" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>2025</v>
-      </c>
-      <c r="B13" s="1">
-        <v>45881</v>
-      </c>
-      <c r="C13" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D13" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E13" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>2025</v>
-      </c>
-      <c r="B14" s="1">
-        <v>45882</v>
-      </c>
-      <c r="C14" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D14" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E14" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>2025</v>
-      </c>
-      <c r="B15" s="1">
-        <v>45883</v>
-      </c>
-      <c r="C15" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D15" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E15" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>2025</v>
-      </c>
-      <c r="B16" s="1">
-        <v>45884</v>
-      </c>
-      <c r="C16" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D16" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E16" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>2025</v>
-      </c>
-      <c r="B17" s="1">
-        <v>45885</v>
-      </c>
-      <c r="C17" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D17" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E17" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>2025</v>
-      </c>
-      <c r="B18" s="1">
-        <v>45886</v>
-      </c>
-      <c r="C18" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D18" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E18" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>2025</v>
-      </c>
-      <c r="B19" s="1">
-        <v>45887</v>
-      </c>
-      <c r="C19" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D19" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E19" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>2025</v>
-      </c>
-      <c r="B20" s="1">
-        <v>45888</v>
-      </c>
-      <c r="C20" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D20" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E20" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>2025</v>
-      </c>
-      <c r="B21" s="1">
-        <v>45889</v>
-      </c>
-      <c r="C21" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D21" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E21" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>2025</v>
-      </c>
-      <c r="B22" s="1">
-        <v>45890</v>
-      </c>
-      <c r="C22" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D22" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E22" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>2025</v>
-      </c>
-      <c r="B23" s="1">
-        <v>45891</v>
-      </c>
-      <c r="C23" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D23" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E23" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>2025</v>
-      </c>
-      <c r="B24" s="1">
-        <v>45892</v>
-      </c>
-      <c r="C24" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D24" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E24" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>2025</v>
-      </c>
-      <c r="B25" s="1">
-        <v>45893</v>
-      </c>
-      <c r="C25" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D25" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E25" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>2025</v>
-      </c>
-      <c r="B26" s="1">
-        <v>45894</v>
-      </c>
-      <c r="C26" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D26" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E26" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>2025</v>
-      </c>
-      <c r="B27" s="1">
-        <v>45895</v>
-      </c>
-      <c r="C27" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D27" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E27" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>2025</v>
-      </c>
-      <c r="B28" s="1">
-        <v>45896</v>
-      </c>
-      <c r="C28" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D28" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E28" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>2025</v>
-      </c>
-      <c r="B29" s="1">
-        <v>45897</v>
-      </c>
-      <c r="C29" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D29" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E29" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>2025</v>
-      </c>
-      <c r="B30" s="1">
-        <v>45898</v>
-      </c>
-      <c r="C30" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D30" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E30" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>2025</v>
-      </c>
-      <c r="B31" s="1">
-        <v>45899</v>
-      </c>
-      <c r="C31" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D31" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E31" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>2025</v>
-      </c>
-      <c r="B32" s="1">
-        <v>45900</v>
-      </c>
-      <c r="C32" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D32" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E32" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>2025</v>
-      </c>
-      <c r="B33" s="1">
-        <v>45901</v>
-      </c>
-      <c r="C33" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D33" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E33" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>2025</v>
-      </c>
-      <c r="B34" s="1">
-        <v>45902</v>
-      </c>
-      <c r="C34" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D34" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E34" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>2025</v>
-      </c>
-      <c r="B35" s="1">
-        <v>45903</v>
-      </c>
-      <c r="C35" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D35" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E35" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>2025</v>
-      </c>
-      <c r="B36" s="1">
-        <v>45904</v>
-      </c>
-      <c r="C36" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D36" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E36" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>2025</v>
-      </c>
-      <c r="B37" s="1">
-        <v>45905</v>
-      </c>
-      <c r="C37" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D37" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E37" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>2025</v>
-      </c>
-      <c r="B38" s="1">
-        <v>45906</v>
-      </c>
-      <c r="C38" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D38" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E38" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>2025</v>
-      </c>
-      <c r="B39" s="1">
-        <v>45907</v>
-      </c>
-      <c r="C39" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D39" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E39" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>2025</v>
-      </c>
-      <c r="B40" s="1">
-        <v>45908</v>
-      </c>
-      <c r="C40" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D40" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E40" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>2025</v>
-      </c>
-      <c r="B41" s="1">
-        <v>45909</v>
-      </c>
-      <c r="C41" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D41" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E41" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>2025</v>
-      </c>
-      <c r="B42" s="1">
-        <v>45910</v>
-      </c>
-      <c r="C42" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D42" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E42" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>2025</v>
-      </c>
-      <c r="B43" s="1">
-        <v>45911</v>
-      </c>
-      <c r="C43" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D43" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E43" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>2025</v>
-      </c>
-      <c r="B44" s="1">
-        <v>45912</v>
-      </c>
-      <c r="C44" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D44" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E44" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>2025</v>
-      </c>
-      <c r="B45" s="1">
-        <v>45913</v>
-      </c>
-      <c r="C45" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D45" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E45" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>2025</v>
-      </c>
-      <c r="B46" s="1">
-        <v>45914</v>
-      </c>
-      <c r="C46" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D46" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E46" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>2025</v>
-      </c>
-      <c r="B47" s="1">
-        <v>45915</v>
-      </c>
-      <c r="C47" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D47" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E47" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>2025</v>
-      </c>
-      <c r="B48" s="1">
-        <v>45916</v>
-      </c>
-      <c r="C48" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D48" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E48" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>2025</v>
-      </c>
-      <c r="B49" s="1">
-        <v>45917</v>
-      </c>
-      <c r="C49" s="7">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="D49" s="7">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E49" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50">
-        <v>2025</v>
-      </c>
-      <c r="B50" s="1">
-        <v>45918</v>
-      </c>
-      <c r="C50" s="7">
-        <v>4.0800000000000003E-2</v>
-      </c>
-      <c r="D50" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-      <c r="E50" s="7">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51">
-        <v>2025</v>
-      </c>
-      <c r="B51" s="1">
-        <v>45919</v>
-      </c>
-      <c r="C51" s="7">
-        <v>4.0800000000000003E-2</v>
-      </c>
-      <c r="D51" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-      <c r="E51" s="7">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52">
-        <v>2025</v>
-      </c>
-      <c r="B52" s="1">
-        <v>45920</v>
-      </c>
-      <c r="C52" s="7">
-        <v>4.0800000000000003E-2</v>
-      </c>
-      <c r="D52" s="7">
-        <v>4.2500000000000003E-2</v>
-      </c>
-      <c r="E52" s="7">
-        <v>0.04</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5137,7 +4234,7 @@
   <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17700,19 +16797,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE3EAA2-8F6D-45D1-94CD-1021786505AF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB728CC-3545-439B-8305-CE331A9F0964}">
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.21875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -17722,7 +16814,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
         <v>28</v>
@@ -18600,5 +17692,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reporte del 15 al 19 de septiembre
</commit_message>
<xml_diff>
--- a/tipo de cambio y tasas de interés.xlsx
+++ b/tipo de cambio y tasas de interés.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conda24\Fondo Sergio\monitoreo-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5AD3D4-18C1-4CAC-B9A8-35AA7CD049C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F51AFD-76AE-48AB-A3EC-0258E5B10A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{30335E2C-89DA-4C79-B82F-6F6D648259F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Tipo de Cambio" sheetId="1" r:id="rId1"/>
     <sheet name="Tasas de interés2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tasas de interés" sheetId="14" state="hidden" r:id="rId3"/>
+    <sheet name="Tasas de interés" sheetId="14" r:id="rId3"/>
     <sheet name="Treasuries_SOFR" sheetId="3" r:id="rId4"/>
     <sheet name="Wallstreet" sheetId="6" r:id="rId5"/>
     <sheet name="InflaciónUS" sheetId="4" r:id="rId6"/>
@@ -4399,8 +4399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4FBFFC-676F-4493-85F5-BF4178BC747B}">
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:F82"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14270,7 +14270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6F7ED1-F67A-4D3F-B065-CA644B535717}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>

</xml_diff>